<commit_message>
integration test case (finish user sheet) Not final
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
+++ b/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="0" windowWidth="26780" windowHeight="14880" tabRatio="543" activeTab="4"/>
+    <workbookView xWindow="1080" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="382">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -1800,6 +1800,63 @@
 4. Click on "sign in" button of login page or press enter
 5. Click on "Avatar" in menu bar
 6. Click "Notification" list in personal page</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Logged in successfully
+4. The "medicinal plants" page is displayed
+5. "Medicinal plants detail" page is displayed
+6. "Author" is displayed</t>
+  </si>
+  <si>
+    <t>1. Enter the website: thuocnam.com
+2. Click on Login button
+3. Input:
++ Email: "dangnhse02992@fpt.edu.vn"
++ Password: "123456789"
+4. Click on "sign in" button of login page or press enter
+5. Click on "Medicinal Plants" in menu bar
+6. Click on a "medicinal plants" picture of medicinal plants page
+7. Click on "author" link of "medicinal plants detail" page</t>
+  </si>
+  <si>
+    <t>1. Enter the website: thuocnam.com
+2. Click on Login button
+3. Input:
++ Email: "dangnhse02992@fpt.edu.vn"
++ Password: "123456789"
+4. Click on "sign in" button of login page or press enter
+5. Click on "Remedy" in menu bar
+6. Click on a "Remedy" picture of remedy page
+7. Click on "relational HMS" of remedy detail page</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Logged in successfully
+4. The "remedy" page is displayed
+5. "Remedy detail" page is displayed
+6. "Author" is displayed</t>
+  </si>
+  <si>
+    <t>1. Enter the website: thuocnam.com
+2. Click on Login button
+3. Input:
++ Email: "dangnhse02992@fpt.edu.vn"
++ Password: "123456789"
+4. Click on "sign in" button of login page or press enter
+5. Click on "Remedy" in menu bar
+6. Click on a "Remedy" picture of remedy page
+7. Click on "author" of remedy detail page</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Logged in successfully
+4. The "remedy" page is displayed
+5. "Remedy detail" page is displayed
+6. "HMS" is displayed</t>
   </si>
 </sst>
 </file>
@@ -2691,7 +2748,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="52">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
@@ -2744,6 +2801,13 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3329,7 +3393,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="52">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -3374,6 +3438,13 @@
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
@@ -4451,7 +4522,7 @@
       </c>
       <c r="F11" s="76">
         <f>User_Function!C6</f>
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="G11" s="76">
         <f>User_Function!D6</f>
@@ -4459,7 +4530,7 @@
       </c>
       <c r="H11" s="77">
         <f>User_Function!E6</f>
-        <v>82</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4507,7 +4578,7 @@
       </c>
       <c r="F13" s="79">
         <f>SUM(F9:F12)</f>
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="G13" s="79">
         <f>SUM(G9:G12)</f>
@@ -4515,7 +4586,7 @@
       </c>
       <c r="H13" s="80">
         <f>SUM(H9:H12)</f>
-        <v>108</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4922,8 +4993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -5050,7 +5121,7 @@
       </c>
       <c r="C6" s="101">
         <f>E6-D6-B6-A6</f>
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="D6" s="102">
         <f>COUNTIF(F11:G688,"N/A")</f>
@@ -5058,7 +5129,7 @@
       </c>
       <c r="E6" s="214">
         <f>COUNTA(A11:A245)*2</f>
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="F6" s="214"/>
       <c r="G6" s="214"/>
@@ -5685,7 +5756,9 @@
       <c r="J38" s="105"/>
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A39" s="169"/>
+      <c r="A39" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="B39" s="169" t="s">
         <v>328</v>
       </c>
@@ -5699,7 +5772,10 @@
       <c r="J39" s="105"/>
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A40" s="163"/>
+      <c r="A40" s="163" t="str">
+        <f t="shared" ref="A39:A58" si="2">IF(OR(B40&lt;&gt;"",D40&lt;E39&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[User_login-30]</v>
+      </c>
       <c r="B40" s="117" t="s">
         <v>329</v>
       </c>
@@ -5717,7 +5793,9 @@
       <c r="J40" s="105"/>
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A41" s="169"/>
+      <c r="A41" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="B41" s="169" t="s">
         <v>331</v>
       </c>
@@ -5731,7 +5809,10 @@
       <c r="J41" s="105"/>
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A42" s="163"/>
+      <c r="A42" s="163" t="str">
+        <f t="shared" si="2"/>
+        <v>[User_login-32]</v>
+      </c>
       <c r="B42" s="117" t="s">
         <v>329</v>
       </c>
@@ -5749,7 +5830,9 @@
       <c r="J42" s="105"/>
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A43" s="169"/>
+      <c r="A43" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="B43" s="169" t="s">
         <v>333</v>
       </c>
@@ -5763,7 +5846,10 @@
       <c r="J43" s="105"/>
     </row>
     <row r="44" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A44" s="163"/>
+      <c r="A44" s="163" t="str">
+        <f t="shared" si="2"/>
+        <v>[User_login-34]</v>
+      </c>
       <c r="B44" s="117" t="s">
         <v>334</v>
       </c>
@@ -5781,7 +5867,9 @@
       <c r="J44" s="105"/>
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A45" s="169"/>
+      <c r="A45" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="B45" s="169" t="s">
         <v>336</v>
       </c>
@@ -5795,7 +5883,10 @@
       <c r="J45" s="105"/>
     </row>
     <row r="46" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A46" s="163"/>
+      <c r="A46" s="163" t="str">
+        <f t="shared" si="2"/>
+        <v>[User_login-36]</v>
+      </c>
       <c r="B46" s="117" t="s">
         <v>337</v>
       </c>
@@ -5813,7 +5904,9 @@
       <c r="J46" s="105"/>
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A47" s="169"/>
+      <c r="A47" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="B47" s="169" t="s">
         <v>357</v>
       </c>
@@ -5827,7 +5920,10 @@
       <c r="J47" s="105"/>
     </row>
     <row r="48" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A48" s="163"/>
+      <c r="A48" s="163" t="str">
+        <f t="shared" si="2"/>
+        <v>[User_login-38]</v>
+      </c>
       <c r="B48" s="117" t="s">
         <v>358</v>
       </c>
@@ -5845,7 +5941,9 @@
       <c r="J48" s="105"/>
     </row>
     <row r="49" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A49" s="169"/>
+      <c r="A49" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="B49" s="169" t="s">
         <v>360</v>
       </c>
@@ -5859,7 +5957,10 @@
       <c r="J49" s="105"/>
     </row>
     <row r="50" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A50" s="163"/>
+      <c r="A50" s="163" t="str">
+        <f t="shared" si="2"/>
+        <v>[User_login-40]</v>
+      </c>
       <c r="B50" s="117" t="s">
         <v>361</v>
       </c>
@@ -5877,7 +5978,9 @@
       <c r="J50" s="105"/>
     </row>
     <row r="51" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A51" s="169"/>
+      <c r="A51" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="B51" s="169" t="s">
         <v>363</v>
       </c>
@@ -5891,7 +5994,10 @@
       <c r="J51" s="105"/>
     </row>
     <row r="52" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A52" s="163"/>
+      <c r="A52" s="163" t="str">
+        <f t="shared" si="2"/>
+        <v>[User_login-42]</v>
+      </c>
       <c r="B52" s="117" t="s">
         <v>368</v>
       </c>
@@ -5909,7 +6015,9 @@
       <c r="J52" s="105"/>
     </row>
     <row r="53" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A53" s="169"/>
+      <c r="A53" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="B53" s="169" t="s">
         <v>370</v>
       </c>
@@ -5923,20 +6031,29 @@
       <c r="J53" s="105"/>
     </row>
     <row r="54" spans="1:10" s="169" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A54" s="193"/>
-      <c r="B54" s="194" t="s">
+      <c r="A54" s="163" t="str">
+        <f t="shared" si="2"/>
+        <v>[User_login-44]</v>
+      </c>
+      <c r="B54" s="117" t="s">
         <v>373</v>
       </c>
-      <c r="C54" s="194"/>
-      <c r="D54" s="194"/>
-      <c r="E54" s="193"/>
-      <c r="F54" s="194"/>
-      <c r="G54" s="194"/>
-      <c r="H54" s="195"/>
-      <c r="I54" s="196"/>
+      <c r="C54" s="117" t="s">
+        <v>377</v>
+      </c>
+      <c r="D54" s="117" t="s">
+        <v>376</v>
+      </c>
+      <c r="E54" s="118"/>
+      <c r="F54" s="117"/>
+      <c r="G54" s="117"/>
+      <c r="H54" s="119"/>
+      <c r="I54" s="120"/>
     </row>
     <row r="55" spans="1:10" s="184" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A55" s="169"/>
+      <c r="A55" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="B55" s="169" t="s">
         <v>371</v>
       </c>
@@ -5949,20 +6066,29 @@
       <c r="I55" s="168"/>
     </row>
     <row r="56" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A56" s="193"/>
-      <c r="B56" s="194" t="s">
+      <c r="A56" s="163" t="str">
+        <f t="shared" si="2"/>
+        <v>[User_login-46]</v>
+      </c>
+      <c r="B56" s="117" t="s">
         <v>374</v>
       </c>
-      <c r="C56" s="194"/>
-      <c r="D56" s="194"/>
-      <c r="E56" s="193"/>
-      <c r="F56" s="194"/>
-      <c r="G56" s="194"/>
-      <c r="H56" s="195"/>
-      <c r="I56" s="196"/>
+      <c r="C56" s="117" t="s">
+        <v>378</v>
+      </c>
+      <c r="D56" s="117" t="s">
+        <v>381</v>
+      </c>
+      <c r="E56" s="118"/>
+      <c r="F56" s="117"/>
+      <c r="G56" s="117"/>
+      <c r="H56" s="119"/>
+      <c r="I56" s="120"/>
     </row>
     <row r="57" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A57" s="169"/>
+      <c r="A57" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="B57" s="169" t="s">
         <v>372</v>
       </c>
@@ -5975,17 +6101,24 @@
       <c r="I57" s="168"/>
     </row>
     <row r="58" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A58" s="193"/>
-      <c r="B58" s="194" t="s">
+      <c r="A58" s="163" t="str">
+        <f t="shared" si="2"/>
+        <v>[User_login-48]</v>
+      </c>
+      <c r="B58" s="117" t="s">
         <v>373</v>
       </c>
-      <c r="C58" s="194"/>
-      <c r="D58" s="194"/>
-      <c r="E58" s="193"/>
-      <c r="F58" s="194"/>
-      <c r="G58" s="194"/>
-      <c r="H58" s="195"/>
-      <c r="I58" s="196"/>
+      <c r="C58" s="117" t="s">
+        <v>380</v>
+      </c>
+      <c r="D58" s="117" t="s">
+        <v>379</v>
+      </c>
+      <c r="E58" s="118"/>
+      <c r="F58" s="117"/>
+      <c r="G58" s="117"/>
+      <c r="H58" s="119"/>
+      <c r="I58" s="120"/>
     </row>
     <row r="59" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A59" s="193"/>
@@ -6038,7 +6171,7 @@
     <row r="63" spans="1:10" s="190" customFormat="1" ht="14.25" customHeight="1">
       <c r="A63" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A62)+1)</f>
-        <v>ID-24</v>
+        <v>ID-44</v>
       </c>
       <c r="B63" s="117" t="s">
         <v>208</v>
@@ -6060,7 +6193,7 @@
     <row r="64" spans="1:10" s="190" customFormat="1" ht="14.25" customHeight="1">
       <c r="A64" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A63)+1)</f>
-        <v>ID-25</v>
+        <v>ID-45</v>
       </c>
       <c r="B64" s="117" t="s">
         <v>248</v>
@@ -6082,7 +6215,7 @@
     <row r="65" spans="1:9" s="190" customFormat="1" ht="14.25" customHeight="1">
       <c r="A65" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A64)+1)</f>
-        <v>ID-26</v>
+        <v>ID-46</v>
       </c>
       <c r="B65" s="117" t="s">
         <v>250</v>
@@ -6104,7 +6237,7 @@
     <row r="66" spans="1:9" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A66" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A65)+1)</f>
-        <v>ID-27</v>
+        <v>ID-47</v>
       </c>
       <c r="B66" s="117" t="s">
         <v>252</v>
@@ -6126,7 +6259,7 @@
     <row r="67" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A67" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A66)+1)</f>
-        <v>ID-28</v>
+        <v>ID-48</v>
       </c>
       <c r="B67" s="117" t="s">
         <v>254</v>
@@ -6148,7 +6281,7 @@
     <row r="68" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A68" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A67)+1)</f>
-        <v>ID-29</v>
+        <v>ID-49</v>
       </c>
       <c r="B68" s="117" t="s">
         <v>256</v>
@@ -6183,7 +6316,7 @@
     <row r="70" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A70" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A69)+1)</f>
-        <v>ID-30</v>
+        <v>ID-50</v>
       </c>
       <c r="B70" s="117" t="s">
         <v>213</v>
@@ -6205,7 +6338,7 @@
     <row r="71" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A71" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A70)+1)</f>
-        <v>ID-31</v>
+        <v>ID-51</v>
       </c>
       <c r="B71" s="117" t="s">
         <v>214</v>
@@ -6227,7 +6360,7 @@
     <row r="72" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A72" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A71)+1)</f>
-        <v>ID-32</v>
+        <v>ID-52</v>
       </c>
       <c r="B72" s="117" t="s">
         <v>217</v>
@@ -6249,7 +6382,7 @@
     <row r="73" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A73" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A72)+1)</f>
-        <v>ID-33</v>
+        <v>ID-53</v>
       </c>
       <c r="B73" s="117" t="s">
         <v>219</v>
@@ -6271,7 +6404,7 @@
     <row r="74" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A74" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A73)+1)</f>
-        <v>ID-34</v>
+        <v>ID-54</v>
       </c>
       <c r="B74" s="117" t="s">
         <v>221</v>
@@ -6293,7 +6426,7 @@
     <row r="75" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A75" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A74)+1)</f>
-        <v>ID-35</v>
+        <v>ID-55</v>
       </c>
       <c r="B75" s="117" t="s">
         <v>224</v>
@@ -6315,7 +6448,7 @@
     <row r="76" spans="1:9" ht="13.5" customHeight="1">
       <c r="A76" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A75)+1)</f>
-        <v>ID-36</v>
+        <v>ID-56</v>
       </c>
       <c r="B76" s="117" t="s">
         <v>227</v>
@@ -6337,7 +6470,7 @@
     <row r="77" spans="1:9" ht="13.5" customHeight="1">
       <c r="A77" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A76)+1)</f>
-        <v>ID-37</v>
+        <v>ID-57</v>
       </c>
       <c r="B77" s="117" t="s">
         <v>230</v>
@@ -6359,7 +6492,7 @@
     <row r="78" spans="1:9" ht="13.5" customHeight="1">
       <c r="A78" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A77)+1)</f>
-        <v>ID-38</v>
+        <v>ID-58</v>
       </c>
       <c r="B78" s="117" t="s">
         <v>233</v>
@@ -6381,7 +6514,7 @@
     <row r="79" spans="1:9" ht="13.5" customHeight="1">
       <c r="A79" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A78)+1)</f>
-        <v>ID-39</v>
+        <v>ID-59</v>
       </c>
       <c r="B79" s="117" t="s">
         <v>236</v>
@@ -6403,7 +6536,7 @@
     <row r="80" spans="1:9" ht="13.5" customHeight="1">
       <c r="A80" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A79)+1)</f>
-        <v>ID-40</v>
+        <v>ID-60</v>
       </c>
       <c r="B80" s="117" t="s">
         <v>239</v>
@@ -6425,7 +6558,7 @@
     <row r="81" spans="1:9" ht="13.5" customHeight="1">
       <c r="A81" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A80)+1)</f>
-        <v>ID-41</v>
+        <v>ID-61</v>
       </c>
       <c r="B81" s="117" t="s">
         <v>242</v>
@@ -6447,7 +6580,7 @@
     <row r="82" spans="1:9" ht="13.5" customHeight="1">
       <c r="A82" s="117" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A81)+1)</f>
-        <v>ID-42</v>
+        <v>ID-62</v>
       </c>
       <c r="B82" s="117" t="s">
         <v>245</v>

</xml_diff>

<commit_message>
finish user sheet of integration test case (not final)
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
+++ b/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27260" windowHeight="14880" tabRatio="543" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -1128,54 +1128,10 @@
     <t>Color of all tabs selection is the same</t>
   </si>
   <si>
-    <t>Backed List</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click Dự án đã ủng hộ
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
-    <t>Starred List</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click Dự án theo dõi
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
-    <t>Created List</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click Dự án đã tạo
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
     <t>Message</t>
   </si>
   <si>
-    <t>1. Login on one browser
-2. Click Tin nhắn
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
     <t>Account</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click Tài khoản
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
   </si>
   <si>
     <t>1. Set language of Browser isVietnamese
@@ -1210,13 +1166,6 @@
   </si>
   <si>
     <t>VMN</t>
-  </si>
-  <si>
-    <t>List enviroment requires in this system
-1. Server: 
-2. Database server: Neo4j
-3. Browser: Google Chrome 40, Mozzila Firefox 30
-4. Operation System: Mac OS X</t>
   </si>
   <si>
     <t>1. Go to thuocnam.com
@@ -1417,9 +1366,6 @@
 6. Show posted article is displayed</t>
   </si>
   <si>
-    <t>Vietnamese Medicinal Plant Network</t>
-  </si>
-  <si>
     <t>Mod Common module</t>
   </si>
   <si>
@@ -1857,6 +1803,60 @@
 4. The "remedy" page is displayed
 5. "Remedy detail" page is displayed
 6. "HMS" is displayed</t>
+  </si>
+  <si>
+    <t>Vietnamese Medicinal Plants Network</t>
+  </si>
+  <si>
+    <t>List enviroment requires in this system
+1. Server: 
+2. Database server: MySQL server
+3. Browser: Google Chrome 40, Mozzila Firefox 30
+4. Operation System: Mac OS X</t>
+  </si>
+  <si>
+    <t>Medicinal Plant</t>
+  </si>
+  <si>
+    <t>Remedy</t>
+  </si>
+  <si>
+    <t>Herb Store Medicine</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click "Mecicinal plant" menu
+3. Copy link
+4. Change to other browser
+5. Paste link and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click "Remedy" menu
+3. Copy link
+4. Change to other browser
+5. Paste link and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click "HMS" menu
+3. Copy link
+4. Change to other browser
+5. Paste link and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click Message
+3. Copy link
+4. Change to other browser
+5. Paste link and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click Account
+3. Copy link
+4. Change to other browser
+5. Paste link and press Enter</t>
   </si>
 </sst>
 </file>
@@ -3901,7 +3901,7 @@
   <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C5" sqref="C5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3937,7 +3937,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="200" t="s">
-        <v>305</v>
+        <v>372</v>
       </c>
       <c r="D4" s="200"/>
       <c r="E4" s="200"/>
@@ -3945,7 +3945,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
@@ -3953,7 +3953,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="200" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D5" s="200"/>
       <c r="E5" s="200"/>
@@ -3961,7 +3961,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
@@ -4045,7 +4045,7 @@
         <v>55</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="19" customFormat="1" ht="21.75" customHeight="1">
@@ -4125,7 +4125,7 @@
   <dimension ref="B1:F20"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4158,7 +4158,7 @@
       <c r="C3" s="205"/>
       <c r="D3" s="206" t="str">
         <f>Cover!C4</f>
-        <v>Vietnamese Medicinal Plant Network</v>
+        <v>Vietnamese Medicinal Plants Network</v>
       </c>
       <c r="E3" s="206"/>
       <c r="F3" s="206"/>
@@ -4181,7 +4181,7 @@
       </c>
       <c r="C5" s="203"/>
       <c r="D5" s="204" t="s">
-        <v>267</v>
+        <v>373</v>
       </c>
       <c r="E5" s="204"/>
       <c r="F5" s="204"/>
@@ -4353,7 +4353,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="C3" s="206" t="str">
         <f>Cover!C4</f>
-        <v>Vietnamese Medicinal Plant Network</v>
+        <v>Vietnamese Medicinal Plants Network</v>
       </c>
       <c r="D3" s="206"/>
       <c r="E3" s="207" t="s">
@@ -4401,7 +4401,7 @@
       </c>
       <c r="F3" s="207"/>
       <c r="G3" s="10" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="H3" s="65"/>
     </row>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="F4" s="207"/>
       <c r="G4" s="10" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H4" s="65"/>
     </row>
@@ -4993,8 +4993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:I58"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -5071,7 +5071,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="212" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C4" s="212"/>
       <c r="D4" s="212"/>
@@ -5228,7 +5228,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="D12" s="117" t="s">
         <v>97</v>
@@ -5249,7 +5249,7 @@
         <v>61</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="D13" s="117" t="s">
         <v>98</v>
@@ -5270,10 +5270,10 @@
         <v>62</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="D14" s="121" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E14" s="122"/>
       <c r="F14" s="117"/>
@@ -5291,7 +5291,7 @@
         <v>63</v>
       </c>
       <c r="C15" s="124" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="D15" s="124" t="s">
         <v>99</v>
@@ -5312,7 +5312,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="124" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="D16" s="124" t="s">
         <v>161</v>
@@ -5333,7 +5333,7 @@
         <v>65</v>
       </c>
       <c r="C17" s="124" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="D17" s="124" t="s">
         <v>162</v>
@@ -5354,7 +5354,7 @@
         <v>66</v>
       </c>
       <c r="C18" s="124" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="D18" s="124" t="s">
         <v>163</v>
@@ -5389,10 +5389,10 @@
         <v>82</v>
       </c>
       <c r="C20" s="91" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="D20" s="91" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="E20" s="91" t="s">
         <v>83</v>
@@ -5406,7 +5406,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="58"/>
       <c r="B21" s="58" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
@@ -5426,7 +5426,7 @@
         <v>87</v>
       </c>
       <c r="C22" s="91" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D22" s="91" t="s">
         <v>164</v>
@@ -5449,7 +5449,7 @@
         <v>88</v>
       </c>
       <c r="C23" s="91" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="D23" s="91" t="s">
         <v>165</v>
@@ -5470,7 +5470,7 @@
         <v>89</v>
       </c>
       <c r="C24" s="91" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="D24" s="91" t="s">
         <v>166</v>
@@ -5504,13 +5504,13 @@
         <v>[User_login-16]</v>
       </c>
       <c r="B26" s="91" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C26" s="91" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="D26" s="136" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="E26" s="91" t="s">
         <v>86</v>
@@ -5530,10 +5530,10 @@
         <v>90</v>
       </c>
       <c r="C27" s="91" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="D27" s="91" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="E27" s="91" t="s">
         <v>84</v>
@@ -5567,10 +5567,10 @@
         <v>167</v>
       </c>
       <c r="C29" s="106" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="D29" s="104" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="E29" s="104" t="s">
         <v>91</v>
@@ -5590,10 +5590,10 @@
         <v>92</v>
       </c>
       <c r="C30" s="106" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D30" s="104" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="E30" s="104" t="s">
         <v>91</v>
@@ -5606,7 +5606,7 @@
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1">
       <c r="A31" s="58" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B31" s="58" t="s">
         <v>169</v>
@@ -5626,13 +5626,13 @@
         <v>[User_login-22]</v>
       </c>
       <c r="B32" s="91" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C32" s="106" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="D32" s="104" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="E32" s="104"/>
       <c r="F32" s="117"/>
@@ -5647,13 +5647,13 @@
         <v>[User_login-23]</v>
       </c>
       <c r="B33" s="91" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C33" s="106" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D33" s="104" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="E33" s="104"/>
       <c r="F33" s="117"/>
@@ -5664,10 +5664,10 @@
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
       <c r="A34" s="58" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B34" s="58" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="59"/>
@@ -5684,13 +5684,13 @@
         <v>[User_login-25]</v>
       </c>
       <c r="B35" s="91" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C35" s="106" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D35" s="104" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E35" s="104"/>
       <c r="F35" s="117"/>
@@ -5722,10 +5722,10 @@
         <v>203</v>
       </c>
       <c r="C37" s="117" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="D37" s="117" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="E37" s="118"/>
       <c r="F37" s="117"/>
@@ -5740,10 +5740,10 @@
         <v>[User_login-28]</v>
       </c>
       <c r="B38" s="117" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="C38" s="117" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D38" s="117" t="s">
         <v>205</v>
@@ -5757,10 +5757,10 @@
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1">
       <c r="A39" s="169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B39" s="169" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="C39" s="166"/>
       <c r="D39" s="166"/>
@@ -5773,17 +5773,17 @@
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1">
       <c r="A40" s="163" t="str">
-        <f t="shared" ref="A39:A58" si="2">IF(OR(B40&lt;&gt;"",D40&lt;E39&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <f t="shared" ref="A40:A58" si="2">IF(OR(B40&lt;&gt;"",D40&lt;E39&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
         <v>[User_login-30]</v>
       </c>
       <c r="B40" s="117" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C40" s="117" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="D40" s="117" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="E40" s="118"/>
       <c r="F40" s="117"/>
@@ -5794,10 +5794,10 @@
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1">
       <c r="A41" s="169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B41" s="169" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="C41" s="166"/>
       <c r="D41" s="166"/>
@@ -5814,13 +5814,13 @@
         <v>[User_login-32]</v>
       </c>
       <c r="B42" s="117" t="s">
+        <v>319</v>
+      </c>
+      <c r="C42" s="117" t="s">
         <v>329</v>
       </c>
-      <c r="C42" s="117" t="s">
-        <v>339</v>
-      </c>
       <c r="D42" s="117" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E42" s="118"/>
       <c r="F42" s="117"/>
@@ -5831,10 +5831,10 @@
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1">
       <c r="A43" s="169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B43" s="169" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="C43" s="166"/>
       <c r="D43" s="166"/>
@@ -5851,13 +5851,13 @@
         <v>[User_login-34]</v>
       </c>
       <c r="B44" s="117" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="C44" s="117" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D44" s="117" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="E44" s="118"/>
       <c r="F44" s="117"/>
@@ -5868,10 +5868,10 @@
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1">
       <c r="A45" s="169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B45" s="169" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="C45" s="166"/>
       <c r="D45" s="166"/>
@@ -5888,13 +5888,13 @@
         <v>[User_login-36]</v>
       </c>
       <c r="B46" s="117" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="C46" s="117" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="D46" s="117" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="E46" s="118"/>
       <c r="F46" s="117"/>
@@ -5905,10 +5905,10 @@
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1">
       <c r="A47" s="169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B47" s="169" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="C47" s="166"/>
       <c r="D47" s="166"/>
@@ -5925,13 +5925,13 @@
         <v>[User_login-38]</v>
       </c>
       <c r="B48" s="117" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="C48" s="117" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="D48" s="117" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="E48" s="118"/>
       <c r="F48" s="117"/>
@@ -5942,10 +5942,10 @@
     </row>
     <row r="49" spans="1:10" ht="14.25" customHeight="1">
       <c r="A49" s="169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B49" s="169" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="C49" s="166"/>
       <c r="D49" s="166"/>
@@ -5962,13 +5962,13 @@
         <v>[User_login-40]</v>
       </c>
       <c r="B50" s="117" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="C50" s="117" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="D50" s="117" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="E50" s="118"/>
       <c r="F50" s="117"/>
@@ -5979,10 +5979,10 @@
     </row>
     <row r="51" spans="1:10" ht="14.25" customHeight="1">
       <c r="A51" s="169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B51" s="169" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="C51" s="166"/>
       <c r="D51" s="166"/>
@@ -5999,13 +5999,13 @@
         <v>[User_login-42]</v>
       </c>
       <c r="B52" s="117" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="C52" s="117" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="D52" s="117" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="E52" s="118"/>
       <c r="F52" s="117"/>
@@ -6016,10 +6016,10 @@
     </row>
     <row r="53" spans="1:10" ht="14.25" customHeight="1">
       <c r="A53" s="169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B53" s="169" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C53" s="166"/>
       <c r="D53" s="166"/>
@@ -6036,13 +6036,13 @@
         <v>[User_login-44]</v>
       </c>
       <c r="B54" s="117" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="C54" s="117" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="D54" s="117" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="E54" s="118"/>
       <c r="F54" s="117"/>
@@ -6052,10 +6052,10 @@
     </row>
     <row r="55" spans="1:10" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A55" s="169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B55" s="169" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="C55" s="166"/>
       <c r="D55" s="166"/>
@@ -6071,13 +6071,13 @@
         <v>[User_login-46]</v>
       </c>
       <c r="B56" s="117" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="C56" s="117" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="D56" s="117" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="E56" s="118"/>
       <c r="F56" s="117"/>
@@ -6087,10 +6087,10 @@
     </row>
     <row r="57" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A57" s="169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B57" s="169" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="C57" s="166"/>
       <c r="D57" s="166"/>
@@ -6106,13 +6106,13 @@
         <v>[User_login-48]</v>
       </c>
       <c r="B58" s="117" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="C58" s="117" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="D58" s="117" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="E58" s="118"/>
       <c r="F58" s="117"/>
@@ -6196,10 +6196,10 @@
         <v>ID-45</v>
       </c>
       <c r="B64" s="117" t="s">
-        <v>248</v>
+        <v>374</v>
       </c>
       <c r="C64" s="117" t="s">
-        <v>249</v>
+        <v>377</v>
       </c>
       <c r="D64" s="117" t="s">
         <v>210</v>
@@ -6218,10 +6218,10 @@
         <v>ID-46</v>
       </c>
       <c r="B65" s="117" t="s">
-        <v>250</v>
+        <v>375</v>
       </c>
       <c r="C65" s="117" t="s">
-        <v>251</v>
+        <v>378</v>
       </c>
       <c r="D65" s="117" t="s">
         <v>210</v>
@@ -6240,10 +6240,10 @@
         <v>ID-47</v>
       </c>
       <c r="B66" s="117" t="s">
-        <v>252</v>
+        <v>376</v>
       </c>
       <c r="C66" s="117" t="s">
-        <v>253</v>
+        <v>379</v>
       </c>
       <c r="D66" s="117" t="s">
         <v>210</v>
@@ -6262,10 +6262,10 @@
         <v>ID-48</v>
       </c>
       <c r="B67" s="117" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C67" s="117" t="s">
-        <v>255</v>
+        <v>380</v>
       </c>
       <c r="D67" s="117" t="s">
         <v>210</v>
@@ -6284,10 +6284,10 @@
         <v>ID-49</v>
       </c>
       <c r="B68" s="117" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C68" s="117" t="s">
-        <v>257</v>
+        <v>381</v>
       </c>
       <c r="D68" s="117" t="s">
         <v>210</v>
@@ -6322,10 +6322,10 @@
         <v>213</v>
       </c>
       <c r="C70" s="117" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D70" s="117" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E70" s="117"/>
       <c r="F70" s="117"/>
@@ -6391,7 +6391,7 @@
         <v>220</v>
       </c>
       <c r="D73" s="117" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="E73" s="117"/>
       <c r="F73" s="117"/>
@@ -6683,7 +6683,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="211" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C2" s="211"/>
       <c r="D2" s="211"/>
@@ -6715,7 +6715,7 @@
         <v>189</v>
       </c>
       <c r="B4" s="212" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C4" s="212"/>
       <c r="D4" s="212"/>
@@ -6845,10 +6845,10 @@
         <v>196</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="117"/>
@@ -6865,10 +6865,10 @@
         <v>67</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D13" s="117" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="E13" s="197"/>
       <c r="F13" s="117"/>
@@ -6885,10 +6885,10 @@
         <v>173</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D14" s="117" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="E14" s="173"/>
       <c r="F14" s="117"/>
@@ -6905,10 +6905,10 @@
         <v>176</v>
       </c>
       <c r="C15" s="117" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D15" s="117" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="E15" s="173"/>
       <c r="F15" s="117"/>
@@ -6925,10 +6925,10 @@
         <v>77</v>
       </c>
       <c r="C16" s="117" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D16" s="117" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="E16" s="173"/>
       <c r="F16" s="117"/>
@@ -6945,10 +6945,10 @@
         <v>69</v>
       </c>
       <c r="C17" s="117" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D17" s="117" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="E17" s="173"/>
       <c r="F17" s="117"/>
@@ -6965,10 +6965,10 @@
         <v>71</v>
       </c>
       <c r="C18" s="117" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="D18" s="117" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E18" s="173"/>
       <c r="F18" s="117"/>
@@ -6985,10 +6985,10 @@
         <v>73</v>
       </c>
       <c r="C19" s="117" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="D19" s="117" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E19" s="173"/>
       <c r="F19" s="117"/>
@@ -7005,10 +7005,10 @@
         <v>75</v>
       </c>
       <c r="C20" s="117" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="D20" s="117" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E20" s="173"/>
       <c r="F20" s="117"/>
@@ -7020,7 +7020,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="176"/>
       <c r="B21" s="177" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="C21" s="176"/>
       <c r="D21" s="176"/>
@@ -7037,13 +7037,13 @@
         <v>[Mod_login-12]</v>
       </c>
       <c r="B22" s="117" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C22" s="117" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="E22" s="179"/>
       <c r="F22" s="117"/>
@@ -7061,10 +7061,10 @@
         <v>198</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="E23" s="179"/>
       <c r="F23" s="117"/>
@@ -7075,7 +7075,7 @@
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
       <c r="A24" s="176" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B24" s="58" t="s">
         <v>81</v>
@@ -7098,10 +7098,10 @@
         <v>82</v>
       </c>
       <c r="C25" s="91" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D25" s="91" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="E25" s="179"/>
       <c r="F25" s="117"/>
@@ -7111,10 +7111,10 @@
     </row>
     <row r="26" spans="1:10" ht="13.5" customHeight="1">
       <c r="A26" s="176" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="C26" s="176"/>
       <c r="D26" s="176"/>
@@ -7130,13 +7130,13 @@
         <v>[Mod_login-17]</v>
       </c>
       <c r="B27" s="117" t="s">
+        <v>298</v>
+      </c>
+      <c r="C27" s="117" t="s">
+        <v>306</v>
+      </c>
+      <c r="D27" s="117" t="s">
         <v>308</v>
-      </c>
-      <c r="C27" s="117" t="s">
-        <v>316</v>
-      </c>
-      <c r="D27" s="117" t="s">
-        <v>318</v>
       </c>
       <c r="E27" s="173"/>
       <c r="F27" s="117"/>
@@ -7146,10 +7146,10 @@
     </row>
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
       <c r="A28" s="176" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>
@@ -7165,13 +7165,13 @@
         <v>[Mod_login-19]</v>
       </c>
       <c r="B29" s="117" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="C29" s="117" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="D29" s="117" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E29" s="173"/>
       <c r="F29" s="117"/>
@@ -7181,10 +7181,10 @@
     </row>
     <row r="30" spans="1:10" ht="13.5" customHeight="1">
       <c r="A30" s="176" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B30" s="58" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="C30" s="176"/>
       <c r="D30" s="176"/>
@@ -7200,13 +7200,13 @@
         <v>[Mod_login-21]</v>
       </c>
       <c r="B31" s="117" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="C31" s="117" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="D31" s="117" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E31" s="173"/>
       <c r="F31" s="117"/>
@@ -7318,7 +7318,7 @@
         <v>189</v>
       </c>
       <c r="B4" s="212" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C4" s="212"/>
       <c r="D4" s="212"/>
@@ -7451,7 +7451,7 @@
         <v>171</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="117"/>
@@ -7474,7 +7474,7 @@
         <v>172</v>
       </c>
       <c r="E13" s="173" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="F13" s="117"/>
       <c r="G13" s="117"/>
@@ -7496,7 +7496,7 @@
         <v>175</v>
       </c>
       <c r="E14" s="173" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="F14" s="117"/>
       <c r="G14" s="117"/>
@@ -7518,7 +7518,7 @@
         <v>178</v>
       </c>
       <c r="E15" s="173" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="F15" s="117"/>
       <c r="G15" s="117"/>
@@ -7540,7 +7540,7 @@
         <v>79</v>
       </c>
       <c r="E16" s="173" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="F16" s="117"/>
       <c r="G16" s="117"/>
@@ -7562,7 +7562,7 @@
         <v>70</v>
       </c>
       <c r="E17" s="173" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="F17" s="117"/>
       <c r="G17" s="117"/>
@@ -7584,7 +7584,7 @@
         <v>72</v>
       </c>
       <c r="E18" s="173" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="F18" s="117"/>
       <c r="G18" s="117"/>
@@ -7606,7 +7606,7 @@
         <v>72</v>
       </c>
       <c r="E19" s="173" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="F19" s="117"/>
       <c r="G19" s="117"/>
@@ -7628,7 +7628,7 @@
         <v>72</v>
       </c>
       <c r="E20" s="173" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="F20" s="117"/>
       <c r="G20" s="117"/>
@@ -7662,10 +7662,10 @@
         <v>171</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="E22" s="179" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="F22" s="117"/>
       <c r="G22" s="117"/>
@@ -7685,10 +7685,10 @@
         <v>182</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="E23" s="179" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="F23" s="117"/>
       <c r="G23" s="117"/>
@@ -7725,7 +7725,7 @@
         <v>200</v>
       </c>
       <c r="E25" s="179" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="F25" s="117"/>
       <c r="G25" s="117"/>
@@ -7771,7 +7771,7 @@
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
       <c r="A28" s="176"/>
       <c r="B28" s="177" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>

</xml_diff>

<commit_message>
final version: integration test case
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
+++ b/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27260" windowHeight="14880" tabRatio="543" activeTab="4"/>
+    <workbookView xWindow="1160" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="383">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -420,15 +420,6 @@
   </si>
   <si>
     <t>Add new</t>
-  </si>
-  <si>
-    <t>Registered User function</t>
-  </si>
-  <si>
-    <t>Integrating all functions of registered user together then execute test</t>
-  </si>
-  <si>
-    <t>Registered_User_function</t>
   </si>
   <si>
     <t>Login</t>
@@ -1857,6 +1848,18 @@
 3. Copy link
 4. Change to other browser
 5. Paste link and press Enter</t>
+  </si>
+  <si>
+    <t>User function</t>
+  </si>
+  <si>
+    <t>Integrating all functions of user together then execute test</t>
+  </si>
+  <si>
+    <t>User_Function</t>
+  </si>
+  <si>
+    <t>Mod_Function</t>
   </si>
 </sst>
 </file>
@@ -2809,7 +2812,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3392,6 +3395,7 @@
     <xf numFmtId="0" fontId="27" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -3937,7 +3941,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="200" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D4" s="200"/>
       <c r="E4" s="200"/>
@@ -3945,7 +3949,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
@@ -3953,7 +3957,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="200" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D5" s="200"/>
       <c r="E5" s="200"/>
@@ -3961,7 +3965,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
@@ -4045,7 +4049,7 @@
         <v>55</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="19" customFormat="1" ht="21.75" customHeight="1">
@@ -4124,8 +4128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4181,7 +4185,7 @@
       </c>
       <c r="C5" s="203"/>
       <c r="D5" s="204" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E5" s="204"/>
       <c r="F5" s="204"/>
@@ -4217,21 +4221,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="39">
+    <row r="9" spans="2:6" ht="26">
       <c r="B9" s="46">
         <v>1</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>56</v>
+        <v>379</v>
       </c>
       <c r="D9" s="149" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="114" t="s">
-        <v>57</v>
+        <v>380</v>
       </c>
       <c r="F9" s="113" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="26">
@@ -4248,7 +4252,7 @@
         <v>52</v>
       </c>
       <c r="F10" s="113" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="17">
@@ -4350,10 +4354,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4401,7 +4405,7 @@
       </c>
       <c r="F3" s="207"/>
       <c r="G3" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H3" s="65"/>
     </row>
@@ -4419,7 +4423,7 @@
       </c>
       <c r="F4" s="207"/>
       <c r="G4" s="10" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H4" s="65"/>
     </row>
@@ -4510,7 +4514,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="149" t="s">
-        <v>58</v>
+        <v>381</v>
       </c>
       <c r="D11" s="76">
         <f>User_Function!A6</f>
@@ -4533,98 +4537,110 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="17">
       <c r="A12" s="75"/>
       <c r="B12" s="151">
         <v>2</v>
       </c>
-      <c r="C12" s="149" t="s">
-        <v>80</v>
+      <c r="C12" s="217" t="s">
+        <v>382</v>
       </c>
       <c r="D12" s="76">
+        <f>Mod_Function!A6</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="76">
+        <f>Mod_Function!B6</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="76">
+        <f>Mod_Function!C6</f>
+        <v>38</v>
+      </c>
+      <c r="G12" s="76">
+        <f>Mod_Function!D6</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="77">
+        <f>Mod_Function!E6</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="75"/>
+      <c r="B13" s="151">
+        <v>3</v>
+      </c>
+      <c r="C13" s="149" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="76">
         <f>Admin_Function!A6</f>
         <v>0</v>
       </c>
-      <c r="E12" s="76">
+      <c r="E13" s="76">
         <f>Admin_Function!B6</f>
         <v>0</v>
       </c>
-      <c r="F12" s="76">
+      <c r="F13" s="76">
         <f>Admin_Function!C6</f>
         <v>26</v>
       </c>
-      <c r="G12" s="76">
+      <c r="G13" s="76">
         <f>Admin_Function!D6</f>
         <v>0</v>
       </c>
-      <c r="H12" s="77">
+      <c r="H13" s="77">
         <f>Admin_Function!E6</f>
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="75"/>
-      <c r="B13" s="152"/>
-      <c r="C13" s="78" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="79">
-        <f>SUM(D9:D12)</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="79">
-        <f>SUM(E9:E12)</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="79">
-        <f>SUM(F9:F12)</f>
-        <v>148</v>
-      </c>
-      <c r="G13" s="79">
-        <f>SUM(G9:G12)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="80">
-        <f>SUM(H9:H12)</f>
-        <v>148</v>
-      </c>
-    </row>
     <row r="14" spans="1:8">
       <c r="A14" s="70"/>
-      <c r="B14" s="81"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
+      <c r="B14" s="152"/>
+      <c r="C14" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="79">
+        <f>SUM(D11:D13)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="79">
+        <f>SUM(E11:E13)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="79">
+        <f>SUM(F11:F13)</f>
+        <v>186</v>
+      </c>
+      <c r="G14" s="79">
+        <f>SUM(G9:G13)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="80">
+        <f>SUM(H11:H13)</f>
+        <v>186</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="70"/>
-      <c r="B15" s="70"/>
-      <c r="C15" s="84" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="70"/>
-      <c r="E15" s="85">
-        <f>(D13+E13)*100/(H13-G13)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="70"/>
-      <c r="H15" s="55"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="83"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="70"/>
       <c r="B16" s="70"/>
       <c r="C16" s="84" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D16" s="70"/>
       <c r="E16" s="85">
-        <f>D13*100/(H13-G13)</f>
+        <f>(D14+E14)*100/(H14-G14)</f>
         <v>0</v>
       </c>
       <c r="F16" s="70" t="s">
@@ -4633,12 +4649,28 @@
       <c r="G16" s="70"/>
       <c r="H16" s="55"/>
     </row>
-    <row r="17" spans="3:4">
-      <c r="C17" s="70"/>
+    <row r="17" spans="2:8">
+      <c r="B17" s="70"/>
+      <c r="C17" s="84" t="s">
+        <v>44</v>
+      </c>
       <c r="D17" s="70"/>
-    </row>
-    <row r="18" spans="3:4" ht="17">
-      <c r="C18" s="198"/>
+      <c r="E17" s="85">
+        <f>D14*100/(H14-G14)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="70"/>
+      <c r="H17" s="55"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+    </row>
+    <row r="19" spans="2:8" ht="17">
+      <c r="C19" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4653,8 +4685,9 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C12" location="Admin_Function!A1" display="Admin_function"/>
+    <hyperlink ref="C13" location="Admin_Function!A1" display="Admin_function"/>
     <hyperlink ref="C11" location="User_Function!A1" display="User_function"/>
+    <hyperlink ref="C12" location="Mod_Function!A1" display="Mod_Function"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777783" bottom="0.98402777777777772" header="0.51180555555555562" footer="0.5"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -4687,7 +4720,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1">
       <c r="A1" s="210" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="210"/>
       <c r="C1" s="210"/>
@@ -4698,279 +4731,279 @@
         <v>16</v>
       </c>
       <c r="B3" s="156" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C3" s="157" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13">
       <c r="A4" s="158" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B4" s="159" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C4" s="159"/>
     </row>
     <row r="5" spans="1:3" ht="13">
       <c r="A5" s="158" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B5" s="159" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C5" s="159"/>
     </row>
     <row r="6" spans="1:3" ht="13">
       <c r="A6" s="158" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B6" s="159" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C6" s="159"/>
     </row>
     <row r="7" spans="1:3" ht="13">
       <c r="A7" s="158" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B7" s="159" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C7" s="159"/>
     </row>
     <row r="8" spans="1:3" ht="13">
       <c r="A8" s="158" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B8" s="159" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C8" s="159"/>
     </row>
     <row r="9" spans="1:3" ht="13">
       <c r="A9" s="158" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B9" s="159" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C9" s="159"/>
     </row>
     <row r="10" spans="1:3" ht="13">
       <c r="A10" s="158" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B10" s="159" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C10" s="159"/>
     </row>
     <row r="11" spans="1:3" ht="13">
       <c r="A11" s="158" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B11" s="159" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C11" s="159"/>
     </row>
     <row r="12" spans="1:3" ht="13">
       <c r="A12" s="158" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B12" s="159" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C12" s="159"/>
     </row>
     <row r="13" spans="1:3" ht="13">
       <c r="A13" s="158" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B13" s="159" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C13" s="159"/>
     </row>
     <row r="14" spans="1:3" ht="13">
       <c r="A14" s="158" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B14" s="160" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C14" s="159"/>
     </row>
     <row r="15" spans="1:3" ht="13">
       <c r="A15" s="158" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B15" s="159" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C15" s="159"/>
     </row>
     <row r="16" spans="1:3" ht="13">
       <c r="A16" s="158" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B16" s="159" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C16" s="159"/>
     </row>
     <row r="17" spans="1:3" ht="13">
       <c r="A17" s="158" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B17" s="159" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C17" s="159"/>
     </row>
     <row r="18" spans="1:3" ht="13">
       <c r="A18" s="158" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B18" s="159" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C18" s="159"/>
     </row>
     <row r="19" spans="1:3" ht="13">
       <c r="A19" s="158" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B19" s="160" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C19" s="159"/>
     </row>
     <row r="20" spans="1:3" ht="13">
       <c r="A20" s="158" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B20" s="160" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C20" s="159"/>
     </row>
     <row r="21" spans="1:3" ht="13">
       <c r="A21" s="158" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B21" s="160" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C21" s="159"/>
     </row>
     <row r="22" spans="1:3" ht="52">
       <c r="A22" s="158" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B22" s="161" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C22" s="159"/>
     </row>
     <row r="23" spans="1:3" ht="13">
       <c r="A23" s="158" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B23" s="159" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C23" s="159"/>
     </row>
     <row r="24" spans="1:3" ht="13">
       <c r="A24" s="158" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B24" s="159" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C24" s="159"/>
     </row>
     <row r="25" spans="1:3" ht="13">
       <c r="A25" s="158" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B25" s="159" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C25" s="159"/>
     </row>
     <row r="26" spans="1:3" ht="13">
       <c r="A26" s="162" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B26" s="159" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C26" s="159"/>
     </row>
     <row r="27" spans="1:3" ht="13">
       <c r="A27" s="162" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B27" s="159" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C27" s="159"/>
     </row>
     <row r="28" spans="1:3" ht="13">
       <c r="A28" s="162" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B28" s="159" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C28" s="159"/>
     </row>
     <row r="29" spans="1:3" ht="13">
       <c r="A29" s="162" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B29" s="159" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C29" s="159"/>
     </row>
     <row r="30" spans="1:3" ht="13">
       <c r="A30" s="162" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B30" s="159" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C30" s="159"/>
     </row>
     <row r="31" spans="1:3" ht="13">
       <c r="A31" s="162" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B31" s="159"/>
       <c r="C31" s="159"/>
     </row>
     <row r="32" spans="1:3" ht="13">
       <c r="A32" s="162" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B32" s="159"/>
       <c r="C32" s="159"/>
     </row>
     <row r="33" spans="1:3" ht="13">
       <c r="A33" s="162" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B33" s="159"/>
       <c r="C33" s="159"/>
     </row>
     <row r="34" spans="1:3" ht="13">
       <c r="A34" s="162" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B34" s="159"/>
       <c r="C34" s="159"/>
@@ -4993,9 +5026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -5071,7 +5102,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="212" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C4" s="212"/>
       <c r="D4" s="212"/>
@@ -5192,10 +5223,10 @@
         <v>34</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H10" s="57" t="s">
         <v>35</v>
@@ -5208,7 +5239,7 @@
     <row r="11" spans="1:10" ht="14.25" customHeight="1">
       <c r="A11" s="133"/>
       <c r="B11" s="58" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C11" s="58"/>
       <c r="D11" s="58"/>
@@ -5225,13 +5256,13 @@
         <v>[User_login-2]</v>
       </c>
       <c r="B12" s="117" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E12" s="118"/>
       <c r="F12" s="117"/>
@@ -5246,13 +5277,13 @@
         <v>[User_login-3]</v>
       </c>
       <c r="B13" s="117" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D13" s="117" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E13" s="118"/>
       <c r="F13" s="117"/>
@@ -5267,13 +5298,13 @@
         <v>[User_login-4]</v>
       </c>
       <c r="B14" s="121" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D14" s="121" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E14" s="122"/>
       <c r="F14" s="117"/>
@@ -5288,13 +5319,13 @@
         <v>[User_login-5]</v>
       </c>
       <c r="B15" s="124" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C15" s="124" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D15" s="124" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E15" s="118"/>
       <c r="F15" s="117"/>
@@ -5309,13 +5340,13 @@
         <v>[User_login-6]</v>
       </c>
       <c r="B16" s="124" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C16" s="124" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D16" s="124" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E16" s="125"/>
       <c r="F16" s="117"/>
@@ -5330,13 +5361,13 @@
         <v>[User_login-7]</v>
       </c>
       <c r="B17" s="124" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C17" s="124" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D17" s="124" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E17" s="125"/>
       <c r="F17" s="117"/>
@@ -5351,13 +5382,13 @@
         <v>[User_login-8]</v>
       </c>
       <c r="B18" s="124" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18" s="124" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D18" s="124" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E18" s="125"/>
       <c r="F18" s="117"/>
@@ -5369,7 +5400,7 @@
     <row r="19" spans="1:10" ht="14.25" customHeight="1">
       <c r="A19" s="58"/>
       <c r="B19" s="58" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="59"/>
@@ -5386,16 +5417,16 @@
         <v>[User_login-10]</v>
       </c>
       <c r="B20" s="91" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C20" s="91" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D20" s="91" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E20" s="91" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F20" s="117"/>
       <c r="G20" s="91"/>
@@ -5406,7 +5437,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="58"/>
       <c r="B21" s="58" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
@@ -5423,16 +5454,16 @@
         <v>[User_login-12]</v>
       </c>
       <c r="B22" s="91" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C22" s="91" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D22" s="91" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E22" s="91" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F22" s="117"/>
       <c r="G22" s="91"/>
@@ -5446,13 +5477,13 @@
         <v>[User_login-13]</v>
       </c>
       <c r="B23" s="91" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C23" s="91" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D23" s="91" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E23" s="91"/>
       <c r="F23" s="117"/>
@@ -5467,16 +5498,16 @@
         <v>[User_login-14]</v>
       </c>
       <c r="B24" s="91" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C24" s="91" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D24" s="91" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E24" s="91" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F24" s="117"/>
       <c r="G24" s="91"/>
@@ -5487,7 +5518,7 @@
     <row r="25" spans="1:10" ht="14.25" customHeight="1">
       <c r="A25" s="58"/>
       <c r="B25" s="58" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C25" s="59"/>
       <c r="D25" s="59"/>
@@ -5504,16 +5535,16 @@
         <v>[User_login-16]</v>
       </c>
       <c r="B26" s="91" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C26" s="91" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D26" s="136" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E26" s="91" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F26" s="91"/>
       <c r="G26" s="91"/>
@@ -5527,16 +5558,16 @@
         <v>[User_login-17]</v>
       </c>
       <c r="B27" s="91" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C27" s="91" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D27" s="91" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E27" s="91" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F27" s="91"/>
       <c r="G27" s="91"/>
@@ -5547,7 +5578,7 @@
     <row r="28" spans="1:10" ht="14.25" customHeight="1">
       <c r="A28" s="58"/>
       <c r="B28" s="58" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C28" s="59"/>
       <c r="D28" s="59"/>
@@ -5564,16 +5595,16 @@
         <v>[User_login-19]</v>
       </c>
       <c r="B29" s="91" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C29" s="106" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D29" s="104" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E29" s="104" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F29" s="117"/>
       <c r="G29" s="91"/>
@@ -5587,16 +5618,16 @@
         <v>[User_login-20]</v>
       </c>
       <c r="B30" s="91" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C30" s="106" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D30" s="104" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E30" s="104" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F30" s="117"/>
       <c r="G30" s="165"/>
@@ -5606,10 +5637,10 @@
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1">
       <c r="A31" s="58" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C31" s="59"/>
       <c r="D31" s="59"/>
@@ -5626,13 +5657,13 @@
         <v>[User_login-22]</v>
       </c>
       <c r="B32" s="91" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C32" s="106" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D32" s="104" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E32" s="104"/>
       <c r="F32" s="117"/>
@@ -5647,13 +5678,13 @@
         <v>[User_login-23]</v>
       </c>
       <c r="B33" s="91" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C33" s="106" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D33" s="104" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E33" s="104"/>
       <c r="F33" s="117"/>
@@ -5664,10 +5695,10 @@
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
       <c r="A34" s="58" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B34" s="58" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="59"/>
@@ -5684,13 +5715,13 @@
         <v>[User_login-25]</v>
       </c>
       <c r="B35" s="91" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C35" s="106" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D35" s="104" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E35" s="104"/>
       <c r="F35" s="117"/>
@@ -5702,7 +5733,7 @@
     <row r="36" spans="1:10" ht="14.25" customHeight="1">
       <c r="A36" s="169"/>
       <c r="B36" s="169" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C36" s="166"/>
       <c r="D36" s="166"/>
@@ -5719,13 +5750,13 @@
         <v>[User_login-27]</v>
       </c>
       <c r="B37" s="117" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C37" s="117" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D37" s="117" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E37" s="118"/>
       <c r="F37" s="117"/>
@@ -5740,13 +5771,13 @@
         <v>[User_login-28]</v>
       </c>
       <c r="B38" s="117" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C38" s="117" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D38" s="117" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E38" s="118"/>
       <c r="F38" s="117"/>
@@ -5757,10 +5788,10 @@
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1">
       <c r="A39" s="169" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B39" s="169" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C39" s="166"/>
       <c r="D39" s="166"/>
@@ -5777,13 +5808,13 @@
         <v>[User_login-30]</v>
       </c>
       <c r="B40" s="117" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C40" s="117" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D40" s="117" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E40" s="118"/>
       <c r="F40" s="117"/>
@@ -5794,10 +5825,10 @@
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1">
       <c r="A41" s="169" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B41" s="169" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C41" s="166"/>
       <c r="D41" s="166"/>
@@ -5814,13 +5845,13 @@
         <v>[User_login-32]</v>
       </c>
       <c r="B42" s="117" t="s">
+        <v>316</v>
+      </c>
+      <c r="C42" s="117" t="s">
+        <v>326</v>
+      </c>
+      <c r="D42" s="117" t="s">
         <v>319</v>
-      </c>
-      <c r="C42" s="117" t="s">
-        <v>329</v>
-      </c>
-      <c r="D42" s="117" t="s">
-        <v>322</v>
       </c>
       <c r="E42" s="118"/>
       <c r="F42" s="117"/>
@@ -5831,10 +5862,10 @@
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1">
       <c r="A43" s="169" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B43" s="169" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C43" s="166"/>
       <c r="D43" s="166"/>
@@ -5851,13 +5882,13 @@
         <v>[User_login-34]</v>
       </c>
       <c r="B44" s="117" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C44" s="117" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D44" s="117" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E44" s="118"/>
       <c r="F44" s="117"/>
@@ -5868,10 +5899,10 @@
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1">
       <c r="A45" s="169" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B45" s="169" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C45" s="166"/>
       <c r="D45" s="166"/>
@@ -5888,13 +5919,13 @@
         <v>[User_login-36]</v>
       </c>
       <c r="B46" s="117" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C46" s="117" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D46" s="117" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E46" s="118"/>
       <c r="F46" s="117"/>
@@ -5905,10 +5936,10 @@
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1">
       <c r="A47" s="169" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B47" s="169" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C47" s="166"/>
       <c r="D47" s="166"/>
@@ -5925,13 +5956,13 @@
         <v>[User_login-38]</v>
       </c>
       <c r="B48" s="117" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C48" s="117" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D48" s="117" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E48" s="118"/>
       <c r="F48" s="117"/>
@@ -5942,10 +5973,10 @@
     </row>
     <row r="49" spans="1:10" ht="14.25" customHeight="1">
       <c r="A49" s="169" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B49" s="169" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C49" s="166"/>
       <c r="D49" s="166"/>
@@ -5962,13 +5993,13 @@
         <v>[User_login-40]</v>
       </c>
       <c r="B50" s="117" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C50" s="117" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D50" s="117" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E50" s="118"/>
       <c r="F50" s="117"/>
@@ -5979,10 +6010,10 @@
     </row>
     <row r="51" spans="1:10" ht="14.25" customHeight="1">
       <c r="A51" s="169" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B51" s="169" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C51" s="166"/>
       <c r="D51" s="166"/>
@@ -5999,13 +6030,13 @@
         <v>[User_login-42]</v>
       </c>
       <c r="B52" s="117" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C52" s="117" t="s">
+        <v>353</v>
+      </c>
+      <c r="D52" s="117" t="s">
         <v>356</v>
-      </c>
-      <c r="D52" s="117" t="s">
-        <v>359</v>
       </c>
       <c r="E52" s="118"/>
       <c r="F52" s="117"/>
@@ -6016,10 +6047,10 @@
     </row>
     <row r="53" spans="1:10" ht="14.25" customHeight="1">
       <c r="A53" s="169" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B53" s="169" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C53" s="166"/>
       <c r="D53" s="166"/>
@@ -6036,13 +6067,13 @@
         <v>[User_login-44]</v>
       </c>
       <c r="B54" s="117" t="s">
+        <v>360</v>
+      </c>
+      <c r="C54" s="117" t="s">
+        <v>364</v>
+      </c>
+      <c r="D54" s="117" t="s">
         <v>363</v>
-      </c>
-      <c r="C54" s="117" t="s">
-        <v>367</v>
-      </c>
-      <c r="D54" s="117" t="s">
-        <v>366</v>
       </c>
       <c r="E54" s="118"/>
       <c r="F54" s="117"/>
@@ -6052,10 +6083,10 @@
     </row>
     <row r="55" spans="1:10" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A55" s="169" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B55" s="169" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C55" s="166"/>
       <c r="D55" s="166"/>
@@ -6071,13 +6102,13 @@
         <v>[User_login-46]</v>
       </c>
       <c r="B56" s="117" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C56" s="117" t="s">
+        <v>365</v>
+      </c>
+      <c r="D56" s="117" t="s">
         <v>368</v>
-      </c>
-      <c r="D56" s="117" t="s">
-        <v>371</v>
       </c>
       <c r="E56" s="118"/>
       <c r="F56" s="117"/>
@@ -6087,10 +6118,10 @@
     </row>
     <row r="57" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A57" s="169" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B57" s="169" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C57" s="166"/>
       <c r="D57" s="166"/>
@@ -6106,13 +6137,13 @@
         <v>[User_login-48]</v>
       </c>
       <c r="B58" s="117" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C58" s="117" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D58" s="117" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E58" s="118"/>
       <c r="F58" s="117"/>
@@ -6145,7 +6176,7 @@
     <row r="61" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A61" s="169"/>
       <c r="B61" s="169" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C61" s="169"/>
       <c r="D61" s="169"/>
@@ -6158,7 +6189,7 @@
     <row r="62" spans="1:10" s="169" customFormat="1" ht="14.25" customHeight="1">
       <c r="A62" s="185"/>
       <c r="B62" s="186" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C62" s="187"/>
       <c r="D62" s="187"/>
@@ -6174,20 +6205,20 @@
         <v>ID-44</v>
       </c>
       <c r="B63" s="117" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C63" s="117" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D63" s="117" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E63" s="117"/>
       <c r="F63" s="117"/>
       <c r="G63" s="117"/>
       <c r="H63" s="117"/>
       <c r="I63" s="188" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="190" customFormat="1" ht="14.25" customHeight="1">
@@ -6196,20 +6227,20 @@
         <v>ID-45</v>
       </c>
       <c r="B64" s="117" t="s">
+        <v>371</v>
+      </c>
+      <c r="C64" s="117" t="s">
         <v>374</v>
       </c>
-      <c r="C64" s="117" t="s">
-        <v>377</v>
-      </c>
       <c r="D64" s="117" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E64" s="117"/>
       <c r="F64" s="117"/>
       <c r="G64" s="117"/>
       <c r="H64" s="117"/>
       <c r="I64" s="188" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="190" customFormat="1" ht="14.25" customHeight="1">
@@ -6218,20 +6249,20 @@
         <v>ID-46</v>
       </c>
       <c r="B65" s="117" t="s">
+        <v>372</v>
+      </c>
+      <c r="C65" s="117" t="s">
         <v>375</v>
       </c>
-      <c r="C65" s="117" t="s">
-        <v>378</v>
-      </c>
       <c r="D65" s="117" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E65" s="117"/>
       <c r="F65" s="117"/>
       <c r="G65" s="117"/>
       <c r="H65" s="117"/>
       <c r="I65" s="188" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="189" customFormat="1" ht="14.25" customHeight="1">
@@ -6240,20 +6271,20 @@
         <v>ID-47</v>
       </c>
       <c r="B66" s="117" t="s">
+        <v>373</v>
+      </c>
+      <c r="C66" s="117" t="s">
         <v>376</v>
       </c>
-      <c r="C66" s="117" t="s">
-        <v>379</v>
-      </c>
       <c r="D66" s="117" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E66" s="117"/>
       <c r="F66" s="117"/>
       <c r="G66" s="117"/>
       <c r="H66" s="117"/>
       <c r="I66" s="188" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6262,20 +6293,20 @@
         <v>ID-48</v>
       </c>
       <c r="B67" s="117" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C67" s="117" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D67" s="117" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E67" s="117"/>
       <c r="F67" s="117"/>
       <c r="G67" s="117"/>
       <c r="H67" s="117"/>
       <c r="I67" s="188" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6284,26 +6315,26 @@
         <v>ID-49</v>
       </c>
       <c r="B68" s="117" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C68" s="117" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D68" s="117" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E68" s="117"/>
       <c r="F68" s="117"/>
       <c r="G68" s="117"/>
       <c r="H68" s="117"/>
       <c r="I68" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A69" s="169"/>
       <c r="B69" s="169" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C69" s="169"/>
       <c r="D69" s="169"/>
@@ -6319,20 +6350,20 @@
         <v>ID-50</v>
       </c>
       <c r="B70" s="117" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C70" s="117" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D70" s="117" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E70" s="117"/>
       <c r="F70" s="117"/>
       <c r="G70" s="117"/>
       <c r="H70" s="117"/>
       <c r="I70" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6341,20 +6372,20 @@
         <v>ID-51</v>
       </c>
       <c r="B71" s="117" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C71" s="117" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D71" s="117" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E71" s="117"/>
       <c r="F71" s="117"/>
       <c r="G71" s="117"/>
       <c r="H71" s="117"/>
       <c r="I71" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6363,20 +6394,20 @@
         <v>ID-52</v>
       </c>
       <c r="B72" s="117" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C72" s="117" t="s">
+        <v>212</v>
+      </c>
+      <c r="D72" s="117" t="s">
         <v>215</v>
-      </c>
-      <c r="D72" s="117" t="s">
-        <v>218</v>
       </c>
       <c r="E72" s="117"/>
       <c r="F72" s="117"/>
       <c r="G72" s="117"/>
       <c r="H72" s="117"/>
       <c r="I72" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6385,20 +6416,20 @@
         <v>ID-53</v>
       </c>
       <c r="B73" s="117" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C73" s="117" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D73" s="117" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E73" s="117"/>
       <c r="F73" s="117"/>
       <c r="G73" s="117"/>
       <c r="H73" s="117"/>
       <c r="I73" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6407,20 +6438,20 @@
         <v>ID-54</v>
       </c>
       <c r="B74" s="117" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C74" s="117" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D74" s="117" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E74" s="117"/>
       <c r="F74" s="117"/>
       <c r="G74" s="117"/>
       <c r="H74" s="117"/>
       <c r="I74" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6429,20 +6460,20 @@
         <v>ID-55</v>
       </c>
       <c r="B75" s="117" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C75" s="117" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D75" s="117" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E75" s="117"/>
       <c r="F75" s="117"/>
       <c r="G75" s="117"/>
       <c r="H75" s="117"/>
       <c r="I75" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="13.5" customHeight="1">
@@ -6451,20 +6482,20 @@
         <v>ID-56</v>
       </c>
       <c r="B76" s="117" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C76" s="117" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D76" s="117" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E76" s="117"/>
       <c r="F76" s="117"/>
       <c r="G76" s="117"/>
       <c r="H76" s="117"/>
       <c r="I76" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="13.5" customHeight="1">
@@ -6473,20 +6504,20 @@
         <v>ID-57</v>
       </c>
       <c r="B77" s="117" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C77" s="117" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D77" s="117" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E77" s="117"/>
       <c r="F77" s="117"/>
       <c r="G77" s="117"/>
       <c r="H77" s="117"/>
       <c r="I77" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="13.5" customHeight="1">
@@ -6495,20 +6526,20 @@
         <v>ID-58</v>
       </c>
       <c r="B78" s="117" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C78" s="117" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D78" s="117" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E78" s="117"/>
       <c r="F78" s="117"/>
       <c r="G78" s="117"/>
       <c r="H78" s="117"/>
       <c r="I78" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="13.5" customHeight="1">
@@ -6517,20 +6548,20 @@
         <v>ID-59</v>
       </c>
       <c r="B79" s="117" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C79" s="117" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D79" s="117" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E79" s="117"/>
       <c r="F79" s="117"/>
       <c r="G79" s="117"/>
       <c r="H79" s="117"/>
       <c r="I79" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13.5" customHeight="1">
@@ -6539,20 +6570,20 @@
         <v>ID-60</v>
       </c>
       <c r="B80" s="117" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C80" s="117" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D80" s="117" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E80" s="117"/>
       <c r="F80" s="117"/>
       <c r="G80" s="117"/>
       <c r="H80" s="117"/>
       <c r="I80" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="13.5" customHeight="1">
@@ -6561,20 +6592,20 @@
         <v>ID-61</v>
       </c>
       <c r="B81" s="117" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C81" s="117" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D81" s="117" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E81" s="117"/>
       <c r="F81" s="117"/>
       <c r="G81" s="117"/>
       <c r="H81" s="117"/>
       <c r="I81" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="13.5" customHeight="1">
@@ -6583,20 +6614,20 @@
         <v>ID-62</v>
       </c>
       <c r="B82" s="117" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C82" s="117" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D82" s="117" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E82" s="117"/>
       <c r="F82" s="117"/>
       <c r="G82" s="117"/>
       <c r="H82" s="117"/>
       <c r="I82" s="117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -6645,9 +6676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -6669,7 +6698,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="137" customFormat="1" ht="18" thickBot="1">
       <c r="A1" s="138" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B1" s="139"/>
       <c r="C1" s="139"/>
@@ -6683,7 +6712,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="211" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C2" s="211"/>
       <c r="D2" s="211"/>
@@ -6696,10 +6725,10 @@
     </row>
     <row r="3" spans="1:10" s="137" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="142" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B3" s="211" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C3" s="211"/>
       <c r="D3" s="211"/>
@@ -6712,10 +6741,10 @@
     </row>
     <row r="4" spans="1:10" s="137" customFormat="1" ht="17">
       <c r="A4" s="141" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B4" s="212" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C4" s="212"/>
       <c r="D4" s="212"/>
@@ -6732,13 +6761,13 @@
         <v>24</v>
       </c>
       <c r="C5" s="144" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D5" s="145" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="215" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F5" s="215"/>
       <c r="G5" s="215"/>
@@ -6799,25 +6828,25 @@
         <v>30</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I10" s="56" t="s">
         <v>36</v>
@@ -6826,7 +6855,7 @@
     <row r="11" spans="1:10" s="137" customFormat="1" ht="14.25" customHeight="1">
       <c r="A11" s="133"/>
       <c r="B11" s="58" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C11" s="58"/>
       <c r="D11" s="58"/>
@@ -6842,13 +6871,13 @@
         <v>[Mod_login-2]</v>
       </c>
       <c r="B12" s="117" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="117"/>
@@ -6862,13 +6891,13 @@
         <v>[Mod_login-3]</v>
       </c>
       <c r="B13" s="117" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D13" s="117" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E13" s="197"/>
       <c r="F13" s="117"/>
@@ -6882,13 +6911,13 @@
         <v>[Mod_login-4]</v>
       </c>
       <c r="B14" s="117" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D14" s="117" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E14" s="173"/>
       <c r="F14" s="117"/>
@@ -6902,13 +6931,13 @@
         <v>[Mod_login-5]</v>
       </c>
       <c r="B15" s="117" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C15" s="117" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D15" s="117" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E15" s="173"/>
       <c r="F15" s="117"/>
@@ -6922,13 +6951,13 @@
         <v>[Mod_login-6]</v>
       </c>
       <c r="B16" s="117" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C16" s="117" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D16" s="117" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E16" s="173"/>
       <c r="F16" s="117"/>
@@ -6942,13 +6971,13 @@
         <v>[Mod_login-7]</v>
       </c>
       <c r="B17" s="117" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" s="117" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D17" s="117" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E17" s="173"/>
       <c r="F17" s="117"/>
@@ -6962,13 +6991,13 @@
         <v>[Mod_login-8]</v>
       </c>
       <c r="B18" s="117" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C18" s="117" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D18" s="117" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E18" s="173"/>
       <c r="F18" s="117"/>
@@ -6982,13 +7011,13 @@
         <v>[Mod_login-9]</v>
       </c>
       <c r="B19" s="117" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C19" s="117" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D19" s="117" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E19" s="173"/>
       <c r="F19" s="117"/>
@@ -7002,13 +7031,13 @@
         <v>[Mod_login-10]</v>
       </c>
       <c r="B20" s="117" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C20" s="117" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D20" s="117" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E20" s="173"/>
       <c r="F20" s="117"/>
@@ -7020,7 +7049,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="176"/>
       <c r="B21" s="177" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C21" s="176"/>
       <c r="D21" s="176"/>
@@ -7037,13 +7066,13 @@
         <v>[Mod_login-12]</v>
       </c>
       <c r="B22" s="117" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C22" s="117" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E22" s="179"/>
       <c r="F22" s="117"/>
@@ -7058,13 +7087,13 @@
         <v>[Mod_login-13]</v>
       </c>
       <c r="B23" s="117" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E23" s="179"/>
       <c r="F23" s="117"/>
@@ -7075,10 +7104,10 @@
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
       <c r="A24" s="176" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C24" s="176"/>
       <c r="D24" s="176"/>
@@ -7095,13 +7124,13 @@
         <v>[Mod_login-15]</v>
       </c>
       <c r="B25" s="91" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C25" s="91" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D25" s="91" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E25" s="179"/>
       <c r="F25" s="117"/>
@@ -7111,10 +7140,10 @@
     </row>
     <row r="26" spans="1:10" ht="13.5" customHeight="1">
       <c r="A26" s="176" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C26" s="176"/>
       <c r="D26" s="176"/>
@@ -7130,13 +7159,13 @@
         <v>[Mod_login-17]</v>
       </c>
       <c r="B27" s="117" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C27" s="117" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D27" s="117" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E27" s="173"/>
       <c r="F27" s="117"/>
@@ -7146,10 +7175,10 @@
     </row>
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
       <c r="A28" s="176" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>
@@ -7165,13 +7194,13 @@
         <v>[Mod_login-19]</v>
       </c>
       <c r="B29" s="117" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C29" s="117" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D29" s="117" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E29" s="173"/>
       <c r="F29" s="117"/>
@@ -7181,10 +7210,10 @@
     </row>
     <row r="30" spans="1:10" ht="13.5" customHeight="1">
       <c r="A30" s="176" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B30" s="58" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C30" s="176"/>
       <c r="D30" s="176"/>
@@ -7200,13 +7229,13 @@
         <v>[Mod_login-21]</v>
       </c>
       <c r="B31" s="117" t="s">
+        <v>310</v>
+      </c>
+      <c r="C31" s="117" t="s">
+        <v>312</v>
+      </c>
+      <c r="D31" s="117" t="s">
         <v>313</v>
-      </c>
-      <c r="C31" s="117" t="s">
-        <v>315</v>
-      </c>
-      <c r="D31" s="117" t="s">
-        <v>316</v>
       </c>
       <c r="E31" s="173"/>
       <c r="F31" s="117"/>
@@ -7248,9 +7277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -7272,7 +7299,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="137" customFormat="1" ht="18" thickBot="1">
       <c r="A1" s="138" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B1" s="139"/>
       <c r="C1" s="139"/>
@@ -7299,10 +7326,10 @@
     </row>
     <row r="3" spans="1:10" s="137" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="142" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B3" s="211" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C3" s="211"/>
       <c r="D3" s="211"/>
@@ -7315,10 +7342,10 @@
     </row>
     <row r="4" spans="1:10" s="137" customFormat="1" ht="17">
       <c r="A4" s="141" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B4" s="212" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C4" s="212"/>
       <c r="D4" s="212"/>
@@ -7335,13 +7362,13 @@
         <v>24</v>
       </c>
       <c r="C5" s="144" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D5" s="145" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="215" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F5" s="215"/>
       <c r="G5" s="215"/>
@@ -7402,25 +7429,25 @@
         <v>30</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I10" s="56" t="s">
         <v>36</v>
@@ -7429,7 +7456,7 @@
     <row r="11" spans="1:10" s="137" customFormat="1" ht="14.25" customHeight="1">
       <c r="A11" s="170"/>
       <c r="B11" s="216" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C11" s="216"/>
       <c r="D11" s="216"/>
@@ -7445,13 +7472,13 @@
         <v>[Admin_login-2]</v>
       </c>
       <c r="B12" s="117" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="117"/>
@@ -7465,16 +7492,16 @@
         <v>[Admin_login-3]</v>
       </c>
       <c r="B13" s="117" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D13" s="117" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E13" s="173" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F13" s="117"/>
       <c r="G13" s="117"/>
@@ -7487,16 +7514,16 @@
         <v>[Admin_login-4]</v>
       </c>
       <c r="B14" s="117" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D14" s="117" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E14" s="173" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F14" s="117"/>
       <c r="G14" s="117"/>
@@ -7509,16 +7536,16 @@
         <v>[Admin_login-5]</v>
       </c>
       <c r="B15" s="117" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C15" s="117" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D15" s="117" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E15" s="173" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F15" s="117"/>
       <c r="G15" s="117"/>
@@ -7531,16 +7558,16 @@
         <v>[Admin_login-6]</v>
       </c>
       <c r="B16" s="117" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C16" s="117" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D16" s="117" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E16" s="173" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F16" s="117"/>
       <c r="G16" s="117"/>
@@ -7553,16 +7580,16 @@
         <v>[Admin_login-7]</v>
       </c>
       <c r="B17" s="117" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" s="117" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D17" s="117" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E17" s="173" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F17" s="117"/>
       <c r="G17" s="117"/>
@@ -7575,16 +7602,16 @@
         <v>[Admin_login-8]</v>
       </c>
       <c r="B18" s="117" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C18" s="117" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D18" s="117" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E18" s="173" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F18" s="117"/>
       <c r="G18" s="117"/>
@@ -7597,16 +7624,16 @@
         <v>[Admin_login-9]</v>
       </c>
       <c r="B19" s="117" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C19" s="117" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D19" s="117" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E19" s="173" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F19" s="117"/>
       <c r="G19" s="117"/>
@@ -7619,16 +7646,16 @@
         <v>[Admin_login-10]</v>
       </c>
       <c r="B20" s="117" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C20" s="117" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D20" s="117" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E20" s="173" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F20" s="117"/>
       <c r="G20" s="117"/>
@@ -7639,7 +7666,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="176"/>
       <c r="B21" s="177" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C21" s="176"/>
       <c r="D21" s="176"/>
@@ -7656,16 +7683,16 @@
         <v>[Admin_login-12]</v>
       </c>
       <c r="B22" s="117" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C22" s="117" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E22" s="179" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F22" s="117"/>
       <c r="G22" s="117"/>
@@ -7679,16 +7706,16 @@
         <v>[Admin_login-13]</v>
       </c>
       <c r="B23" s="117" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E23" s="179" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F23" s="117"/>
       <c r="G23" s="117"/>
@@ -7699,7 +7726,7 @@
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
       <c r="A24" s="176"/>
       <c r="B24" s="177" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C24" s="176"/>
       <c r="D24" s="176"/>
@@ -7716,16 +7743,16 @@
         <v>[Admin_login-15]</v>
       </c>
       <c r="B25" s="117" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C25" s="117" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D25" s="180" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E25" s="179" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F25" s="117"/>
       <c r="G25" s="117"/>
@@ -7736,7 +7763,7 @@
     <row r="26" spans="1:10" ht="14.25" customHeight="1">
       <c r="A26" s="176"/>
       <c r="B26" s="177" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C26" s="176"/>
       <c r="D26" s="176"/>
@@ -7753,13 +7780,13 @@
         <v>[Admin_login-17]</v>
       </c>
       <c r="B27" s="117" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C27" s="117" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D27" s="180" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E27" s="179"/>
       <c r="F27" s="117"/>
@@ -7771,7 +7798,7 @@
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
       <c r="A28" s="176"/>
       <c r="B28" s="177" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>

</xml_diff>

<commit_message>
update final version: integration test case
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
+++ b/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" activeTab="2"/>
+    <workbookView xWindow="620" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="382">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -743,93 +743,8 @@
     <t>MS31</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Homepage is displayed
-2. Login panel is displayed
-3. Display message: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>MS02</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Homepage is displayed
-2. Login page is displayed
-3. 
-- "username@gmail.com" is displayed in user name text box
-- "••••••" is displayed in password text box
-3. Display message: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>MS06</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Homepage is displayed
-2. Login page is displayed
-3. Display message: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>MS12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t>1.The Homepage is displayed 
 2. Register page is displayed with "Register" form</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. Register page is displayed with "Register" form
-4. New account registered sucessfully</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-3. Login page is displayed
-4. Logged in successfully</t>
   </si>
   <si>
     <t>Check "Account" button</t>
@@ -961,10 +876,6 @@
   </si>
   <si>
     <t>Common</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Log out successfully
-2. Homepage is displayed </t>
   </si>
   <si>
     <t>Security</t>
@@ -1214,12 +1125,6 @@
 6. Click on Edit profile button</t>
   </si>
   <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Logged in successfully
-4. The Account page is displayed</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Log in Page is displayed
 </t>
   </si>
@@ -1234,61 +1139,7 @@
 - "Login" button</t>
   </si>
   <si>
-    <t>1. Enter the mod page</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Click on "Login" button</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Click "Username" field</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Click "Password" field</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Input data to "Password" field</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Input username "email0@gmail.com" password "123456", then click "Login" button</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Input username "email0@gmail.com" and password "fsdfs", then click "Login" button</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Input username and password, then click "Login" button</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Input wrong username "fsdfsd" and password "123456789", then click "Login" button</t>
-  </si>
-  <si>
     <t>Check mod view</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Click logout button in Right Slide bar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Mod Page is displayed with the following list:
-- Header
-- Right Side bar:
-+ Logout button
-- Content details left
-+ Dashboard (default)
-+ Medicinal plant management
-+ Remedy management 
-- Content details middle
-+ Total medicinal plant article
-+ Total remedy article
-+ Pending approved article
-</t>
   </si>
   <si>
     <t xml:space="preserve">1. Admin Page is displayed with the following list:
@@ -1307,33 +1158,11 @@
 </t>
   </si>
   <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Logged in successfully
-4. Click on avatar account dropdown list
-5. Click Edit profile button is displayed</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Login successfully
 2. Click on avatar at right side screen
 3. Click on Logout button </t>
   </si>
   <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Logged in successfully
-4. The Account page is displayed
-5. Message list displayed</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Logged in successfully
-4. The Account page is displayed
-5. Message list displayed
-6. Message detail displayed</t>
-  </si>
-  <si>
     <t>Integration Login with Posted Article</t>
   </si>
   <si>
@@ -1347,14 +1176,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Logged in successfully
-4. The Account page is displayed
-5. Posted Article list
-6. Show posted article is displayed</t>
   </si>
   <si>
     <t>Mod Common module</t>
@@ -1399,16 +1220,6 @@
   <si>
     <t>1.The login of mod page is displayed 
 2. Logged in successfully, The "Mod" page is displayed</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Input username "email0@gmail.com" password "123456", then click "Login" button
-3. Click Dashboard tap</t>
-  </si>
-  <si>
-    <t>1. Enter the mod page
-2. Input username "email0@gmail.com" password "123456", then click "Login" button
-3. Click Medicinal plant management tab</t>
   </si>
   <si>
     <t>1. The login of mod page is displayed 
@@ -1443,11 +1254,6 @@
     <t>Check "medicinal plant" management</t>
   </si>
   <si>
-    <t>1. Enter the mod page
-2. Input username "email0@gmail.com" password "123456", then click "Login" button
-3. Click remedy management tab</t>
-  </si>
-  <si>
     <t>1. The login of mod page is displayed 
 2. Logged in successfully, The "Mod" page is displayed
 3. Show remedy management content 
@@ -1463,9 +1269,6 @@
     <t>Integration Login with medicinal plants</t>
   </si>
   <si>
-    <t>Check "Medicinal plants" button in menu</t>
-  </si>
-  <si>
     <t>1.The Homepage is displayed 
 2. The log in page is displayed
 3. Logged in successfully
@@ -1484,19 +1287,10 @@
     <t>Integration Login with HMS</t>
   </si>
   <si>
-    <t>Check "HMS" button in menu</t>
-  </si>
-  <si>
     <t>1.The Homepage is displayed 
 2. The log in page is displayed
 3. Logged in successfully
 4. The "HMS" page is displayed</t>
-  </si>
-  <si>
-    <t>Integration Personal page with medicinal plants link</t>
-  </si>
-  <si>
-    <t>Check "Medicinal plants" link</t>
   </si>
   <si>
     <t>1. Enter the website: thuocnam.com
@@ -1565,106 +1359,11 @@
 4. Click "Sign up" button of register page</t>
   </si>
   <si>
-    <t>1.The Homepage is displayed 
-2. Login page is displayed
-3. Forgot password form is displayed
-4. Change password page is sent to email "thuocnam@fpt.edu.vn"</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. Login page is displayed
-3. Log in successfully</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button in header
-3. Input: 
-Email: "dangnhse02992@fpt.edu.vn"
-Password: Enter new password which has been changed in change password page
-4. Click "Sign in" button of login page</t>
-  </si>
-  <si>
-    <t>1. Enter the website
-2. Click on Login button in header
-3. Click on "Forgot password" link
-4. Input "dangnhse02992@fpt.edu.vn"
-5. Click "send" button</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on Avatar menu
-6. Click on Account button
-7. Show message list</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on Avatar menu
-6. Click on Account button
-7. Show message list
-8. Click a message of message list
-9. Show message detail modal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on Avatar menu
-6. Click on Account button
-7. Click on Image of posted article
-8. Show posted article </t>
-  </si>
-  <si>
     <t>1. Enter the website: thuocnam.com
 2. Click on Home button</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Homepage is displayed </t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Logged in successfully
-4. The "personal" page is displayed
-5. "Medicinal plants detail" page is displayed</t>
-  </si>
-  <si>
-    <t>Integration Personal page with remedy link</t>
-  </si>
-  <si>
-    <t>Check "remedy" link</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Logged in successfully
-4. The "personal" page is displayed
-5. "Remedy detail" page is displayed</t>
-  </si>
-  <si>
     <t>Integration Personal page with notification</t>
-  </si>
-  <si>
-    <t>Check "Notification" list</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Logged in successfully
-4. The "personal" page is displayed
-5. "Notification" list is displayed</t>
   </si>
   <si>
     <t>Integration Medicinal plants with remedy</t>
@@ -1703,9 +1402,6 @@
     <t>Check "log out"  when user login successfully</t>
   </si>
   <si>
-    <t xml:space="preserve">Check "relational remedy" link </t>
-  </si>
-  <si>
     <t>1.The Homepage is displayed 
 2. The log in page is displayed
 3. Logged in successfully
@@ -1721,12 +1417,6 @@
   </si>
   <si>
     <t>Integration Remedy with author</t>
-  </si>
-  <si>
-    <t>Check "Author" link</t>
-  </si>
-  <si>
-    <t>Check "HMS" link</t>
   </si>
   <si>
     <t>1. Enter the website: thuocnam.com
@@ -1737,14 +1427,6 @@
 4. Click on "sign in" button of login page or press enter
 5. Click on "Avatar" in menu bar
 6. Click "Notification" list in personal page</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Logged in successfully
-4. The "medicinal plants" page is displayed
-5. "Medicinal plants detail" page is displayed
-6. "Author" is displayed</t>
   </si>
   <si>
     <t>1. Enter the website: thuocnam.com
@@ -1766,15 +1448,220 @@
 4. Click on "sign in" button of login page or press enter
 5. Click on "Remedy" in menu bar
 6. Click on a "Remedy" picture of remedy page
-7. Click on "relational HMS" of remedy detail page</t>
+7. Click on "author" of remedy detail page</t>
+  </si>
+  <si>
+    <t>Vietnamese Medicinal Plants Network</t>
+  </si>
+  <si>
+    <t>List enviroment requires in this system
+1. Server: 
+2. Database server: MySQL server
+3. Browser: Google Chrome 40, Mozzila Firefox 30
+4. Operation System: Mac OS X</t>
+  </si>
+  <si>
+    <t>Medicinal Plant</t>
+  </si>
+  <si>
+    <t>Remedy</t>
+  </si>
+  <si>
+    <t>Herb Store Medicine</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click "Mecicinal plant" menu
+3. Copy link
+4. Change to other browser
+5. Paste link and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click "Remedy" menu
+3. Copy link
+4. Change to other browser
+5. Paste link and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click "HMS" menu
+3. Copy link
+4. Change to other browser
+5. Paste link and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click Message
+3. Copy link
+4. Change to other browser
+5. Paste link and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click Account
+3. Copy link
+4. Change to other browser
+5. Paste link and press Enter</t>
+  </si>
+  <si>
+    <t>User function</t>
+  </si>
+  <si>
+    <t>Integrating all functions of user together then execute test</t>
+  </si>
+  <si>
+    <t>User_Function</t>
+  </si>
+  <si>
+    <t>Mod_Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Mod Page is displayed with the following list:
+- Header
+- Right Side bar:
++ Logout button
+- Content details left
++ Dashboard (default)
++ Medicinal plant management
++ Remedy management 
+</t>
+  </si>
+  <si>
+    <t>Check "Medicinal plants" tab</t>
+  </si>
+  <si>
+    <t>Check "HMS" tab</t>
+  </si>
+  <si>
+    <t>Integration Personal page with related remedy</t>
+  </si>
+  <si>
+    <t>Integration Personal page with related medicinal plants</t>
+  </si>
+  <si>
+    <t>Check "Notification" tab</t>
+  </si>
+  <si>
+    <t>1. Enter the website: thuocnam.com
+2. Click on Login button
+3. Input:
++ Email: "dangnhse02992@fpt.edu.vn"
++ Password: "123456789"
+4. Click on "sign in" button of login page or press enter
+5. Click on Avatar menu
+6. Click on Account button
+7. Show message tab</t>
+  </si>
+  <si>
+    <t>Check "related remedy" tab</t>
+  </si>
+  <si>
+    <t>Check "remedy" tab</t>
+  </si>
+  <si>
+    <t>Check "Author" tab</t>
+  </si>
+  <si>
+    <t>1. Homepage is displayed 
+2. Reload homepage, homepage is displayed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Homepage is displayed
+2. Login panel is displayed
+3. Username and password textarea is displayed
+4. Display message: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>MS02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Homepage is displayed
+2. Login page is displayed
+3. 
+  "username@gmail.com" is displayed in user name text box
+- "••••••" is displayed in password text box
+4. Display message: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>MS06</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the website
+2. Click on Login button in header
+3. Click on "Forgot password" link
+4. Input "dangnh@fpt.edu.vn"
+5. Click "send" button</t>
   </si>
   <si>
     <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Logged in successfully
-4. The "remedy" page is displayed
-5. "Remedy detail" page is displayed
-6. "Author" is displayed</t>
+2. Login page is displayed
+3. Forgot password form is displayed
+4. Email textarea is displayed
+5. Change password page is sent to email "dangnh@fpt.edu.vn"</t>
+  </si>
+  <si>
+    <t>1. Enter the website: thuocnam.com
+2. Click on Login button in header
+3. Input: 
+Email: "dangnhse02992@fpt.edu.vn"
+Password: Enter new password (which has been changed in change password page)
+4. Click "Sign in" button of login page</t>
+  </si>
+  <si>
+    <t>1. Enter the website: thuocnam.com
+2. Click on Login button
+3. Input:
++ Email: "dangnhse02992@fpt.edu.vn"
++ Password: "123456789"
+4. Click on "sign in" button of login page or press enter
+5. Click on Avatar menu
+6. Click on Account button
+7. Click message tab
+8. Click a message of message tab</t>
+  </si>
+  <si>
+    <t>1. Enter the website: thuocnam.com
+2. Click on Login button
+3. Input:
++ Email: "dangnhse02992@fpt.edu.vn"
++ Password: "123456789"
+4. Click on "sign in" button of login page or press enter
+5. Click on Avatar menu
+6. Click on Account button
+7. Click on Image of posted article tab</t>
   </si>
   <si>
     <t>1. Enter the website: thuocnam.com
@@ -1785,81 +1672,211 @@
 4. Click on "sign in" button of login page or press enter
 5. Click on "Remedy" in menu bar
 6. Click on a "Remedy" picture of remedy page
-7. Click on "author" of remedy detail page</t>
+7. Click on "related HMS" of remedy detail page</t>
   </si>
   <si>
     <t>1.The Homepage is displayed 
 2. The log in page is displayed
-3. Logged in successfully
-4. The "remedy" page is displayed
-5. "Remedy detail" page is displayed
-6. "HMS" is displayed</t>
-  </si>
-  <si>
-    <t>Vietnamese Medicinal Plants Network</t>
-  </si>
-  <si>
-    <t>List enviroment requires in this system
-1. Server: 
-2. Database server: MySQL server
-3. Browser: Google Chrome 40, Mozzila Firefox 30
-4. Operation System: Mac OS X</t>
-  </si>
-  <si>
-    <t>Medicinal Plant</t>
-  </si>
-  <si>
-    <t>Remedy</t>
-  </si>
-  <si>
-    <t>Herb Store Medicine</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click "Mecicinal plant" menu
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click "Remedy" menu
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click "HMS" menu
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click Message
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click Account
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
-    <t>User function</t>
-  </si>
-  <si>
-    <t>Integrating all functions of user together then execute test</t>
-  </si>
-  <si>
-    <t>User_Function</t>
-  </si>
-  <si>
-    <t>Mod_Function</t>
+3. Email and password textarea are displayed
+4. Logged in successfully
+5. The "medicinal plants" page is displayed
+6. "Medicinal plants detail" page is displayed
+7. "Author" is displayed</t>
+  </si>
+  <si>
+    <t>1. The Homepage is displayed 
+2. The log in page is displayed
+3. Email and password textarea are displayed
+4. Logged in successfully
+5. The "remedy" page is displayed
+6. "Remedy detail" page is displayed
+7. "Related HMS" is displayed</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Email and password textarea are displayed
+4. Logged in successfully
+5. The "remedy" page is displayed
+6. "Remedy detail" page is displayed
+7. "Author" is displayed</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Email and password textarea are displayed
+4. Logged in successfully
+5. The "personal" page is displayed
+6. "Notification" list is displayed</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Email and password textarea are displayed
+4. Logged in successfully
+5. The "personal" page is displayed
+6. "Remedy detail" page is displayed</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Email and password textarea are displayed
+4. Logged in successfully
+5. The "personal" page is displayed
+6. "Medicinal plants detail" page is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Homepage and avatar is displayed 
+2. Log out successfully
+3. Homepage is displayed </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Homepage is displayed
+2. Login page is displayed
+3. Username and password is displayed
+4. Display message: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>MS12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>1. The Homepage is displayed 
+2. Login page is displayed
+3. Username and password textarea are displayed
+4. Logged in successfully</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. Register page is displayed with "Register" form
+3. Username, password, email, address, phone textarea are displayed
+4. New account registered sucessfully</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. Login page is displayed
+3. Email and password textarea ara displayed
+4. Log in successfully</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Email, password text area are displayed
+4. Logged in successfully
+5. Avatar logo is displayed
+6. The Edit page is displayed</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Email, password text area are displayed
+4. Logged in successfully
+5. Avatar logo is displayed
+6. The Account page is displayed</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Email, password text area are displayed
+4. Logged in successfully
+5. Avatar logo is displayed
+6. The Account page is displayed
+7. Message is displayed</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Email, password text area are displayed
+4. Logged in successfully
+5. Avatar logo is displayed
+6. The Account page is displayed
+7. Message is displayed
+8. Message detail is displayed</t>
+  </si>
+  <si>
+    <t>1.The Homepage is displayed 
+2. The log in page is displayed
+3. Email, password text area are displayed
+4. Logged in successfully
+5. Avatar logo is displayed
+6. The Account page is displayed
+7. Posted article is displayed</t>
+  </si>
+  <si>
+    <t>1. The Homepage is displayed
+2. Avatar menu is showed
+3. Logout user and redirect to homepage as guest rule</t>
+  </si>
+  <si>
+    <t>1. Enter mod page</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Click on "Login" button</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Click "Username" field</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Click "Password" field</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Input data to "Password" field</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Input username "email0@gmail.com" password "123456", then click "Login" button</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Input username "email0@gmail.com" and password "fsdfs", then click "Login" button</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Input username and password, then click "Login" button</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Input wrong username "fsdfsd" and password "123456789", then click "Login" button</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Click logout button in Right Slide bar</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Input username "email0@gmail.com" password "123456", then click "Login" button
+3. Click Dashboard tap</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Input username "email0@gmail.com" password "123456"
+3. Click "Login" button
+4. Click Medicinal plant management tab</t>
+  </si>
+  <si>
+    <t>1. Enter mod page
+2. Input username "email0@gmail.com" password "123456"
+3. Click "Login" button
+4. Click remedy management tab</t>
   </si>
 </sst>
 </file>
@@ -2751,7 +2768,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
@@ -2811,6 +2828,11 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3343,6 +3365,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3395,9 +3418,8 @@
     <xf numFmtId="0" fontId="27" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="64">
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -3449,6 +3471,11 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
@@ -3923,13 +3950,13 @@
     <row r="2" spans="1:7" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="199" t="s">
+      <c r="C2" s="200" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
+      <c r="G2" s="200"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="6"/>
@@ -3940,44 +3967,44 @@
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="200" t="s">
-        <v>369</v>
-      </c>
-      <c r="D4" s="200"/>
-      <c r="E4" s="200"/>
+      <c r="C4" s="201" t="s">
+        <v>319</v>
+      </c>
+      <c r="D4" s="201"/>
+      <c r="E4" s="201"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="200" t="s">
-        <v>255</v>
-      </c>
-      <c r="D5" s="200"/>
-      <c r="E5" s="200"/>
+      <c r="C5" s="201" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="201"/>
+      <c r="E5" s="201"/>
       <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="201" t="s">
+      <c r="B6" s="202" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="202" t="str">
+      <c r="C6" s="203" t="str">
         <f>C5&amp;"_"&amp;"Integration Test Case"&amp;"_"&amp;"v1.0"</f>
         <v>VMN_Integration Test Case_v1.0</v>
       </c>
-      <c r="D6" s="202"/>
-      <c r="E6" s="202"/>
+      <c r="D6" s="203"/>
+      <c r="E6" s="203"/>
       <c r="F6" s="9" t="s">
         <v>6</v>
       </c>
@@ -3986,10 +4013,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B7" s="201"/>
-      <c r="C7" s="202"/>
-      <c r="D7" s="202"/>
-      <c r="E7" s="202"/>
+      <c r="B7" s="202"/>
+      <c r="C7" s="203"/>
+      <c r="D7" s="203"/>
+      <c r="E7" s="203"/>
       <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
@@ -4049,7 +4076,7 @@
         <v>55</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="19" customFormat="1" ht="21.75" customHeight="1">
@@ -4156,39 +4183,39 @@
       <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="205" t="s">
+      <c r="B3" s="206" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="205"/>
-      <c r="D3" s="206" t="str">
+      <c r="C3" s="206"/>
+      <c r="D3" s="207" t="str">
         <f>Cover!C4</f>
         <v>Vietnamese Medicinal Plants Network</v>
       </c>
-      <c r="E3" s="206"/>
-      <c r="F3" s="206"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="205" t="s">
+      <c r="B4" s="206" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="205"/>
-      <c r="D4" s="206" t="str">
+      <c r="C4" s="206"/>
+      <c r="D4" s="207" t="str">
         <f>Cover!C5</f>
         <v>VMN</v>
       </c>
-      <c r="E4" s="206"/>
-      <c r="F4" s="206"/>
+      <c r="E4" s="207"/>
+      <c r="F4" s="207"/>
     </row>
     <row r="5" spans="2:6" s="35" customFormat="1" ht="72" customHeight="1">
-      <c r="B5" s="203" t="s">
+      <c r="B5" s="204" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="203"/>
-      <c r="D5" s="204" t="s">
-        <v>370</v>
-      </c>
-      <c r="E5" s="204"/>
-      <c r="F5" s="204"/>
+      <c r="C5" s="204"/>
+      <c r="D5" s="205" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="36"/>
@@ -4226,13 +4253,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
       <c r="D9" s="149" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="114" t="s">
-        <v>380</v>
+        <v>330</v>
       </c>
       <c r="F9" s="113" t="s">
         <v>90</v>
@@ -4356,7 +4383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -4371,15 +4398,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B1" s="209" t="s">
+      <c r="B1" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="209"/>
-      <c r="G1" s="209"/>
-      <c r="H1" s="209"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="210"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="62"/>
@@ -4395,17 +4422,17 @@
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="206" t="str">
+      <c r="C3" s="207" t="str">
         <f>Cover!C4</f>
         <v>Vietnamese Medicinal Plants Network</v>
       </c>
-      <c r="D3" s="206"/>
-      <c r="E3" s="207" t="s">
+      <c r="D3" s="207"/>
+      <c r="E3" s="208" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="207"/>
+      <c r="F3" s="208"/>
       <c r="G3" s="10" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="H3" s="65"/>
     </row>
@@ -4413,17 +4440,17 @@
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="206" t="str">
+      <c r="C4" s="207" t="str">
         <f>Cover!C5</f>
         <v>VMN</v>
       </c>
-      <c r="D4" s="206"/>
-      <c r="E4" s="207" t="s">
+      <c r="D4" s="207"/>
+      <c r="E4" s="208" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="207"/>
+      <c r="F4" s="208"/>
       <c r="G4" s="10" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="H4" s="65"/>
     </row>
@@ -4431,15 +4458,15 @@
       <c r="B5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="206" t="str">
+      <c r="C5" s="207" t="str">
         <f>C4&amp;"_"&amp;"Integration Test Report"&amp;"_"&amp;"v1.0"</f>
         <v>VMN_Integration Test Report_v1.0</v>
       </c>
-      <c r="D5" s="206"/>
-      <c r="E5" s="207" t="s">
+      <c r="D5" s="207"/>
+      <c r="E5" s="208" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="207"/>
+      <c r="F5" s="208"/>
       <c r="G5" s="115"/>
       <c r="H5" s="67"/>
     </row>
@@ -4448,12 +4475,12 @@
       <c r="B6" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="208"/>
-      <c r="D6" s="208"/>
-      <c r="E6" s="208"/>
-      <c r="F6" s="208"/>
-      <c r="G6" s="208"/>
-      <c r="H6" s="208"/>
+      <c r="C6" s="209"/>
+      <c r="D6" s="209"/>
+      <c r="E6" s="209"/>
+      <c r="F6" s="209"/>
+      <c r="G6" s="209"/>
+      <c r="H6" s="209"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
       <c r="A7" s="62"/>
@@ -4514,7 +4541,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="149" t="s">
-        <v>381</v>
+        <v>331</v>
       </c>
       <c r="D11" s="76">
         <f>User_Function!A6</f>
@@ -4542,8 +4569,8 @@
       <c r="B12" s="151">
         <v>2</v>
       </c>
-      <c r="C12" s="217" t="s">
-        <v>382</v>
+      <c r="C12" s="199" t="s">
+        <v>332</v>
       </c>
       <c r="D12" s="76">
         <f>Mod_Function!A6</f>
@@ -4719,11 +4746,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="211" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" thickBot="1"/>
     <row r="3" spans="1:3" ht="13">
@@ -5026,7 +5053,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -5061,14 +5090,14 @@
       <c r="A2" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="211" t="s">
+      <c r="B2" s="212" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="212"/>
+      <c r="F2" s="212"/>
+      <c r="G2" s="212"/>
       <c r="H2" s="147" t="s">
         <v>22</v>
       </c>
@@ -5081,14 +5110,14 @@
       <c r="A3" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="211" t="s">
+      <c r="B3" s="212" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="211"/>
-      <c r="D3" s="211"/>
-      <c r="E3" s="211"/>
-      <c r="F3" s="211"/>
-      <c r="G3" s="211"/>
+      <c r="C3" s="212"/>
+      <c r="D3" s="212"/>
+      <c r="E3" s="212"/>
+      <c r="F3" s="212"/>
+      <c r="G3" s="212"/>
       <c r="H3" s="147" t="s">
         <v>24</v>
       </c>
@@ -5101,14 +5130,14 @@
       <c r="A4" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="212" t="s">
-        <v>253</v>
-      </c>
-      <c r="C4" s="212"/>
-      <c r="D4" s="212"/>
-      <c r="E4" s="212"/>
-      <c r="F4" s="212"/>
-      <c r="G4" s="212"/>
+      <c r="B4" s="213" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="213"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
+      <c r="F4" s="213"/>
+      <c r="G4" s="213"/>
       <c r="H4" s="147" t="s">
         <v>27</v>
       </c>
@@ -5128,11 +5157,11 @@
       <c r="D5" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="213" t="s">
+      <c r="E5" s="214" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="213"/>
-      <c r="G5" s="213"/>
+      <c r="F5" s="214"/>
+      <c r="G5" s="214"/>
       <c r="H5" s="148" t="s">
         <v>26</v>
       </c>
@@ -5158,12 +5187,12 @@
         <f>COUNTIF(F11:G688,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="214">
+      <c r="E6" s="215">
         <f>COUNTA(A11:A245)*2</f>
         <v>122</v>
       </c>
-      <c r="F6" s="214"/>
-      <c r="G6" s="214"/>
+      <c r="F6" s="215"/>
+      <c r="G6" s="215"/>
       <c r="H6" s="99"/>
       <c r="I6" s="95"/>
       <c r="J6" s="95" t="s">
@@ -5259,7 +5288,7 @@
         <v>57</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D12" s="117" t="s">
         <v>94</v>
@@ -5280,7 +5309,7 @@
         <v>58</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D13" s="117" t="s">
         <v>95</v>
@@ -5301,10 +5330,10 @@
         <v>59</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
       <c r="D14" s="121" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E14" s="122"/>
       <c r="F14" s="117"/>
@@ -5322,7 +5351,7 @@
         <v>60</v>
       </c>
       <c r="C15" s="124" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D15" s="124" t="s">
         <v>96</v>
@@ -5343,10 +5372,10 @@
         <v>61</v>
       </c>
       <c r="C16" s="124" t="s">
-        <v>331</v>
+        <v>302</v>
       </c>
       <c r="D16" s="124" t="s">
-        <v>158</v>
+        <v>344</v>
       </c>
       <c r="E16" s="125"/>
       <c r="F16" s="117"/>
@@ -5364,10 +5393,10 @@
         <v>62</v>
       </c>
       <c r="C17" s="124" t="s">
-        <v>329</v>
+        <v>300</v>
       </c>
       <c r="D17" s="124" t="s">
-        <v>159</v>
+        <v>345</v>
       </c>
       <c r="E17" s="125"/>
       <c r="F17" s="117"/>
@@ -5385,10 +5414,10 @@
         <v>63</v>
       </c>
       <c r="C18" s="124" t="s">
-        <v>330</v>
+        <v>301</v>
       </c>
       <c r="D18" s="124" t="s">
-        <v>160</v>
+        <v>359</v>
       </c>
       <c r="E18" s="125"/>
       <c r="F18" s="117"/>
@@ -5420,10 +5449,10 @@
         <v>79</v>
       </c>
       <c r="C20" s="91" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D20" s="91" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E20" s="91" t="s">
         <v>80</v>
@@ -5437,7 +5466,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="58"/>
       <c r="B21" s="58" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
@@ -5457,10 +5486,10 @@
         <v>84</v>
       </c>
       <c r="C22" s="91" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D22" s="91" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E22" s="91" t="s">
         <v>81</v>
@@ -5480,10 +5509,10 @@
         <v>85</v>
       </c>
       <c r="C23" s="91" t="s">
-        <v>333</v>
+        <v>304</v>
       </c>
       <c r="D23" s="91" t="s">
-        <v>162</v>
+        <v>361</v>
       </c>
       <c r="E23" s="91"/>
       <c r="F23" s="117"/>
@@ -5501,10 +5530,10 @@
         <v>86</v>
       </c>
       <c r="C24" s="91" t="s">
-        <v>332</v>
+        <v>303</v>
       </c>
       <c r="D24" s="91" t="s">
-        <v>163</v>
+        <v>360</v>
       </c>
       <c r="E24" s="91" t="s">
         <v>81</v>
@@ -5535,13 +5564,13 @@
         <v>[User_login-16]</v>
       </c>
       <c r="B26" s="91" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C26" s="91" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="D26" s="136" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="E26" s="91" t="s">
         <v>83</v>
@@ -5561,10 +5590,10 @@
         <v>87</v>
       </c>
       <c r="C27" s="91" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="D27" s="91" t="s">
-        <v>335</v>
+        <v>362</v>
       </c>
       <c r="E27" s="91" t="s">
         <v>81</v>
@@ -5578,7 +5607,7 @@
     <row r="28" spans="1:10" ht="14.25" customHeight="1">
       <c r="A28" s="58"/>
       <c r="B28" s="58" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C28" s="59"/>
       <c r="D28" s="59"/>
@@ -5595,13 +5624,13 @@
         <v>[User_login-19]</v>
       </c>
       <c r="B29" s="91" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C29" s="106" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D29" s="104" t="s">
-        <v>266</v>
+        <v>364</v>
       </c>
       <c r="E29" s="104" t="s">
         <v>88</v>
@@ -5621,10 +5650,10 @@
         <v>89</v>
       </c>
       <c r="C30" s="106" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D30" s="104" t="s">
-        <v>283</v>
+        <v>363</v>
       </c>
       <c r="E30" s="104" t="s">
         <v>88</v>
@@ -5637,10 +5666,10 @@
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1">
       <c r="A31" s="58" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C31" s="59"/>
       <c r="D31" s="59"/>
@@ -5657,13 +5686,13 @@
         <v>[User_login-22]</v>
       </c>
       <c r="B32" s="91" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="C32" s="106" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D32" s="104" t="s">
-        <v>285</v>
+        <v>365</v>
       </c>
       <c r="E32" s="104"/>
       <c r="F32" s="117"/>
@@ -5678,13 +5707,13 @@
         <v>[User_login-23]</v>
       </c>
       <c r="B33" s="91" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="C33" s="106" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="D33" s="104" t="s">
-        <v>286</v>
+        <v>366</v>
       </c>
       <c r="E33" s="104"/>
       <c r="F33" s="117"/>
@@ -5695,10 +5724,10 @@
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
       <c r="A34" s="58" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B34" s="58" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="59"/>
@@ -5715,13 +5744,13 @@
         <v>[User_login-25]</v>
       </c>
       <c r="B35" s="91" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="C35" s="106" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="D35" s="104" t="s">
-        <v>292</v>
+        <v>367</v>
       </c>
       <c r="E35" s="104"/>
       <c r="F35" s="117"/>
@@ -5733,7 +5762,7 @@
     <row r="36" spans="1:10" ht="14.25" customHeight="1">
       <c r="A36" s="169"/>
       <c r="B36" s="169" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C36" s="166"/>
       <c r="D36" s="166"/>
@@ -5750,13 +5779,13 @@
         <v>[User_login-27]</v>
       </c>
       <c r="B37" s="117" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C37" s="117" t="s">
-        <v>341</v>
+        <v>305</v>
       </c>
       <c r="D37" s="117" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E37" s="118"/>
       <c r="F37" s="117"/>
@@ -5771,13 +5800,13 @@
         <v>[User_login-28]</v>
       </c>
       <c r="B38" s="117" t="s">
-        <v>354</v>
+        <v>311</v>
       </c>
       <c r="C38" s="117" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="D38" s="117" t="s">
-        <v>202</v>
+        <v>358</v>
       </c>
       <c r="E38" s="118"/>
       <c r="F38" s="117"/>
@@ -5788,10 +5817,10 @@
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1">
       <c r="A39" s="169" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B39" s="169" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
       <c r="C39" s="166"/>
       <c r="D39" s="166"/>
@@ -5808,13 +5837,13 @@
         <v>[User_login-30]</v>
       </c>
       <c r="B40" s="117" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
       <c r="C40" s="117" t="s">
-        <v>325</v>
+        <v>296</v>
       </c>
       <c r="D40" s="117" t="s">
-        <v>317</v>
+        <v>291</v>
       </c>
       <c r="E40" s="118"/>
       <c r="F40" s="117"/>
@@ -5825,10 +5854,10 @@
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1">
       <c r="A41" s="169" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B41" s="169" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="C41" s="166"/>
       <c r="D41" s="166"/>
@@ -5845,13 +5874,13 @@
         <v>[User_login-32]</v>
       </c>
       <c r="B42" s="117" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
       <c r="C42" s="117" t="s">
-        <v>326</v>
+        <v>297</v>
       </c>
       <c r="D42" s="117" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
       <c r="E42" s="118"/>
       <c r="F42" s="117"/>
@@ -5862,10 +5891,10 @@
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1">
       <c r="A43" s="169" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B43" s="169" t="s">
-        <v>320</v>
+        <v>294</v>
       </c>
       <c r="C43" s="166"/>
       <c r="D43" s="166"/>
@@ -5882,13 +5911,13 @@
         <v>[User_login-34]</v>
       </c>
       <c r="B44" s="117" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="C44" s="117" t="s">
-        <v>327</v>
+        <v>298</v>
       </c>
       <c r="D44" s="117" t="s">
-        <v>322</v>
+        <v>295</v>
       </c>
       <c r="E44" s="118"/>
       <c r="F44" s="117"/>
@@ -5899,10 +5928,10 @@
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1">
       <c r="A45" s="169" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B45" s="169" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="C45" s="166"/>
       <c r="D45" s="166"/>
@@ -5919,13 +5948,13 @@
         <v>[User_login-36]</v>
       </c>
       <c r="B46" s="117" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="C46" s="117" t="s">
-        <v>351</v>
+        <v>308</v>
       </c>
       <c r="D46" s="117" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="E46" s="118"/>
       <c r="F46" s="117"/>
@@ -5936,10 +5965,10 @@
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1">
       <c r="A47" s="169" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B47" s="169" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C47" s="166"/>
       <c r="D47" s="166"/>
@@ -5956,13 +5985,13 @@
         <v>[User_login-38]</v>
       </c>
       <c r="B48" s="117" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C48" s="117" t="s">
-        <v>352</v>
+        <v>309</v>
       </c>
       <c r="D48" s="117" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="E48" s="118"/>
       <c r="F48" s="117"/>
@@ -5973,10 +6002,10 @@
     </row>
     <row r="49" spans="1:10" ht="14.25" customHeight="1">
       <c r="A49" s="169" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B49" s="169" t="s">
-        <v>347</v>
+        <v>306</v>
       </c>
       <c r="C49" s="166"/>
       <c r="D49" s="166"/>
@@ -5993,13 +6022,13 @@
         <v>[User_login-40]</v>
       </c>
       <c r="B50" s="117" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="C50" s="117" t="s">
-        <v>362</v>
+        <v>316</v>
       </c>
       <c r="D50" s="117" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="E50" s="118"/>
       <c r="F50" s="117"/>
@@ -6010,10 +6039,10 @@
     </row>
     <row r="51" spans="1:10" ht="14.25" customHeight="1">
       <c r="A51" s="169" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B51" s="169" t="s">
-        <v>350</v>
+        <v>307</v>
       </c>
       <c r="C51" s="166"/>
       <c r="D51" s="166"/>
@@ -6030,13 +6059,13 @@
         <v>[User_login-42]</v>
       </c>
       <c r="B52" s="117" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="C52" s="117" t="s">
-        <v>353</v>
+        <v>310</v>
       </c>
       <c r="D52" s="117" t="s">
-        <v>356</v>
+        <v>312</v>
       </c>
       <c r="E52" s="118"/>
       <c r="F52" s="117"/>
@@ -6047,10 +6076,10 @@
     </row>
     <row r="53" spans="1:10" ht="14.25" customHeight="1">
       <c r="A53" s="169" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B53" s="169" t="s">
-        <v>357</v>
+        <v>313</v>
       </c>
       <c r="C53" s="166"/>
       <c r="D53" s="166"/>
@@ -6067,13 +6096,13 @@
         <v>[User_login-44]</v>
       </c>
       <c r="B54" s="117" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="C54" s="117" t="s">
-        <v>364</v>
+        <v>317</v>
       </c>
       <c r="D54" s="117" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="E54" s="118"/>
       <c r="F54" s="117"/>
@@ -6083,10 +6112,10 @@
     </row>
     <row r="55" spans="1:10" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A55" s="169" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B55" s="169" t="s">
-        <v>358</v>
+        <v>314</v>
       </c>
       <c r="C55" s="166"/>
       <c r="D55" s="166"/>
@@ -6102,13 +6131,13 @@
         <v>[User_login-46]</v>
       </c>
       <c r="B56" s="117" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
       <c r="C56" s="117" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="D56" s="117" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="E56" s="118"/>
       <c r="F56" s="117"/>
@@ -6118,10 +6147,10 @@
     </row>
     <row r="57" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A57" s="169" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B57" s="169" t="s">
-        <v>359</v>
+        <v>315</v>
       </c>
       <c r="C57" s="166"/>
       <c r="D57" s="166"/>
@@ -6137,13 +6166,13 @@
         <v>[User_login-48]</v>
       </c>
       <c r="B58" s="117" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="C58" s="117" t="s">
-        <v>367</v>
+        <v>318</v>
       </c>
       <c r="D58" s="117" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="E58" s="118"/>
       <c r="F58" s="117"/>
@@ -6176,7 +6205,7 @@
     <row r="61" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A61" s="169"/>
       <c r="B61" s="169" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C61" s="169"/>
       <c r="D61" s="169"/>
@@ -6189,7 +6218,7 @@
     <row r="62" spans="1:10" s="169" customFormat="1" ht="14.25" customHeight="1">
       <c r="A62" s="185"/>
       <c r="B62" s="186" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C62" s="187"/>
       <c r="D62" s="187"/>
@@ -6205,20 +6234,20 @@
         <v>ID-44</v>
       </c>
       <c r="B63" s="117" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C63" s="117" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D63" s="117" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E63" s="117"/>
       <c r="F63" s="117"/>
       <c r="G63" s="117"/>
       <c r="H63" s="117"/>
       <c r="I63" s="188" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="190" customFormat="1" ht="14.25" customHeight="1">
@@ -6227,20 +6256,20 @@
         <v>ID-45</v>
       </c>
       <c r="B64" s="117" t="s">
-        <v>371</v>
+        <v>321</v>
       </c>
       <c r="C64" s="117" t="s">
-        <v>374</v>
+        <v>324</v>
       </c>
       <c r="D64" s="117" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E64" s="117"/>
       <c r="F64" s="117"/>
       <c r="G64" s="117"/>
       <c r="H64" s="117"/>
       <c r="I64" s="188" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="190" customFormat="1" ht="14.25" customHeight="1">
@@ -6249,20 +6278,20 @@
         <v>ID-46</v>
       </c>
       <c r="B65" s="117" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="C65" s="117" t="s">
-        <v>375</v>
+        <v>325</v>
       </c>
       <c r="D65" s="117" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E65" s="117"/>
       <c r="F65" s="117"/>
       <c r="G65" s="117"/>
       <c r="H65" s="117"/>
       <c r="I65" s="188" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="189" customFormat="1" ht="14.25" customHeight="1">
@@ -6271,20 +6300,20 @@
         <v>ID-47</v>
       </c>
       <c r="B66" s="117" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="C66" s="117" t="s">
-        <v>376</v>
+        <v>326</v>
       </c>
       <c r="D66" s="117" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E66" s="117"/>
       <c r="F66" s="117"/>
       <c r="G66" s="117"/>
       <c r="H66" s="117"/>
       <c r="I66" s="188" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6293,20 +6322,20 @@
         <v>ID-48</v>
       </c>
       <c r="B67" s="117" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C67" s="117" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
       <c r="D67" s="117" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E67" s="117"/>
       <c r="F67" s="117"/>
       <c r="G67" s="117"/>
       <c r="H67" s="117"/>
       <c r="I67" s="188" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6315,26 +6344,26 @@
         <v>ID-49</v>
       </c>
       <c r="B68" s="117" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C68" s="117" t="s">
-        <v>378</v>
+        <v>328</v>
       </c>
       <c r="D68" s="117" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E68" s="117"/>
       <c r="F68" s="117"/>
       <c r="G68" s="117"/>
       <c r="H68" s="117"/>
       <c r="I68" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A69" s="169"/>
       <c r="B69" s="169" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C69" s="169"/>
       <c r="D69" s="169"/>
@@ -6350,20 +6379,20 @@
         <v>ID-50</v>
       </c>
       <c r="B70" s="117" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C70" s="117" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D70" s="117" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E70" s="117"/>
       <c r="F70" s="117"/>
       <c r="G70" s="117"/>
       <c r="H70" s="117"/>
       <c r="I70" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6372,20 +6401,20 @@
         <v>ID-51</v>
       </c>
       <c r="B71" s="117" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C71" s="117" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D71" s="117" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E71" s="117"/>
       <c r="F71" s="117"/>
       <c r="G71" s="117"/>
       <c r="H71" s="117"/>
       <c r="I71" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6394,20 +6423,20 @@
         <v>ID-52</v>
       </c>
       <c r="B72" s="117" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C72" s="117" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D72" s="117" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E72" s="117"/>
       <c r="F72" s="117"/>
       <c r="G72" s="117"/>
       <c r="H72" s="117"/>
       <c r="I72" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6416,20 +6445,20 @@
         <v>ID-53</v>
       </c>
       <c r="B73" s="117" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C73" s="117" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D73" s="117" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E73" s="117"/>
       <c r="F73" s="117"/>
       <c r="G73" s="117"/>
       <c r="H73" s="117"/>
       <c r="I73" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6438,20 +6467,20 @@
         <v>ID-54</v>
       </c>
       <c r="B74" s="117" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C74" s="117" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D74" s="117" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E74" s="117"/>
       <c r="F74" s="117"/>
       <c r="G74" s="117"/>
       <c r="H74" s="117"/>
       <c r="I74" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6460,20 +6489,20 @@
         <v>ID-55</v>
       </c>
       <c r="B75" s="117" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C75" s="117" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D75" s="117" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E75" s="117"/>
       <c r="F75" s="117"/>
       <c r="G75" s="117"/>
       <c r="H75" s="117"/>
       <c r="I75" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="13.5" customHeight="1">
@@ -6482,20 +6511,20 @@
         <v>ID-56</v>
       </c>
       <c r="B76" s="117" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C76" s="117" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D76" s="117" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E76" s="117"/>
       <c r="F76" s="117"/>
       <c r="G76" s="117"/>
       <c r="H76" s="117"/>
       <c r="I76" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="13.5" customHeight="1">
@@ -6504,20 +6533,20 @@
         <v>ID-57</v>
       </c>
       <c r="B77" s="117" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C77" s="117" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D77" s="117" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E77" s="117"/>
       <c r="F77" s="117"/>
       <c r="G77" s="117"/>
       <c r="H77" s="117"/>
       <c r="I77" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="13.5" customHeight="1">
@@ -6526,20 +6555,20 @@
         <v>ID-58</v>
       </c>
       <c r="B78" s="117" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C78" s="117" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D78" s="117" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E78" s="117"/>
       <c r="F78" s="117"/>
       <c r="G78" s="117"/>
       <c r="H78" s="117"/>
       <c r="I78" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="13.5" customHeight="1">
@@ -6548,20 +6577,20 @@
         <v>ID-59</v>
       </c>
       <c r="B79" s="117" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C79" s="117" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D79" s="117" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E79" s="117"/>
       <c r="F79" s="117"/>
       <c r="G79" s="117"/>
       <c r="H79" s="117"/>
       <c r="I79" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13.5" customHeight="1">
@@ -6570,20 +6599,20 @@
         <v>ID-60</v>
       </c>
       <c r="B80" s="117" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C80" s="117" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D80" s="117" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E80" s="117"/>
       <c r="F80" s="117"/>
       <c r="G80" s="117"/>
       <c r="H80" s="117"/>
       <c r="I80" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="13.5" customHeight="1">
@@ -6592,20 +6621,20 @@
         <v>ID-61</v>
       </c>
       <c r="B81" s="117" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C81" s="117" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D81" s="117" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="E81" s="117"/>
       <c r="F81" s="117"/>
       <c r="G81" s="117"/>
       <c r="H81" s="117"/>
       <c r="I81" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="13.5" customHeight="1">
@@ -6614,20 +6643,20 @@
         <v>ID-62</v>
       </c>
       <c r="B82" s="117" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C82" s="117" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D82" s="117" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E82" s="117"/>
       <c r="F82" s="117"/>
       <c r="G82" s="117"/>
       <c r="H82" s="117"/>
       <c r="I82" s="117" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -6676,7 +6705,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -6698,7 +6729,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="137" customFormat="1" ht="18" thickBot="1">
       <c r="A1" s="138" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B1" s="139"/>
       <c r="C1" s="139"/>
@@ -6711,46 +6742,46 @@
       <c r="A2" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="211" t="s">
-        <v>268</v>
-      </c>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
+      <c r="B2" s="212" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="212"/>
+      <c r="F2" s="212"/>
+      <c r="G2" s="212"/>
       <c r="J2" s="95" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="137" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="142" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="211" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" s="211"/>
-      <c r="D3" s="211"/>
-      <c r="E3" s="211"/>
-      <c r="F3" s="211"/>
-      <c r="G3" s="211"/>
+        <v>179</v>
+      </c>
+      <c r="B3" s="212" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="212"/>
+      <c r="D3" s="212"/>
+      <c r="E3" s="212"/>
+      <c r="F3" s="212"/>
+      <c r="G3" s="212"/>
       <c r="J3" s="95" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="137" customFormat="1" ht="17">
       <c r="A4" s="141" t="s">
-        <v>186</v>
-      </c>
-      <c r="B4" s="212" t="s">
-        <v>253</v>
-      </c>
-      <c r="C4" s="212"/>
-      <c r="D4" s="212"/>
-      <c r="E4" s="212"/>
-      <c r="F4" s="212"/>
-      <c r="G4" s="212"/>
+        <v>181</v>
+      </c>
+      <c r="B4" s="213" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="213"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
+      <c r="F4" s="213"/>
+      <c r="G4" s="213"/>
       <c r="J4" s="96"/>
     </row>
     <row r="5" spans="1:10" s="137" customFormat="1" ht="17">
@@ -6761,16 +6792,16 @@
         <v>24</v>
       </c>
       <c r="C5" s="144" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D5" s="145" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="215" t="s">
-        <v>188</v>
-      </c>
-      <c r="F5" s="215"/>
-      <c r="G5" s="215"/>
+      <c r="E5" s="216" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="216"/>
+      <c r="G5" s="216"/>
       <c r="J5" s="95" t="s">
         <v>29</v>
       </c>
@@ -6792,12 +6823,12 @@
         <f>COUNTIF(F11:G705,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="214">
+      <c r="E6" s="215">
         <f>COUNTA(A11:A263)*2</f>
         <v>38</v>
       </c>
-      <c r="F6" s="214"/>
-      <c r="G6" s="214"/>
+      <c r="F6" s="215"/>
+      <c r="G6" s="215"/>
       <c r="J6" s="95" t="s">
         <v>27</v>
       </c>
@@ -6828,16 +6859,16 @@
         <v>30</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F10" s="57" t="s">
         <v>92</v>
@@ -6846,7 +6877,7 @@
         <v>93</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I10" s="56" t="s">
         <v>36</v>
@@ -6855,7 +6886,7 @@
     <row r="11" spans="1:10" s="137" customFormat="1" ht="14.25" customHeight="1">
       <c r="A11" s="133"/>
       <c r="B11" s="58" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C11" s="58"/>
       <c r="D11" s="58"/>
@@ -6871,13 +6902,13 @@
         <v>[Mod_login-2]</v>
       </c>
       <c r="B12" s="117" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>270</v>
+        <v>369</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>296</v>
+        <v>274</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="117"/>
@@ -6894,10 +6925,10 @@
         <v>64</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>271</v>
+        <v>370</v>
       </c>
       <c r="D13" s="117" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="E13" s="197"/>
       <c r="F13" s="117"/>
@@ -6911,13 +6942,13 @@
         <v>[Mod_login-4]</v>
       </c>
       <c r="B14" s="117" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>272</v>
+        <v>371</v>
       </c>
       <c r="D14" s="117" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="E14" s="173"/>
       <c r="F14" s="117"/>
@@ -6931,13 +6962,13 @@
         <v>[Mod_login-5]</v>
       </c>
       <c r="B15" s="117" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C15" s="117" t="s">
-        <v>273</v>
+        <v>372</v>
       </c>
       <c r="D15" s="117" t="s">
-        <v>299</v>
+        <v>277</v>
       </c>
       <c r="E15" s="173"/>
       <c r="F15" s="117"/>
@@ -6954,10 +6985,10 @@
         <v>74</v>
       </c>
       <c r="C16" s="117" t="s">
-        <v>274</v>
+        <v>373</v>
       </c>
       <c r="D16" s="117" t="s">
-        <v>300</v>
+        <v>278</v>
       </c>
       <c r="E16" s="173"/>
       <c r="F16" s="117"/>
@@ -6974,10 +7005,10 @@
         <v>66</v>
       </c>
       <c r="C17" s="117" t="s">
-        <v>275</v>
+        <v>374</v>
       </c>
       <c r="D17" s="117" t="s">
-        <v>302</v>
+        <v>280</v>
       </c>
       <c r="E17" s="173"/>
       <c r="F17" s="117"/>
@@ -6994,10 +7025,10 @@
         <v>68</v>
       </c>
       <c r="C18" s="117" t="s">
-        <v>276</v>
+        <v>375</v>
       </c>
       <c r="D18" s="117" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="E18" s="173"/>
       <c r="F18" s="117"/>
@@ -7014,10 +7045,10 @@
         <v>70</v>
       </c>
       <c r="C19" s="117" t="s">
-        <v>277</v>
+        <v>376</v>
       </c>
       <c r="D19" s="117" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="E19" s="173"/>
       <c r="F19" s="117"/>
@@ -7034,10 +7065,10 @@
         <v>72</v>
       </c>
       <c r="C20" s="117" t="s">
-        <v>278</v>
+        <v>377</v>
       </c>
       <c r="D20" s="117" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="E20" s="173"/>
       <c r="F20" s="117"/>
@@ -7049,7 +7080,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="176"/>
       <c r="B21" s="177" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="C21" s="176"/>
       <c r="D21" s="176"/>
@@ -7066,13 +7097,13 @@
         <v>[Mod_login-12]</v>
       </c>
       <c r="B22" s="117" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="C22" s="117" t="s">
-        <v>270</v>
+        <v>369</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>281</v>
+        <v>333</v>
       </c>
       <c r="E22" s="179"/>
       <c r="F22" s="117"/>
@@ -7087,13 +7118,13 @@
         <v>[Mod_login-13]</v>
       </c>
       <c r="B23" s="117" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>280</v>
+        <v>378</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E23" s="179"/>
       <c r="F23" s="117"/>
@@ -7104,7 +7135,7 @@
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
       <c r="A24" s="176" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B24" s="58" t="s">
         <v>78</v>
@@ -7127,10 +7158,10 @@
         <v>79</v>
       </c>
       <c r="C25" s="91" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="D25" s="91" t="s">
-        <v>261</v>
+        <v>368</v>
       </c>
       <c r="E25" s="179"/>
       <c r="F25" s="117"/>
@@ -7140,10 +7171,10 @@
     </row>
     <row r="26" spans="1:10" ht="13.5" customHeight="1">
       <c r="A26" s="176" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="C26" s="176"/>
       <c r="D26" s="176"/>
@@ -7159,13 +7190,13 @@
         <v>[Mod_login-17]</v>
       </c>
       <c r="B27" s="117" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="C27" s="117" t="s">
-        <v>303</v>
+        <v>379</v>
       </c>
       <c r="D27" s="117" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="E27" s="173"/>
       <c r="F27" s="117"/>
@@ -7175,10 +7206,10 @@
     </row>
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
       <c r="A28" s="176" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>
@@ -7194,13 +7225,13 @@
         <v>[Mod_login-19]</v>
       </c>
       <c r="B29" s="117" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="C29" s="117" t="s">
-        <v>304</v>
+        <v>380</v>
       </c>
       <c r="D29" s="117" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="E29" s="173"/>
       <c r="F29" s="117"/>
@@ -7210,10 +7241,10 @@
     </row>
     <row r="30" spans="1:10" ht="13.5" customHeight="1">
       <c r="A30" s="176" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B30" s="58" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="C30" s="176"/>
       <c r="D30" s="176"/>
@@ -7229,13 +7260,13 @@
         <v>[Mod_login-21]</v>
       </c>
       <c r="B31" s="117" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="C31" s="117" t="s">
-        <v>312</v>
+        <v>381</v>
       </c>
       <c r="D31" s="117" t="s">
-        <v>313</v>
+        <v>288</v>
       </c>
       <c r="E31" s="173"/>
       <c r="F31" s="117"/>
@@ -7277,7 +7308,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView topLeftCell="B6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -7299,7 +7332,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="137" customFormat="1" ht="18" thickBot="1">
       <c r="A1" s="138" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B1" s="139"/>
       <c r="C1" s="139"/>
@@ -7312,46 +7345,46 @@
       <c r="A2" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="211" t="s">
+      <c r="B2" s="212" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="212"/>
+      <c r="F2" s="212"/>
+      <c r="G2" s="212"/>
       <c r="J2" s="95" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="137" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="142" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="211" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" s="211"/>
-      <c r="D3" s="211"/>
-      <c r="E3" s="211"/>
-      <c r="F3" s="211"/>
-      <c r="G3" s="211"/>
+        <v>179</v>
+      </c>
+      <c r="B3" s="212" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="212"/>
+      <c r="D3" s="212"/>
+      <c r="E3" s="212"/>
+      <c r="F3" s="212"/>
+      <c r="G3" s="212"/>
       <c r="J3" s="95" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="137" customFormat="1" ht="17">
       <c r="A4" s="141" t="s">
-        <v>186</v>
-      </c>
-      <c r="B4" s="212" t="s">
-        <v>253</v>
-      </c>
-      <c r="C4" s="212"/>
-      <c r="D4" s="212"/>
-      <c r="E4" s="212"/>
-      <c r="F4" s="212"/>
-      <c r="G4" s="212"/>
+        <v>181</v>
+      </c>
+      <c r="B4" s="213" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="213"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
+      <c r="F4" s="213"/>
+      <c r="G4" s="213"/>
       <c r="J4" s="96"/>
     </row>
     <row r="5" spans="1:10" s="137" customFormat="1" ht="17">
@@ -7362,16 +7395,16 @@
         <v>24</v>
       </c>
       <c r="C5" s="144" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D5" s="145" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="215" t="s">
-        <v>188</v>
-      </c>
-      <c r="F5" s="215"/>
-      <c r="G5" s="215"/>
+      <c r="E5" s="216" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="216"/>
+      <c r="G5" s="216"/>
       <c r="J5" s="95" t="s">
         <v>29</v>
       </c>
@@ -7393,12 +7426,12 @@
         <f>COUNTIF(F11:G708,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="214">
+      <c r="E6" s="215">
         <f>COUNTA(A11:A265)*2</f>
         <v>26</v>
       </c>
-      <c r="F6" s="214"/>
-      <c r="G6" s="214"/>
+      <c r="F6" s="215"/>
+      <c r="G6" s="215"/>
       <c r="J6" s="95" t="s">
         <v>27</v>
       </c>
@@ -7429,16 +7462,16 @@
         <v>30</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F10" s="57" t="s">
         <v>92</v>
@@ -7447,7 +7480,7 @@
         <v>93</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I10" s="56" t="s">
         <v>36</v>
@@ -7455,16 +7488,16 @@
     </row>
     <row r="11" spans="1:10" s="137" customFormat="1" ht="14.25" customHeight="1">
       <c r="A11" s="170"/>
-      <c r="B11" s="216" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="216"/>
-      <c r="D11" s="216"/>
-      <c r="E11" s="216"/>
-      <c r="F11" s="216"/>
-      <c r="G11" s="216"/>
-      <c r="H11" s="216"/>
-      <c r="I11" s="216"/>
+      <c r="B11" s="217" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="217"/>
+      <c r="D11" s="217"/>
+      <c r="E11" s="217"/>
+      <c r="F11" s="217"/>
+      <c r="G11" s="217"/>
+      <c r="H11" s="217"/>
+      <c r="I11" s="217"/>
     </row>
     <row r="12" spans="1:10" s="111" customFormat="1" ht="14.25" customHeight="1">
       <c r="A12" s="165" t="str">
@@ -7472,13 +7505,13 @@
         <v>[Admin_login-2]</v>
       </c>
       <c r="B12" s="117" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="117"/>
@@ -7498,10 +7531,10 @@
         <v>65</v>
       </c>
       <c r="D13" s="117" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E13" s="173" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F13" s="117"/>
       <c r="G13" s="117"/>
@@ -7514,16 +7547,16 @@
         <v>[Admin_login-4]</v>
       </c>
       <c r="B14" s="117" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D14" s="117" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E14" s="173" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F14" s="117"/>
       <c r="G14" s="117"/>
@@ -7536,16 +7569,16 @@
         <v>[Admin_login-5]</v>
       </c>
       <c r="B15" s="117" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C15" s="117" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D15" s="117" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E15" s="173" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F15" s="117"/>
       <c r="G15" s="117"/>
@@ -7567,7 +7600,7 @@
         <v>76</v>
       </c>
       <c r="E16" s="173" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F16" s="117"/>
       <c r="G16" s="117"/>
@@ -7583,13 +7616,13 @@
         <v>66</v>
       </c>
       <c r="C17" s="117" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D17" s="117" t="s">
         <v>67</v>
       </c>
       <c r="E17" s="173" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F17" s="117"/>
       <c r="G17" s="117"/>
@@ -7605,13 +7638,13 @@
         <v>68</v>
       </c>
       <c r="C18" s="117" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D18" s="117" t="s">
         <v>69</v>
       </c>
       <c r="E18" s="173" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F18" s="117"/>
       <c r="G18" s="117"/>
@@ -7633,7 +7666,7 @@
         <v>69</v>
       </c>
       <c r="E19" s="173" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F19" s="117"/>
       <c r="G19" s="117"/>
@@ -7655,7 +7688,7 @@
         <v>69</v>
       </c>
       <c r="E20" s="173" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F20" s="117"/>
       <c r="G20" s="117"/>
@@ -7666,7 +7699,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="176"/>
       <c r="B21" s="177" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C21" s="176"/>
       <c r="D21" s="176"/>
@@ -7683,16 +7716,16 @@
         <v>[Admin_login-12]</v>
       </c>
       <c r="B22" s="117" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C22" s="117" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="E22" s="179" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F22" s="117"/>
       <c r="G22" s="117"/>
@@ -7706,16 +7739,16 @@
         <v>[Admin_login-13]</v>
       </c>
       <c r="B23" s="117" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E23" s="179" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F23" s="117"/>
       <c r="G23" s="117"/>
@@ -7726,7 +7759,7 @@
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
       <c r="A24" s="176"/>
       <c r="B24" s="177" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C24" s="176"/>
       <c r="D24" s="176"/>
@@ -7743,16 +7776,16 @@
         <v>[Admin_login-15]</v>
       </c>
       <c r="B25" s="117" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C25" s="117" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D25" s="180" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E25" s="179" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F25" s="117"/>
       <c r="G25" s="117"/>
@@ -7763,7 +7796,7 @@
     <row r="26" spans="1:10" ht="14.25" customHeight="1">
       <c r="A26" s="176"/>
       <c r="B26" s="177" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C26" s="176"/>
       <c r="D26" s="176"/>
@@ -7780,13 +7813,13 @@
         <v>[Admin_login-17]</v>
       </c>
       <c r="B27" s="117" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C27" s="117" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D27" s="180" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E27" s="179"/>
       <c r="F27" s="117"/>
@@ -7798,7 +7831,7 @@
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
       <c r="A28" s="176"/>
       <c r="B28" s="177" t="s">
-        <v>314</v>
+        <v>289</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>

</xml_diff>

<commit_message>
update integration testcase final version
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
+++ b/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" activeTab="5"/>
+    <workbookView xWindow="660" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="383">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -801,18 +801,9 @@
     <t>Admin Common module</t>
   </si>
   <si>
-    <t>1. Enter the admin page
-2. Click logout button in Right Slide bar</t>
-  </si>
-  <si>
     <t>Admin Dashboard module</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Enter the admin page
-2. Click Dashboard button in Right Slide bar
-</t>
-  </si>
-  <si>
     <t>User Management module</t>
   </si>
   <si>
@@ -853,16 +844,10 @@
   </si>
   <si>
     <t>Check Logout button</t>
-  </si>
-  <si>
-    <t>Check Admin when admin click Dashboard button in sidebar</t>
   </si>
   <si>
     <t>1. Admin Page is displayed
 2. Content about dashboard is displayed</t>
-  </si>
-  <si>
-    <t>Check  User button in sidebar</t>
   </si>
   <si>
     <t>1. Admin Page is displayed
@@ -1140,22 +1125,6 @@
   </si>
   <si>
     <t>Check mod view</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Admin Page is displayed with the following list:
-- Header
-- Right Side bar:
-+ Logout button
-- Content details left
-+ Dashboard (default)
-+ User management
-+ New herb medicine store resgister 
-- Content details middle
-+ Total user account
-+ Total herb medicine store
-+ Pending approved herb medicine store
-+ Total viewer
-</t>
   </si>
   <si>
     <t xml:space="preserve">1. Login successfully
@@ -1877,6 +1846,38 @@
 2. Input username "email0@gmail.com" password "123456"
 3. Click "Login" button
 4. Click remedy management tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Admin Page is displayed with the following list:
+- Header
+- Right Side bar:
++ Logout button
+- Content details left
++ Dashboard (default)
++ User management
++ New herb medicine store resgister 
+</t>
+  </si>
+  <si>
+    <t>1. Enter the admin page
+2. Input correct account and password as admin rule
+3. Click logout button in Right Slide bar</t>
+  </si>
+  <si>
+    <t>1. Log in Page is displayed
+2. Login successful as admin rule
+3. Login page is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter the admin page
+2. Click Dashboard tab in Left Slide bar
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click Dashboard tab </t>
+  </si>
+  <si>
+    <t>Check User Management tab</t>
   </si>
 </sst>
 </file>
@@ -3968,7 +3969,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="201" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D4" s="201"/>
       <c r="E4" s="201"/>
@@ -3976,7 +3977,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
@@ -3984,7 +3985,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="201" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D5" s="201"/>
       <c r="E5" s="201"/>
@@ -3992,7 +3993,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
@@ -4076,7 +4077,7 @@
         <v>55</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="19" customFormat="1" ht="21.75" customHeight="1">
@@ -4212,7 +4213,7 @@
       </c>
       <c r="C5" s="204"/>
       <c r="D5" s="205" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E5" s="205"/>
       <c r="F5" s="205"/>
@@ -4253,13 +4254,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D9" s="149" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="114" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F9" s="113" t="s">
         <v>90</v>
@@ -4432,7 +4433,7 @@
       </c>
       <c r="F3" s="208"/>
       <c r="G3" s="10" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H3" s="65"/>
     </row>
@@ -4450,7 +4451,7 @@
       </c>
       <c r="F4" s="208"/>
       <c r="G4" s="10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H4" s="65"/>
     </row>
@@ -4541,7 +4542,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="149" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D11" s="76">
         <f>User_Function!A6</f>
@@ -4570,7 +4571,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="199" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D12" s="76">
         <f>Mod_Function!A6</f>
@@ -5131,7 +5132,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="213" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C4" s="213"/>
       <c r="D4" s="213"/>
@@ -5288,7 +5289,7 @@
         <v>57</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D12" s="117" t="s">
         <v>94</v>
@@ -5309,7 +5310,7 @@
         <v>58</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D13" s="117" t="s">
         <v>95</v>
@@ -5330,10 +5331,10 @@
         <v>59</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D14" s="121" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E14" s="122"/>
       <c r="F14" s="117"/>
@@ -5351,7 +5352,7 @@
         <v>60</v>
       </c>
       <c r="C15" s="124" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D15" s="124" t="s">
         <v>96</v>
@@ -5372,10 +5373,10 @@
         <v>61</v>
       </c>
       <c r="C16" s="124" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D16" s="124" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E16" s="125"/>
       <c r="F16" s="117"/>
@@ -5393,10 +5394,10 @@
         <v>62</v>
       </c>
       <c r="C17" s="124" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D17" s="124" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E17" s="125"/>
       <c r="F17" s="117"/>
@@ -5414,10 +5415,10 @@
         <v>63</v>
       </c>
       <c r="C18" s="124" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D18" s="124" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E18" s="125"/>
       <c r="F18" s="117"/>
@@ -5449,10 +5450,10 @@
         <v>79</v>
       </c>
       <c r="C20" s="91" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D20" s="91" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E20" s="91" t="s">
         <v>80</v>
@@ -5466,7 +5467,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="58"/>
       <c r="B21" s="58" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
@@ -5486,7 +5487,7 @@
         <v>84</v>
       </c>
       <c r="C22" s="91" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D22" s="91" t="s">
         <v>158</v>
@@ -5509,10 +5510,10 @@
         <v>85</v>
       </c>
       <c r="C23" s="91" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D23" s="91" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E23" s="91"/>
       <c r="F23" s="117"/>
@@ -5530,10 +5531,10 @@
         <v>86</v>
       </c>
       <c r="C24" s="91" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D24" s="91" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E24" s="91" t="s">
         <v>81</v>
@@ -5564,13 +5565,13 @@
         <v>[User_login-16]</v>
       </c>
       <c r="B26" s="91" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C26" s="91" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D26" s="136" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E26" s="91" t="s">
         <v>83</v>
@@ -5590,10 +5591,10 @@
         <v>87</v>
       </c>
       <c r="C27" s="91" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D27" s="91" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="E27" s="91" t="s">
         <v>81</v>
@@ -5627,10 +5628,10 @@
         <v>159</v>
       </c>
       <c r="C29" s="106" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D29" s="104" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E29" s="104" t="s">
         <v>88</v>
@@ -5650,10 +5651,10 @@
         <v>89</v>
       </c>
       <c r="C30" s="106" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D30" s="104" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="E30" s="104" t="s">
         <v>88</v>
@@ -5666,7 +5667,7 @@
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1">
       <c r="A31" s="58" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B31" s="58" t="s">
         <v>161</v>
@@ -5686,13 +5687,13 @@
         <v>[User_login-22]</v>
       </c>
       <c r="B32" s="91" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C32" s="106" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D32" s="104" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="E32" s="104"/>
       <c r="F32" s="117"/>
@@ -5707,13 +5708,13 @@
         <v>[User_login-23]</v>
       </c>
       <c r="B33" s="91" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C33" s="106" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D33" s="104" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E33" s="104"/>
       <c r="F33" s="117"/>
@@ -5724,10 +5725,10 @@
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
       <c r="A34" s="58" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B34" s="58" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="59"/>
@@ -5744,13 +5745,13 @@
         <v>[User_login-25]</v>
       </c>
       <c r="B35" s="91" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C35" s="106" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="D35" s="104" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="E35" s="104"/>
       <c r="F35" s="117"/>
@@ -5762,7 +5763,7 @@
     <row r="36" spans="1:10" ht="14.25" customHeight="1">
       <c r="A36" s="169"/>
       <c r="B36" s="169" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C36" s="166"/>
       <c r="D36" s="166"/>
@@ -5779,13 +5780,13 @@
         <v>[User_login-27]</v>
       </c>
       <c r="B37" s="117" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C37" s="117" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D37" s="117" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E37" s="118"/>
       <c r="F37" s="117"/>
@@ -5800,13 +5801,13 @@
         <v>[User_login-28]</v>
       </c>
       <c r="B38" s="117" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C38" s="117" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D38" s="117" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E38" s="118"/>
       <c r="F38" s="117"/>
@@ -5817,10 +5818,10 @@
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1">
       <c r="A39" s="169" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B39" s="169" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C39" s="166"/>
       <c r="D39" s="166"/>
@@ -5837,13 +5838,13 @@
         <v>[User_login-30]</v>
       </c>
       <c r="B40" s="117" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C40" s="117" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D40" s="117" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E40" s="118"/>
       <c r="F40" s="117"/>
@@ -5854,10 +5855,10 @@
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1">
       <c r="A41" s="169" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B41" s="169" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C41" s="166"/>
       <c r="D41" s="166"/>
@@ -5874,13 +5875,13 @@
         <v>[User_login-32]</v>
       </c>
       <c r="B42" s="117" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C42" s="117" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D42" s="117" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E42" s="118"/>
       <c r="F42" s="117"/>
@@ -5891,10 +5892,10 @@
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1">
       <c r="A43" s="169" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B43" s="169" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C43" s="166"/>
       <c r="D43" s="166"/>
@@ -5911,13 +5912,13 @@
         <v>[User_login-34]</v>
       </c>
       <c r="B44" s="117" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C44" s="117" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D44" s="117" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E44" s="118"/>
       <c r="F44" s="117"/>
@@ -5928,10 +5929,10 @@
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1">
       <c r="A45" s="169" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B45" s="169" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C45" s="166"/>
       <c r="D45" s="166"/>
@@ -5948,13 +5949,13 @@
         <v>[User_login-36]</v>
       </c>
       <c r="B46" s="117" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C46" s="117" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D46" s="117" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="E46" s="118"/>
       <c r="F46" s="117"/>
@@ -5965,10 +5966,10 @@
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1">
       <c r="A47" s="169" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B47" s="169" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C47" s="166"/>
       <c r="D47" s="166"/>
@@ -5985,13 +5986,13 @@
         <v>[User_login-38]</v>
       </c>
       <c r="B48" s="117" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C48" s="117" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D48" s="117" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E48" s="118"/>
       <c r="F48" s="117"/>
@@ -6002,10 +6003,10 @@
     </row>
     <row r="49" spans="1:10" ht="14.25" customHeight="1">
       <c r="A49" s="169" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B49" s="169" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C49" s="166"/>
       <c r="D49" s="166"/>
@@ -6022,13 +6023,13 @@
         <v>[User_login-40]</v>
       </c>
       <c r="B50" s="117" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C50" s="117" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D50" s="117" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="E50" s="118"/>
       <c r="F50" s="117"/>
@@ -6039,10 +6040,10 @@
     </row>
     <row r="51" spans="1:10" ht="14.25" customHeight="1">
       <c r="A51" s="169" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B51" s="169" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C51" s="166"/>
       <c r="D51" s="166"/>
@@ -6059,13 +6060,13 @@
         <v>[User_login-42]</v>
       </c>
       <c r="B52" s="117" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C52" s="117" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D52" s="117" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E52" s="118"/>
       <c r="F52" s="117"/>
@@ -6076,10 +6077,10 @@
     </row>
     <row r="53" spans="1:10" ht="14.25" customHeight="1">
       <c r="A53" s="169" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B53" s="169" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C53" s="166"/>
       <c r="D53" s="166"/>
@@ -6096,13 +6097,13 @@
         <v>[User_login-44]</v>
       </c>
       <c r="B54" s="117" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C54" s="117" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D54" s="117" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="E54" s="118"/>
       <c r="F54" s="117"/>
@@ -6112,10 +6113,10 @@
     </row>
     <row r="55" spans="1:10" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A55" s="169" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B55" s="169" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C55" s="166"/>
       <c r="D55" s="166"/>
@@ -6131,13 +6132,13 @@
         <v>[User_login-46]</v>
       </c>
       <c r="B56" s="117" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C56" s="117" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D56" s="117" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="E56" s="118"/>
       <c r="F56" s="117"/>
@@ -6147,10 +6148,10 @@
     </row>
     <row r="57" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A57" s="169" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B57" s="169" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C57" s="166"/>
       <c r="D57" s="166"/>
@@ -6166,13 +6167,13 @@
         <v>[User_login-48]</v>
       </c>
       <c r="B58" s="117" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C58" s="117" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D58" s="117" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E58" s="118"/>
       <c r="F58" s="117"/>
@@ -6205,7 +6206,7 @@
     <row r="61" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A61" s="169"/>
       <c r="B61" s="169" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C61" s="169"/>
       <c r="D61" s="169"/>
@@ -6218,7 +6219,7 @@
     <row r="62" spans="1:10" s="169" customFormat="1" ht="14.25" customHeight="1">
       <c r="A62" s="185"/>
       <c r="B62" s="186" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C62" s="187"/>
       <c r="D62" s="187"/>
@@ -6234,20 +6235,20 @@
         <v>ID-44</v>
       </c>
       <c r="B63" s="117" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C63" s="117" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D63" s="117" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E63" s="117"/>
       <c r="F63" s="117"/>
       <c r="G63" s="117"/>
       <c r="H63" s="117"/>
       <c r="I63" s="188" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="190" customFormat="1" ht="14.25" customHeight="1">
@@ -6256,20 +6257,20 @@
         <v>ID-45</v>
       </c>
       <c r="B64" s="117" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C64" s="117" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D64" s="117" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E64" s="117"/>
       <c r="F64" s="117"/>
       <c r="G64" s="117"/>
       <c r="H64" s="117"/>
       <c r="I64" s="188" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="190" customFormat="1" ht="14.25" customHeight="1">
@@ -6278,20 +6279,20 @@
         <v>ID-46</v>
       </c>
       <c r="B65" s="117" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C65" s="117" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D65" s="117" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E65" s="117"/>
       <c r="F65" s="117"/>
       <c r="G65" s="117"/>
       <c r="H65" s="117"/>
       <c r="I65" s="188" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="189" customFormat="1" ht="14.25" customHeight="1">
@@ -6300,20 +6301,20 @@
         <v>ID-47</v>
       </c>
       <c r="B66" s="117" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C66" s="117" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D66" s="117" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E66" s="117"/>
       <c r="F66" s="117"/>
       <c r="G66" s="117"/>
       <c r="H66" s="117"/>
       <c r="I66" s="188" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6322,20 +6323,20 @@
         <v>ID-48</v>
       </c>
       <c r="B67" s="117" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C67" s="117" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D67" s="117" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E67" s="117"/>
       <c r="F67" s="117"/>
       <c r="G67" s="117"/>
       <c r="H67" s="117"/>
       <c r="I67" s="188" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6344,26 +6345,26 @@
         <v>ID-49</v>
       </c>
       <c r="B68" s="117" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C68" s="117" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D68" s="117" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E68" s="117"/>
       <c r="F68" s="117"/>
       <c r="G68" s="117"/>
       <c r="H68" s="117"/>
       <c r="I68" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A69" s="169"/>
       <c r="B69" s="169" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C69" s="169"/>
       <c r="D69" s="169"/>
@@ -6379,20 +6380,20 @@
         <v>ID-50</v>
       </c>
       <c r="B70" s="117" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C70" s="117" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D70" s="117" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E70" s="117"/>
       <c r="F70" s="117"/>
       <c r="G70" s="117"/>
       <c r="H70" s="117"/>
       <c r="I70" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6401,20 +6402,20 @@
         <v>ID-51</v>
       </c>
       <c r="B71" s="117" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C71" s="117" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D71" s="117" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E71" s="117"/>
       <c r="F71" s="117"/>
       <c r="G71" s="117"/>
       <c r="H71" s="117"/>
       <c r="I71" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6423,20 +6424,20 @@
         <v>ID-52</v>
       </c>
       <c r="B72" s="117" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C72" s="117" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D72" s="117" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E72" s="117"/>
       <c r="F72" s="117"/>
       <c r="G72" s="117"/>
       <c r="H72" s="117"/>
       <c r="I72" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6445,20 +6446,20 @@
         <v>ID-53</v>
       </c>
       <c r="B73" s="117" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C73" s="117" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D73" s="117" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E73" s="117"/>
       <c r="F73" s="117"/>
       <c r="G73" s="117"/>
       <c r="H73" s="117"/>
       <c r="I73" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6467,20 +6468,20 @@
         <v>ID-54</v>
       </c>
       <c r="B74" s="117" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C74" s="117" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D74" s="117" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E74" s="117"/>
       <c r="F74" s="117"/>
       <c r="G74" s="117"/>
       <c r="H74" s="117"/>
       <c r="I74" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6489,20 +6490,20 @@
         <v>ID-55</v>
       </c>
       <c r="B75" s="117" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C75" s="117" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D75" s="117" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E75" s="117"/>
       <c r="F75" s="117"/>
       <c r="G75" s="117"/>
       <c r="H75" s="117"/>
       <c r="I75" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="13.5" customHeight="1">
@@ -6511,20 +6512,20 @@
         <v>ID-56</v>
       </c>
       <c r="B76" s="117" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C76" s="117" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D76" s="117" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E76" s="117"/>
       <c r="F76" s="117"/>
       <c r="G76" s="117"/>
       <c r="H76" s="117"/>
       <c r="I76" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="13.5" customHeight="1">
@@ -6533,20 +6534,20 @@
         <v>ID-57</v>
       </c>
       <c r="B77" s="117" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C77" s="117" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D77" s="117" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E77" s="117"/>
       <c r="F77" s="117"/>
       <c r="G77" s="117"/>
       <c r="H77" s="117"/>
       <c r="I77" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="13.5" customHeight="1">
@@ -6555,20 +6556,20 @@
         <v>ID-58</v>
       </c>
       <c r="B78" s="117" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C78" s="117" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D78" s="117" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E78" s="117"/>
       <c r="F78" s="117"/>
       <c r="G78" s="117"/>
       <c r="H78" s="117"/>
       <c r="I78" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="13.5" customHeight="1">
@@ -6577,20 +6578,20 @@
         <v>ID-59</v>
       </c>
       <c r="B79" s="117" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C79" s="117" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D79" s="117" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E79" s="117"/>
       <c r="F79" s="117"/>
       <c r="G79" s="117"/>
       <c r="H79" s="117"/>
       <c r="I79" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13.5" customHeight="1">
@@ -6599,20 +6600,20 @@
         <v>ID-60</v>
       </c>
       <c r="B80" s="117" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C80" s="117" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D80" s="117" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E80" s="117"/>
       <c r="F80" s="117"/>
       <c r="G80" s="117"/>
       <c r="H80" s="117"/>
       <c r="I80" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="13.5" customHeight="1">
@@ -6621,20 +6622,20 @@
         <v>ID-61</v>
       </c>
       <c r="B81" s="117" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C81" s="117" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D81" s="117" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E81" s="117"/>
       <c r="F81" s="117"/>
       <c r="G81" s="117"/>
       <c r="H81" s="117"/>
       <c r="I81" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="13.5" customHeight="1">
@@ -6643,20 +6644,20 @@
         <v>ID-62</v>
       </c>
       <c r="B82" s="117" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C82" s="117" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D82" s="117" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E82" s="117"/>
       <c r="F82" s="117"/>
       <c r="G82" s="117"/>
       <c r="H82" s="117"/>
       <c r="I82" s="117" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -6705,8 +6706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -6729,7 +6730,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="137" customFormat="1" ht="18" thickBot="1">
       <c r="A1" s="138" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="139"/>
       <c r="C1" s="139"/>
@@ -6743,7 +6744,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="212" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C2" s="212"/>
       <c r="D2" s="212"/>
@@ -6756,10 +6757,10 @@
     </row>
     <row r="3" spans="1:10" s="137" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="142" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B3" s="212" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C3" s="212"/>
       <c r="D3" s="212"/>
@@ -6772,10 +6773,10 @@
     </row>
     <row r="4" spans="1:10" s="137" customFormat="1" ht="17">
       <c r="A4" s="141" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B4" s="213" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C4" s="213"/>
       <c r="D4" s="213"/>
@@ -6792,13 +6793,13 @@
         <v>24</v>
       </c>
       <c r="C5" s="144" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D5" s="145" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="216" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F5" s="216"/>
       <c r="G5" s="216"/>
@@ -6859,16 +6860,16 @@
         <v>30</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F10" s="57" t="s">
         <v>92</v>
@@ -6877,7 +6878,7 @@
         <v>93</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I10" s="56" t="s">
         <v>36</v>
@@ -6902,13 +6903,13 @@
         <v>[Mod_login-2]</v>
       </c>
       <c r="B12" s="117" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="117"/>
@@ -6925,10 +6926,10 @@
         <v>64</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D13" s="117" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E13" s="197"/>
       <c r="F13" s="117"/>
@@ -6945,10 +6946,10 @@
         <v>165</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D14" s="117" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E14" s="173"/>
       <c r="F14" s="117"/>
@@ -6965,10 +6966,10 @@
         <v>168</v>
       </c>
       <c r="C15" s="117" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D15" s="117" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E15" s="173"/>
       <c r="F15" s="117"/>
@@ -6985,10 +6986,10 @@
         <v>74</v>
       </c>
       <c r="C16" s="117" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D16" s="117" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E16" s="173"/>
       <c r="F16" s="117"/>
@@ -7005,10 +7006,10 @@
         <v>66</v>
       </c>
       <c r="C17" s="117" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D17" s="117" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E17" s="173"/>
       <c r="F17" s="117"/>
@@ -7025,10 +7026,10 @@
         <v>68</v>
       </c>
       <c r="C18" s="117" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D18" s="117" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E18" s="173"/>
       <c r="F18" s="117"/>
@@ -7045,10 +7046,10 @@
         <v>70</v>
       </c>
       <c r="C19" s="117" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D19" s="117" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E19" s="173"/>
       <c r="F19" s="117"/>
@@ -7065,10 +7066,10 @@
         <v>72</v>
       </c>
       <c r="C20" s="117" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D20" s="117" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E20" s="173"/>
       <c r="F20" s="117"/>
@@ -7080,7 +7081,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="176"/>
       <c r="B21" s="177" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C21" s="176"/>
       <c r="D21" s="176"/>
@@ -7097,13 +7098,13 @@
         <v>[Mod_login-12]</v>
       </c>
       <c r="B22" s="117" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C22" s="117" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="E22" s="179"/>
       <c r="F22" s="117"/>
@@ -7118,13 +7119,13 @@
         <v>[Mod_login-13]</v>
       </c>
       <c r="B23" s="117" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E23" s="179"/>
       <c r="F23" s="117"/>
@@ -7135,7 +7136,7 @@
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
       <c r="A24" s="176" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B24" s="58" t="s">
         <v>78</v>
@@ -7158,10 +7159,10 @@
         <v>79</v>
       </c>
       <c r="C25" s="91" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D25" s="91" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E25" s="179"/>
       <c r="F25" s="117"/>
@@ -7171,10 +7172,10 @@
     </row>
     <row r="26" spans="1:10" ht="13.5" customHeight="1">
       <c r="A26" s="176" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C26" s="176"/>
       <c r="D26" s="176"/>
@@ -7190,13 +7191,13 @@
         <v>[Mod_login-17]</v>
       </c>
       <c r="B27" s="117" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C27" s="117" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D27" s="117" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E27" s="173"/>
       <c r="F27" s="117"/>
@@ -7206,10 +7207,10 @@
     </row>
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
       <c r="A28" s="176" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>
@@ -7225,13 +7226,13 @@
         <v>[Mod_login-19]</v>
       </c>
       <c r="B29" s="117" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C29" s="117" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D29" s="117" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E29" s="173"/>
       <c r="F29" s="117"/>
@@ -7241,10 +7242,10 @@
     </row>
     <row r="30" spans="1:10" ht="13.5" customHeight="1">
       <c r="A30" s="176" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B30" s="58" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C30" s="176"/>
       <c r="D30" s="176"/>
@@ -7260,13 +7261,13 @@
         <v>[Mod_login-21]</v>
       </c>
       <c r="B31" s="117" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C31" s="117" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D31" s="117" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E31" s="173"/>
       <c r="F31" s="117"/>
@@ -7308,8 +7309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -7332,7 +7333,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="137" customFormat="1" ht="18" thickBot="1">
       <c r="A1" s="138" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="139"/>
       <c r="C1" s="139"/>
@@ -7359,10 +7360,10 @@
     </row>
     <row r="3" spans="1:10" s="137" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="142" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B3" s="212" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C3" s="212"/>
       <c r="D3" s="212"/>
@@ -7375,10 +7376,10 @@
     </row>
     <row r="4" spans="1:10" s="137" customFormat="1" ht="17">
       <c r="A4" s="141" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B4" s="213" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C4" s="213"/>
       <c r="D4" s="213"/>
@@ -7395,13 +7396,13 @@
         <v>24</v>
       </c>
       <c r="C5" s="144" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D5" s="145" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="216" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F5" s="216"/>
       <c r="G5" s="216"/>
@@ -7462,16 +7463,16 @@
         <v>30</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F10" s="57" t="s">
         <v>92</v>
@@ -7480,7 +7481,7 @@
         <v>93</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I10" s="56" t="s">
         <v>36</v>
@@ -7505,13 +7506,13 @@
         <v>[Admin_login-2]</v>
       </c>
       <c r="B12" s="117" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C12" s="117" t="s">
         <v>163</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="117"/>
@@ -7534,7 +7535,7 @@
         <v>164</v>
       </c>
       <c r="E13" s="173" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F13" s="117"/>
       <c r="G13" s="117"/>
@@ -7556,7 +7557,7 @@
         <v>167</v>
       </c>
       <c r="E14" s="173" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F14" s="117"/>
       <c r="G14" s="117"/>
@@ -7578,7 +7579,7 @@
         <v>170</v>
       </c>
       <c r="E15" s="173" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F15" s="117"/>
       <c r="G15" s="117"/>
@@ -7600,7 +7601,7 @@
         <v>76</v>
       </c>
       <c r="E16" s="173" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F16" s="117"/>
       <c r="G16" s="117"/>
@@ -7622,7 +7623,7 @@
         <v>67</v>
       </c>
       <c r="E17" s="173" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F17" s="117"/>
       <c r="G17" s="117"/>
@@ -7644,7 +7645,7 @@
         <v>69</v>
       </c>
       <c r="E18" s="173" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F18" s="117"/>
       <c r="G18" s="117"/>
@@ -7666,7 +7667,7 @@
         <v>69</v>
       </c>
       <c r="E19" s="173" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F19" s="117"/>
       <c r="G19" s="117"/>
@@ -7688,7 +7689,7 @@
         <v>69</v>
       </c>
       <c r="E20" s="173" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F20" s="117"/>
       <c r="G20" s="117"/>
@@ -7716,16 +7717,16 @@
         <v>[Admin_login-12]</v>
       </c>
       <c r="B22" s="117" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C22" s="117" t="s">
         <v>163</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>264</v>
+        <v>377</v>
       </c>
       <c r="E22" s="179" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F22" s="117"/>
       <c r="G22" s="117"/>
@@ -7739,16 +7740,16 @@
         <v>[Admin_login-13]</v>
       </c>
       <c r="B23" s="117" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>174</v>
+        <v>378</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>260</v>
+        <v>379</v>
       </c>
       <c r="E23" s="179" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F23" s="117"/>
       <c r="G23" s="117"/>
@@ -7759,7 +7760,7 @@
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
       <c r="A24" s="176"/>
       <c r="B24" s="177" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C24" s="176"/>
       <c r="D24" s="176"/>
@@ -7776,16 +7777,16 @@
         <v>[Admin_login-15]</v>
       </c>
       <c r="B25" s="117" t="s">
-        <v>191</v>
+        <v>381</v>
       </c>
       <c r="C25" s="117" t="s">
-        <v>176</v>
+        <v>380</v>
       </c>
       <c r="D25" s="180" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E25" s="179" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F25" s="117"/>
       <c r="G25" s="117"/>
@@ -7796,7 +7797,7 @@
     <row r="26" spans="1:10" ht="14.25" customHeight="1">
       <c r="A26" s="176"/>
       <c r="B26" s="177" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C26" s="176"/>
       <c r="D26" s="176"/>
@@ -7813,13 +7814,13 @@
         <v>[Admin_login-17]</v>
       </c>
       <c r="B27" s="117" t="s">
-        <v>193</v>
+        <v>382</v>
       </c>
       <c r="C27" s="117" t="s">
-        <v>176</v>
+        <v>380</v>
       </c>
       <c r="D27" s="180" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E27" s="179"/>
       <c r="F27" s="117"/>
@@ -7831,7 +7832,7 @@
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
       <c r="A28" s="176"/>
       <c r="B28" s="177" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>

</xml_diff>

<commit_message>
update final integration test report 3
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
+++ b/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" activeTab="6"/>
+    <workbookView xWindow="700" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,10 @@
     <sheet name="User_Function" sheetId="9" r:id="rId5"/>
     <sheet name="Mod_Function" sheetId="12" r:id="rId6"/>
     <sheet name="Admin_Function" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="ACTION" localSheetId="3">#REF!</definedName>
@@ -252,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="387">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -848,13 +849,6 @@
   <si>
     <t>1. Admin Page is displayed
 2. Content about dashboard is displayed</t>
-  </si>
-  <si>
-    <t>1. Admin Page is displayed
-2. Dropdowlist is displayed with:
-+ Dashboard
-+ User list
-3. Content about dashboard of user is displayed</t>
   </si>
   <si>
     <t>Check clicking on link on Home page screen</t>
@@ -1230,9 +1224,6 @@
 + Remedy
 + Author
 + Posted date</t>
-  </si>
-  <si>
-    <t>New herb medicine store</t>
   </si>
   <si>
     <t>Integration Login with medicinal plants</t>
@@ -1878,6 +1869,30 @@
   </si>
   <si>
     <t>Check User Management tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter the admin page
+2. Click User Management tab in Left Slide bar
+</t>
+  </si>
+  <si>
+    <t>1. Admin Page is displayed
+2. User Information Management page is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter the admin page
+2. Click New Herb Medicine Store tab in Left Slide bar
+</t>
+  </si>
+  <si>
+    <t>1. Admin Page is displayed
+2. New register of herb medicine store information page is displayed</t>
+  </si>
+  <si>
+    <t>New register of herb medicine store</t>
+  </si>
+  <si>
+    <t>Check New register of Herb Medicine Store tap</t>
   </si>
 </sst>
 </file>
@@ -2769,7 +2784,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
@@ -2834,6 +2849,8 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3420,7 +3437,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -3477,6 +3494,8 @@
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
@@ -3969,7 +3988,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="201" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D4" s="201"/>
       <c r="E4" s="201"/>
@@ -3977,7 +3996,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
@@ -3985,7 +4004,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="201" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D5" s="201"/>
       <c r="E5" s="201"/>
@@ -3993,7 +4012,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
@@ -4077,7 +4096,7 @@
         <v>55</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="19" customFormat="1" ht="21.75" customHeight="1">
@@ -4213,7 +4232,7 @@
       </c>
       <c r="C5" s="204"/>
       <c r="D5" s="205" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E5" s="205"/>
       <c r="F5" s="205"/>
@@ -4254,13 +4273,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D9" s="149" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="114" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F9" s="113" t="s">
         <v>90</v>
@@ -4433,7 +4452,7 @@
       </c>
       <c r="F3" s="208"/>
       <c r="G3" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H3" s="65"/>
     </row>
@@ -4451,7 +4470,7 @@
       </c>
       <c r="F4" s="208"/>
       <c r="G4" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H4" s="65"/>
     </row>
@@ -4542,7 +4561,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="149" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D11" s="76">
         <f>User_Function!A6</f>
@@ -4571,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="199" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D12" s="76">
         <f>Mod_Function!A6</f>
@@ -4612,7 +4631,7 @@
       </c>
       <c r="F13" s="76">
         <f>Admin_Function!C6</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G13" s="76">
         <f>Admin_Function!D6</f>
@@ -4620,7 +4639,7 @@
       </c>
       <c r="H13" s="77">
         <f>Admin_Function!E6</f>
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4639,7 +4658,7 @@
       </c>
       <c r="F14" s="79">
         <f>SUM(F11:F13)</f>
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="G14" s="79">
         <f>SUM(G9:G13)</f>
@@ -4647,7 +4666,7 @@
       </c>
       <c r="H14" s="80">
         <f>SUM(H11:H13)</f>
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -5132,7 +5151,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="213" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="213"/>
       <c r="D4" s="213"/>
@@ -5289,7 +5308,7 @@
         <v>57</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D12" s="117" t="s">
         <v>94</v>
@@ -5310,7 +5329,7 @@
         <v>58</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D13" s="117" t="s">
         <v>95</v>
@@ -5331,10 +5350,10 @@
         <v>59</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D14" s="121" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E14" s="122"/>
       <c r="F14" s="117"/>
@@ -5352,7 +5371,7 @@
         <v>60</v>
       </c>
       <c r="C15" s="124" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D15" s="124" t="s">
         <v>96</v>
@@ -5373,10 +5392,10 @@
         <v>61</v>
       </c>
       <c r="C16" s="124" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D16" s="124" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E16" s="125"/>
       <c r="F16" s="117"/>
@@ -5394,10 +5413,10 @@
         <v>62</v>
       </c>
       <c r="C17" s="124" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D17" s="124" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E17" s="125"/>
       <c r="F17" s="117"/>
@@ -5415,10 +5434,10 @@
         <v>63</v>
       </c>
       <c r="C18" s="124" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D18" s="124" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E18" s="125"/>
       <c r="F18" s="117"/>
@@ -5450,10 +5469,10 @@
         <v>79</v>
       </c>
       <c r="C20" s="91" t="s">
+        <v>249</v>
+      </c>
+      <c r="D20" s="91" t="s">
         <v>250</v>
-      </c>
-      <c r="D20" s="91" t="s">
-        <v>251</v>
       </c>
       <c r="E20" s="91" t="s">
         <v>80</v>
@@ -5467,7 +5486,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="58"/>
       <c r="B21" s="58" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
@@ -5487,7 +5506,7 @@
         <v>84</v>
       </c>
       <c r="C22" s="91" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D22" s="91" t="s">
         <v>158</v>
@@ -5510,10 +5529,10 @@
         <v>85</v>
       </c>
       <c r="C23" s="91" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D23" s="91" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E23" s="91"/>
       <c r="F23" s="117"/>
@@ -5531,10 +5550,10 @@
         <v>86</v>
       </c>
       <c r="C24" s="91" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D24" s="91" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E24" s="91" t="s">
         <v>81</v>
@@ -5565,13 +5584,13 @@
         <v>[User_login-16]</v>
       </c>
       <c r="B26" s="91" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C26" s="91" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D26" s="136" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E26" s="91" t="s">
         <v>83</v>
@@ -5591,10 +5610,10 @@
         <v>87</v>
       </c>
       <c r="C27" s="91" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D27" s="91" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E27" s="91" t="s">
         <v>81</v>
@@ -5628,10 +5647,10 @@
         <v>159</v>
       </c>
       <c r="C29" s="106" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D29" s="104" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E29" s="104" t="s">
         <v>88</v>
@@ -5651,10 +5670,10 @@
         <v>89</v>
       </c>
       <c r="C30" s="106" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D30" s="104" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E30" s="104" t="s">
         <v>88</v>
@@ -5667,7 +5686,7 @@
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1">
       <c r="A31" s="58" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B31" s="58" t="s">
         <v>161</v>
@@ -5687,13 +5706,13 @@
         <v>[User_login-22]</v>
       </c>
       <c r="B32" s="91" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C32" s="106" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D32" s="104" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E32" s="104"/>
       <c r="F32" s="117"/>
@@ -5708,13 +5727,13 @@
         <v>[User_login-23]</v>
       </c>
       <c r="B33" s="91" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C33" s="106" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D33" s="104" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E33" s="104"/>
       <c r="F33" s="117"/>
@@ -5725,10 +5744,10 @@
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
       <c r="A34" s="58" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B34" s="58" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="59"/>
@@ -5745,13 +5764,13 @@
         <v>[User_login-25]</v>
       </c>
       <c r="B35" s="91" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C35" s="106" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D35" s="104" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E35" s="104"/>
       <c r="F35" s="117"/>
@@ -5763,7 +5782,7 @@
     <row r="36" spans="1:10" ht="14.25" customHeight="1">
       <c r="A36" s="169"/>
       <c r="B36" s="169" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C36" s="166"/>
       <c r="D36" s="166"/>
@@ -5780,13 +5799,13 @@
         <v>[User_login-27]</v>
       </c>
       <c r="B37" s="117" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C37" s="117" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D37" s="117" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E37" s="118"/>
       <c r="F37" s="117"/>
@@ -5801,13 +5820,13 @@
         <v>[User_login-28]</v>
       </c>
       <c r="B38" s="117" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C38" s="117" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D38" s="117" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E38" s="118"/>
       <c r="F38" s="117"/>
@@ -5818,10 +5837,10 @@
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1">
       <c r="A39" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B39" s="169" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C39" s="166"/>
       <c r="D39" s="166"/>
@@ -5838,13 +5857,13 @@
         <v>[User_login-30]</v>
       </c>
       <c r="B40" s="117" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C40" s="117" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D40" s="117" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E40" s="118"/>
       <c r="F40" s="117"/>
@@ -5855,10 +5874,10 @@
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1">
       <c r="A41" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B41" s="169" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C41" s="166"/>
       <c r="D41" s="166"/>
@@ -5875,13 +5894,13 @@
         <v>[User_login-32]</v>
       </c>
       <c r="B42" s="117" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C42" s="117" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D42" s="117" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E42" s="118"/>
       <c r="F42" s="117"/>
@@ -5892,10 +5911,10 @@
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1">
       <c r="A43" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B43" s="169" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C43" s="166"/>
       <c r="D43" s="166"/>
@@ -5912,13 +5931,13 @@
         <v>[User_login-34]</v>
       </c>
       <c r="B44" s="117" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C44" s="117" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D44" s="117" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E44" s="118"/>
       <c r="F44" s="117"/>
@@ -5929,10 +5948,10 @@
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1">
       <c r="A45" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B45" s="169" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C45" s="166"/>
       <c r="D45" s="166"/>
@@ -5949,13 +5968,13 @@
         <v>[User_login-36]</v>
       </c>
       <c r="B46" s="117" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C46" s="117" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D46" s="117" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E46" s="118"/>
       <c r="F46" s="117"/>
@@ -5966,10 +5985,10 @@
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1">
       <c r="A47" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B47" s="169" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C47" s="166"/>
       <c r="D47" s="166"/>
@@ -5986,13 +6005,13 @@
         <v>[User_login-38]</v>
       </c>
       <c r="B48" s="117" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C48" s="117" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D48" s="117" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E48" s="118"/>
       <c r="F48" s="117"/>
@@ -6003,10 +6022,10 @@
     </row>
     <row r="49" spans="1:10" ht="14.25" customHeight="1">
       <c r="A49" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B49" s="169" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C49" s="166"/>
       <c r="D49" s="166"/>
@@ -6023,13 +6042,13 @@
         <v>[User_login-40]</v>
       </c>
       <c r="B50" s="117" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C50" s="117" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D50" s="117" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E50" s="118"/>
       <c r="F50" s="117"/>
@@ -6040,10 +6059,10 @@
     </row>
     <row r="51" spans="1:10" ht="14.25" customHeight="1">
       <c r="A51" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B51" s="169" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C51" s="166"/>
       <c r="D51" s="166"/>
@@ -6060,13 +6079,13 @@
         <v>[User_login-42]</v>
       </c>
       <c r="B52" s="117" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C52" s="117" t="s">
+        <v>303</v>
+      </c>
+      <c r="D52" s="117" t="s">
         <v>305</v>
-      </c>
-      <c r="D52" s="117" t="s">
-        <v>307</v>
       </c>
       <c r="E52" s="118"/>
       <c r="F52" s="117"/>
@@ -6077,10 +6096,10 @@
     </row>
     <row r="53" spans="1:10" ht="14.25" customHeight="1">
       <c r="A53" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B53" s="169" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C53" s="166"/>
       <c r="D53" s="166"/>
@@ -6097,13 +6116,13 @@
         <v>[User_login-44]</v>
       </c>
       <c r="B54" s="117" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C54" s="117" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D54" s="117" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E54" s="118"/>
       <c r="F54" s="117"/>
@@ -6113,10 +6132,10 @@
     </row>
     <row r="55" spans="1:10" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A55" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B55" s="169" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C55" s="166"/>
       <c r="D55" s="166"/>
@@ -6132,13 +6151,13 @@
         <v>[User_login-46]</v>
       </c>
       <c r="B56" s="117" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C56" s="117" t="s">
+        <v>344</v>
+      </c>
+      <c r="D56" s="117" t="s">
         <v>346</v>
-      </c>
-      <c r="D56" s="117" t="s">
-        <v>348</v>
       </c>
       <c r="E56" s="118"/>
       <c r="F56" s="117"/>
@@ -6148,10 +6167,10 @@
     </row>
     <row r="57" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A57" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B57" s="169" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C57" s="166"/>
       <c r="D57" s="166"/>
@@ -6167,13 +6186,13 @@
         <v>[User_login-48]</v>
       </c>
       <c r="B58" s="117" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C58" s="117" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D58" s="117" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E58" s="118"/>
       <c r="F58" s="117"/>
@@ -6206,7 +6225,7 @@
     <row r="61" spans="1:10" s="189" customFormat="1" ht="14.25" customHeight="1">
       <c r="A61" s="169"/>
       <c r="B61" s="169" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C61" s="169"/>
       <c r="D61" s="169"/>
@@ -6219,7 +6238,7 @@
     <row r="62" spans="1:10" s="169" customFormat="1" ht="14.25" customHeight="1">
       <c r="A62" s="185"/>
       <c r="B62" s="186" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C62" s="187"/>
       <c r="D62" s="187"/>
@@ -6235,20 +6254,20 @@
         <v>ID-44</v>
       </c>
       <c r="B63" s="117" t="s">
+        <v>194</v>
+      </c>
+      <c r="C63" s="117" t="s">
         <v>195</v>
       </c>
-      <c r="C63" s="117" t="s">
+      <c r="D63" s="117" t="s">
         <v>196</v>
-      </c>
-      <c r="D63" s="117" t="s">
-        <v>197</v>
       </c>
       <c r="E63" s="117"/>
       <c r="F63" s="117"/>
       <c r="G63" s="117"/>
       <c r="H63" s="117"/>
       <c r="I63" s="188" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="190" customFormat="1" ht="14.25" customHeight="1">
@@ -6257,20 +6276,20 @@
         <v>ID-45</v>
       </c>
       <c r="B64" s="117" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C64" s="117" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D64" s="117" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E64" s="117"/>
       <c r="F64" s="117"/>
       <c r="G64" s="117"/>
       <c r="H64" s="117"/>
       <c r="I64" s="188" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="190" customFormat="1" ht="14.25" customHeight="1">
@@ -6279,20 +6298,20 @@
         <v>ID-46</v>
       </c>
       <c r="B65" s="117" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C65" s="117" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D65" s="117" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E65" s="117"/>
       <c r="F65" s="117"/>
       <c r="G65" s="117"/>
       <c r="H65" s="117"/>
       <c r="I65" s="188" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="189" customFormat="1" ht="14.25" customHeight="1">
@@ -6301,20 +6320,20 @@
         <v>ID-47</v>
       </c>
       <c r="B66" s="117" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C66" s="117" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D66" s="117" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E66" s="117"/>
       <c r="F66" s="117"/>
       <c r="G66" s="117"/>
       <c r="H66" s="117"/>
       <c r="I66" s="188" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6323,20 +6342,20 @@
         <v>ID-48</v>
       </c>
       <c r="B67" s="117" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C67" s="117" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D67" s="117" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E67" s="117"/>
       <c r="F67" s="117"/>
       <c r="G67" s="117"/>
       <c r="H67" s="117"/>
       <c r="I67" s="188" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6345,26 +6364,26 @@
         <v>ID-49</v>
       </c>
       <c r="B68" s="117" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C68" s="117" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D68" s="117" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E68" s="117"/>
       <c r="F68" s="117"/>
       <c r="G68" s="117"/>
       <c r="H68" s="117"/>
       <c r="I68" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
       <c r="A69" s="169"/>
       <c r="B69" s="169" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C69" s="169"/>
       <c r="D69" s="169"/>
@@ -6380,20 +6399,20 @@
         <v>ID-50</v>
       </c>
       <c r="B70" s="117" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C70" s="117" t="s">
+        <v>236</v>
+      </c>
+      <c r="D70" s="117" t="s">
         <v>237</v>
-      </c>
-      <c r="D70" s="117" t="s">
-        <v>238</v>
       </c>
       <c r="E70" s="117"/>
       <c r="F70" s="117"/>
       <c r="G70" s="117"/>
       <c r="H70" s="117"/>
       <c r="I70" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6402,20 +6421,20 @@
         <v>ID-51</v>
       </c>
       <c r="B71" s="117" t="s">
+        <v>200</v>
+      </c>
+      <c r="C71" s="117" t="s">
         <v>201</v>
       </c>
-      <c r="C71" s="117" t="s">
+      <c r="D71" s="117" t="s">
         <v>202</v>
-      </c>
-      <c r="D71" s="117" t="s">
-        <v>203</v>
       </c>
       <c r="E71" s="117"/>
       <c r="F71" s="117"/>
       <c r="G71" s="117"/>
       <c r="H71" s="117"/>
       <c r="I71" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6424,20 +6443,20 @@
         <v>ID-52</v>
       </c>
       <c r="B72" s="117" t="s">
+        <v>203</v>
+      </c>
+      <c r="C72" s="117" t="s">
+        <v>201</v>
+      </c>
+      <c r="D72" s="117" t="s">
         <v>204</v>
-      </c>
-      <c r="C72" s="117" t="s">
-        <v>202</v>
-      </c>
-      <c r="D72" s="117" t="s">
-        <v>205</v>
       </c>
       <c r="E72" s="117"/>
       <c r="F72" s="117"/>
       <c r="G72" s="117"/>
       <c r="H72" s="117"/>
       <c r="I72" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6446,20 +6465,20 @@
         <v>ID-53</v>
       </c>
       <c r="B73" s="117" t="s">
+        <v>205</v>
+      </c>
+      <c r="C73" s="117" t="s">
         <v>206</v>
       </c>
-      <c r="C73" s="117" t="s">
-        <v>207</v>
-      </c>
       <c r="D73" s="117" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E73" s="117"/>
       <c r="F73" s="117"/>
       <c r="G73" s="117"/>
       <c r="H73" s="117"/>
       <c r="I73" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6468,20 +6487,20 @@
         <v>ID-54</v>
       </c>
       <c r="B74" s="117" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" s="117" t="s">
         <v>208</v>
       </c>
-      <c r="C74" s="117" t="s">
+      <c r="D74" s="117" t="s">
         <v>209</v>
-      </c>
-      <c r="D74" s="117" t="s">
-        <v>210</v>
       </c>
       <c r="E74" s="117"/>
       <c r="F74" s="117"/>
       <c r="G74" s="117"/>
       <c r="H74" s="117"/>
       <c r="I74" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="184" customFormat="1" ht="14.25" customHeight="1">
@@ -6490,20 +6509,20 @@
         <v>ID-55</v>
       </c>
       <c r="B75" s="117" t="s">
+        <v>210</v>
+      </c>
+      <c r="C75" s="117" t="s">
         <v>211</v>
       </c>
-      <c r="C75" s="117" t="s">
+      <c r="D75" s="117" t="s">
         <v>212</v>
-      </c>
-      <c r="D75" s="117" t="s">
-        <v>213</v>
       </c>
       <c r="E75" s="117"/>
       <c r="F75" s="117"/>
       <c r="G75" s="117"/>
       <c r="H75" s="117"/>
       <c r="I75" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="13.5" customHeight="1">
@@ -6512,20 +6531,20 @@
         <v>ID-56</v>
       </c>
       <c r="B76" s="117" t="s">
+        <v>213</v>
+      </c>
+      <c r="C76" s="117" t="s">
         <v>214</v>
       </c>
-      <c r="C76" s="117" t="s">
+      <c r="D76" s="117" t="s">
         <v>215</v>
-      </c>
-      <c r="D76" s="117" t="s">
-        <v>216</v>
       </c>
       <c r="E76" s="117"/>
       <c r="F76" s="117"/>
       <c r="G76" s="117"/>
       <c r="H76" s="117"/>
       <c r="I76" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="13.5" customHeight="1">
@@ -6534,20 +6553,20 @@
         <v>ID-57</v>
       </c>
       <c r="B77" s="117" t="s">
+        <v>216</v>
+      </c>
+      <c r="C77" s="117" t="s">
         <v>217</v>
       </c>
-      <c r="C77" s="117" t="s">
+      <c r="D77" s="117" t="s">
         <v>218</v>
-      </c>
-      <c r="D77" s="117" t="s">
-        <v>219</v>
       </c>
       <c r="E77" s="117"/>
       <c r="F77" s="117"/>
       <c r="G77" s="117"/>
       <c r="H77" s="117"/>
       <c r="I77" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="13.5" customHeight="1">
@@ -6556,20 +6575,20 @@
         <v>ID-58</v>
       </c>
       <c r="B78" s="117" t="s">
+        <v>219</v>
+      </c>
+      <c r="C78" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="C78" s="117" t="s">
+      <c r="D78" s="117" t="s">
         <v>221</v>
-      </c>
-      <c r="D78" s="117" t="s">
-        <v>222</v>
       </c>
       <c r="E78" s="117"/>
       <c r="F78" s="117"/>
       <c r="G78" s="117"/>
       <c r="H78" s="117"/>
       <c r="I78" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="13.5" customHeight="1">
@@ -6578,20 +6597,20 @@
         <v>ID-59</v>
       </c>
       <c r="B79" s="117" t="s">
+        <v>222</v>
+      </c>
+      <c r="C79" s="117" t="s">
         <v>223</v>
       </c>
-      <c r="C79" s="117" t="s">
+      <c r="D79" s="117" t="s">
         <v>224</v>
-      </c>
-      <c r="D79" s="117" t="s">
-        <v>225</v>
       </c>
       <c r="E79" s="117"/>
       <c r="F79" s="117"/>
       <c r="G79" s="117"/>
       <c r="H79" s="117"/>
       <c r="I79" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13.5" customHeight="1">
@@ -6600,20 +6619,20 @@
         <v>ID-60</v>
       </c>
       <c r="B80" s="117" t="s">
+        <v>225</v>
+      </c>
+      <c r="C80" s="117" t="s">
         <v>226</v>
       </c>
-      <c r="C80" s="117" t="s">
+      <c r="D80" s="117" t="s">
         <v>227</v>
-      </c>
-      <c r="D80" s="117" t="s">
-        <v>228</v>
       </c>
       <c r="E80" s="117"/>
       <c r="F80" s="117"/>
       <c r="G80" s="117"/>
       <c r="H80" s="117"/>
       <c r="I80" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="13.5" customHeight="1">
@@ -6622,20 +6641,20 @@
         <v>ID-61</v>
       </c>
       <c r="B81" s="117" t="s">
+        <v>228</v>
+      </c>
+      <c r="C81" s="117" t="s">
         <v>229</v>
       </c>
-      <c r="C81" s="117" t="s">
+      <c r="D81" s="117" t="s">
         <v>230</v>
-      </c>
-      <c r="D81" s="117" t="s">
-        <v>231</v>
       </c>
       <c r="E81" s="117"/>
       <c r="F81" s="117"/>
       <c r="G81" s="117"/>
       <c r="H81" s="117"/>
       <c r="I81" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="13.5" customHeight="1">
@@ -6644,20 +6663,20 @@
         <v>ID-62</v>
       </c>
       <c r="B82" s="117" t="s">
+        <v>231</v>
+      </c>
+      <c r="C82" s="117" t="s">
         <v>232</v>
       </c>
-      <c r="C82" s="117" t="s">
+      <c r="D82" s="117" t="s">
         <v>233</v>
-      </c>
-      <c r="D82" s="117" t="s">
-        <v>234</v>
       </c>
       <c r="E82" s="117"/>
       <c r="F82" s="117"/>
       <c r="G82" s="117"/>
       <c r="H82" s="117"/>
       <c r="I82" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -6706,7 +6725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -6744,7 +6763,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="212" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C2" s="212"/>
       <c r="D2" s="212"/>
@@ -6776,7 +6795,7 @@
         <v>179</v>
       </c>
       <c r="B4" s="213" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="213"/>
       <c r="D4" s="213"/>
@@ -6906,10 +6925,10 @@
         <v>186</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="117"/>
@@ -6926,10 +6945,10 @@
         <v>64</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D13" s="117" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E13" s="197"/>
       <c r="F13" s="117"/>
@@ -6946,10 +6965,10 @@
         <v>165</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D14" s="117" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E14" s="173"/>
       <c r="F14" s="117"/>
@@ -6966,10 +6985,10 @@
         <v>168</v>
       </c>
       <c r="C15" s="117" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D15" s="117" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E15" s="173"/>
       <c r="F15" s="117"/>
@@ -6986,10 +7005,10 @@
         <v>74</v>
       </c>
       <c r="C16" s="117" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D16" s="117" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E16" s="173"/>
       <c r="F16" s="117"/>
@@ -7006,10 +7025,10 @@
         <v>66</v>
       </c>
       <c r="C17" s="117" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D17" s="117" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E17" s="173"/>
       <c r="F17" s="117"/>
@@ -7026,10 +7045,10 @@
         <v>68</v>
       </c>
       <c r="C18" s="117" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D18" s="117" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E18" s="173"/>
       <c r="F18" s="117"/>
@@ -7046,10 +7065,10 @@
         <v>70</v>
       </c>
       <c r="C19" s="117" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D19" s="117" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E19" s="173"/>
       <c r="F19" s="117"/>
@@ -7066,10 +7085,10 @@
         <v>72</v>
       </c>
       <c r="C20" s="117" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D20" s="117" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E20" s="173"/>
       <c r="F20" s="117"/>
@@ -7081,7 +7100,7 @@
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
       <c r="A21" s="176"/>
       <c r="B21" s="177" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C21" s="176"/>
       <c r="D21" s="176"/>
@@ -7098,13 +7117,13 @@
         <v>[Mod_login-12]</v>
       </c>
       <c r="B22" s="117" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C22" s="117" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E22" s="179"/>
       <c r="F22" s="117"/>
@@ -7122,10 +7141,10 @@
         <v>188</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E23" s="179"/>
       <c r="F23" s="117"/>
@@ -7136,7 +7155,7 @@
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
       <c r="A24" s="176" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B24" s="58" t="s">
         <v>78</v>
@@ -7159,10 +7178,10 @@
         <v>79</v>
       </c>
       <c r="C25" s="91" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D25" s="91" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E25" s="179"/>
       <c r="F25" s="117"/>
@@ -7172,10 +7191,10 @@
     </row>
     <row r="26" spans="1:10" ht="13.5" customHeight="1">
       <c r="A26" s="176" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C26" s="176"/>
       <c r="D26" s="176"/>
@@ -7191,13 +7210,13 @@
         <v>[Mod_login-17]</v>
       </c>
       <c r="B27" s="117" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C27" s="117" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D27" s="117" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E27" s="173"/>
       <c r="F27" s="117"/>
@@ -7207,10 +7226,10 @@
     </row>
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
       <c r="A28" s="176" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>
@@ -7226,13 +7245,13 @@
         <v>[Mod_login-19]</v>
       </c>
       <c r="B29" s="117" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C29" s="117" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D29" s="117" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E29" s="173"/>
       <c r="F29" s="117"/>
@@ -7242,10 +7261,10 @@
     </row>
     <row r="30" spans="1:10" ht="13.5" customHeight="1">
       <c r="A30" s="176" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B30" s="58" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C30" s="176"/>
       <c r="D30" s="176"/>
@@ -7261,13 +7280,13 @@
         <v>[Mod_login-21]</v>
       </c>
       <c r="B31" s="117" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C31" s="117" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D31" s="117" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E31" s="173"/>
       <c r="F31" s="117"/>
@@ -7307,10 +7326,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -7379,7 +7398,7 @@
         <v>179</v>
       </c>
       <c r="B4" s="213" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="213"/>
       <c r="D4" s="213"/>
@@ -7421,7 +7440,7 @@
       </c>
       <c r="C6" s="101">
         <f>E6-D6-B6-A6</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D6" s="102">
         <f>COUNTIF(F11:G708,"N/A")</f>
@@ -7429,7 +7448,7 @@
       </c>
       <c r="E6" s="215">
         <f>COUNTA(A11:A265)*2</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F6" s="215"/>
       <c r="G6" s="215"/>
@@ -7512,7 +7531,7 @@
         <v>163</v>
       </c>
       <c r="D12" s="117" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E12" s="171"/>
       <c r="F12" s="117"/>
@@ -7535,7 +7554,7 @@
         <v>164</v>
       </c>
       <c r="E13" s="173" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F13" s="117"/>
       <c r="G13" s="117"/>
@@ -7557,7 +7576,7 @@
         <v>167</v>
       </c>
       <c r="E14" s="173" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F14" s="117"/>
       <c r="G14" s="117"/>
@@ -7579,7 +7598,7 @@
         <v>170</v>
       </c>
       <c r="E15" s="173" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F15" s="117"/>
       <c r="G15" s="117"/>
@@ -7601,7 +7620,7 @@
         <v>76</v>
       </c>
       <c r="E16" s="173" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F16" s="117"/>
       <c r="G16" s="117"/>
@@ -7623,7 +7642,7 @@
         <v>67</v>
       </c>
       <c r="E17" s="173" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F17" s="117"/>
       <c r="G17" s="117"/>
@@ -7645,7 +7664,7 @@
         <v>69</v>
       </c>
       <c r="E18" s="173" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F18" s="117"/>
       <c r="G18" s="117"/>
@@ -7667,7 +7686,7 @@
         <v>69</v>
       </c>
       <c r="E19" s="173" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F19" s="117"/>
       <c r="G19" s="117"/>
@@ -7689,7 +7708,7 @@
         <v>69</v>
       </c>
       <c r="E20" s="173" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F20" s="117"/>
       <c r="G20" s="117"/>
@@ -7723,10 +7742,10 @@
         <v>163</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E22" s="179" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F22" s="117"/>
       <c r="G22" s="117"/>
@@ -7743,13 +7762,13 @@
         <v>188</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E23" s="179" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F23" s="117"/>
       <c r="G23" s="117"/>
@@ -7777,16 +7796,16 @@
         <v>[Admin_login-15]</v>
       </c>
       <c r="B25" s="117" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C25" s="117" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D25" s="180" t="s">
         <v>189</v>
       </c>
       <c r="E25" s="179" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F25" s="117"/>
       <c r="G25" s="117"/>
@@ -7810,17 +7829,17 @@
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1">
       <c r="A27" s="165" t="str">
-        <f t="shared" ref="A27" si="3">IF(OR(B27&lt;&gt;"",D27&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <f t="shared" ref="A27:A29" si="3">IF(OR(B27&lt;&gt;"",D27&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
         <v>[Admin_login-17]</v>
       </c>
       <c r="B27" s="117" t="s">
+        <v>380</v>
+      </c>
+      <c r="C27" s="117" t="s">
+        <v>381</v>
+      </c>
+      <c r="D27" s="180" t="s">
         <v>382</v>
-      </c>
-      <c r="C27" s="117" t="s">
-        <v>380</v>
-      </c>
-      <c r="D27" s="180" t="s">
-        <v>190</v>
       </c>
       <c r="E27" s="179"/>
       <c r="F27" s="117"/>
@@ -7830,9 +7849,11 @@
       <c r="J27" s="105"/>
     </row>
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A28" s="176"/>
+      <c r="A28" s="176" t="s">
+        <v>264</v>
+      </c>
       <c r="B28" s="177" t="s">
-        <v>284</v>
+        <v>385</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>
@@ -7841,6 +7862,26 @@
       <c r="G28" s="176"/>
       <c r="H28" s="176"/>
       <c r="I28" s="178"/>
+    </row>
+    <row r="29" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A29" s="165" t="str">
+        <f t="shared" si="3"/>
+        <v>[Admin_login-19]</v>
+      </c>
+      <c r="B29" s="117" t="s">
+        <v>386</v>
+      </c>
+      <c r="C29" s="117" t="s">
+        <v>383</v>
+      </c>
+      <c r="D29" s="180" t="s">
+        <v>384</v>
+      </c>
+      <c r="E29" s="179"/>
+      <c r="F29" s="117"/>
+      <c r="G29" s="117"/>
+      <c r="H29" s="174"/>
+      <c r="I29" s="175"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -7871,4 +7912,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
delete common testcase, update integration testcase
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
+++ b/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="700" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="543" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -1414,13 +1414,6 @@
     <t>Vietnamese Medicinal Plants Network</t>
   </si>
   <si>
-    <t>List enviroment requires in this system
-1. Server: 
-2. Database server: MySQL server
-3. Browser: Google Chrome 40, Mozzila Firefox 30
-4. Operation System: Mac OS X</t>
-  </si>
-  <si>
     <t>Medicinal Plant</t>
   </si>
   <si>
@@ -1893,6 +1886,13 @@
   </si>
   <si>
     <t>Check New register of Herb Medicine Store tap</t>
+  </si>
+  <si>
+    <t>List enviroment requires in this system
+1. Server: Ubuntu 14.03
+2. Database server: MySQL server
+3. Browser: Google Chrome 40, Mozzila Firefox 30
+4. Operation System: Mac OS X</t>
   </si>
 </sst>
 </file>
@@ -4175,8 +4175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="C5" s="204"/>
       <c r="D5" s="205" t="s">
-        <v>313</v>
+        <v>386</v>
       </c>
       <c r="E5" s="205"/>
       <c r="F5" s="205"/>
@@ -4273,13 +4273,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D9" s="149" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="114" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F9" s="113" t="s">
         <v>90</v>
@@ -4561,7 +4561,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="149" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D11" s="76">
         <f>User_Function!A6</f>
@@ -4590,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="199" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D12" s="76">
         <f>Mod_Function!A6</f>
@@ -5395,7 +5395,7 @@
         <v>295</v>
       </c>
       <c r="D16" s="124" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E16" s="125"/>
       <c r="F16" s="117"/>
@@ -5416,7 +5416,7 @@
         <v>293</v>
       </c>
       <c r="D17" s="124" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E17" s="125"/>
       <c r="F17" s="117"/>
@@ -5437,7 +5437,7 @@
         <v>294</v>
       </c>
       <c r="D18" s="124" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E18" s="125"/>
       <c r="F18" s="117"/>
@@ -5532,7 +5532,7 @@
         <v>297</v>
       </c>
       <c r="D23" s="91" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E23" s="91"/>
       <c r="F23" s="117"/>
@@ -5553,7 +5553,7 @@
         <v>296</v>
       </c>
       <c r="D24" s="91" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E24" s="91" t="s">
         <v>81</v>
@@ -5587,10 +5587,10 @@
         <v>252</v>
       </c>
       <c r="C26" s="91" t="s">
+        <v>338</v>
+      </c>
+      <c r="D26" s="136" t="s">
         <v>339</v>
-      </c>
-      <c r="D26" s="136" t="s">
-        <v>340</v>
       </c>
       <c r="E26" s="91" t="s">
         <v>83</v>
@@ -5610,10 +5610,10 @@
         <v>87</v>
       </c>
       <c r="C27" s="91" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D27" s="91" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E27" s="91" t="s">
         <v>81</v>
@@ -5650,7 +5650,7 @@
         <v>253</v>
       </c>
       <c r="D29" s="104" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E29" s="104" t="s">
         <v>88</v>
@@ -5673,7 +5673,7 @@
         <v>254</v>
       </c>
       <c r="D30" s="104" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E30" s="104" t="s">
         <v>88</v>
@@ -5709,10 +5709,10 @@
         <v>261</v>
       </c>
       <c r="C32" s="106" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D32" s="104" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E32" s="104"/>
       <c r="F32" s="117"/>
@@ -5730,10 +5730,10 @@
         <v>262</v>
       </c>
       <c r="C33" s="106" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D33" s="104" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E33" s="104"/>
       <c r="F33" s="117"/>
@@ -5767,10 +5767,10 @@
         <v>263</v>
       </c>
       <c r="C35" s="106" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D35" s="104" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E35" s="104"/>
       <c r="F35" s="117"/>
@@ -5805,7 +5805,7 @@
         <v>298</v>
       </c>
       <c r="D37" s="117" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E37" s="118"/>
       <c r="F37" s="117"/>
@@ -5826,7 +5826,7 @@
         <v>259</v>
       </c>
       <c r="D38" s="117" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E38" s="118"/>
       <c r="F38" s="117"/>
@@ -5857,7 +5857,7 @@
         <v>[User_login-30]</v>
       </c>
       <c r="B40" s="117" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C40" s="117" t="s">
         <v>289</v>
@@ -5894,7 +5894,7 @@
         <v>[User_login-32]</v>
       </c>
       <c r="B42" s="117" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C42" s="117" t="s">
         <v>290</v>
@@ -5931,7 +5931,7 @@
         <v>[User_login-34]</v>
       </c>
       <c r="B44" s="117" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C44" s="117" t="s">
         <v>291</v>
@@ -5951,7 +5951,7 @@
         <v>264</v>
       </c>
       <c r="B45" s="169" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C45" s="166"/>
       <c r="D45" s="166"/>
@@ -5968,13 +5968,13 @@
         <v>[User_login-36]</v>
       </c>
       <c r="B46" s="117" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C46" s="117" t="s">
         <v>301</v>
       </c>
       <c r="D46" s="117" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E46" s="118"/>
       <c r="F46" s="117"/>
@@ -5988,7 +5988,7 @@
         <v>264</v>
       </c>
       <c r="B47" s="169" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C47" s="166"/>
       <c r="D47" s="166"/>
@@ -6005,13 +6005,13 @@
         <v>[User_login-38]</v>
       </c>
       <c r="B48" s="117" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C48" s="117" t="s">
         <v>302</v>
       </c>
       <c r="D48" s="117" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E48" s="118"/>
       <c r="F48" s="117"/>
@@ -6042,13 +6042,13 @@
         <v>[User_login-40]</v>
       </c>
       <c r="B50" s="117" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C50" s="117" t="s">
         <v>309</v>
       </c>
       <c r="D50" s="117" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E50" s="118"/>
       <c r="F50" s="117"/>
@@ -6079,7 +6079,7 @@
         <v>[User_login-42]</v>
       </c>
       <c r="B52" s="117" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C52" s="117" t="s">
         <v>303</v>
@@ -6116,13 +6116,13 @@
         <v>[User_login-44]</v>
       </c>
       <c r="B54" s="117" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C54" s="117" t="s">
         <v>310</v>
       </c>
       <c r="D54" s="117" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E54" s="118"/>
       <c r="F54" s="117"/>
@@ -6151,13 +6151,13 @@
         <v>[User_login-46]</v>
       </c>
       <c r="B56" s="117" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C56" s="117" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D56" s="117" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E56" s="118"/>
       <c r="F56" s="117"/>
@@ -6186,13 +6186,13 @@
         <v>[User_login-48]</v>
       </c>
       <c r="B58" s="117" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C58" s="117" t="s">
         <v>311</v>
       </c>
       <c r="D58" s="117" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E58" s="118"/>
       <c r="F58" s="117"/>
@@ -6276,10 +6276,10 @@
         <v>ID-45</v>
       </c>
       <c r="B64" s="117" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C64" s="117" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D64" s="117" t="s">
         <v>196</v>
@@ -6298,10 +6298,10 @@
         <v>ID-46</v>
       </c>
       <c r="B65" s="117" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C65" s="117" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D65" s="117" t="s">
         <v>196</v>
@@ -6320,10 +6320,10 @@
         <v>ID-47</v>
       </c>
       <c r="B66" s="117" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C66" s="117" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D66" s="117" t="s">
         <v>196</v>
@@ -6345,7 +6345,7 @@
         <v>234</v>
       </c>
       <c r="C67" s="117" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D67" s="117" t="s">
         <v>196</v>
@@ -6367,7 +6367,7 @@
         <v>235</v>
       </c>
       <c r="C68" s="117" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D68" s="117" t="s">
         <v>196</v>
@@ -6925,7 +6925,7 @@
         <v>186</v>
       </c>
       <c r="C12" s="117" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D12" s="117" t="s">
         <v>268</v>
@@ -6945,7 +6945,7 @@
         <v>64</v>
       </c>
       <c r="C13" s="117" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D13" s="117" t="s">
         <v>269</v>
@@ -6965,7 +6965,7 @@
         <v>165</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D14" s="117" t="s">
         <v>270</v>
@@ -6985,7 +6985,7 @@
         <v>168</v>
       </c>
       <c r="C15" s="117" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D15" s="117" t="s">
         <v>271</v>
@@ -7005,7 +7005,7 @@
         <v>74</v>
       </c>
       <c r="C16" s="117" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D16" s="117" t="s">
         <v>272</v>
@@ -7025,7 +7025,7 @@
         <v>66</v>
       </c>
       <c r="C17" s="117" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D17" s="117" t="s">
         <v>274</v>
@@ -7045,7 +7045,7 @@
         <v>68</v>
       </c>
       <c r="C18" s="117" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D18" s="117" t="s">
         <v>273</v>
@@ -7065,7 +7065,7 @@
         <v>70</v>
       </c>
       <c r="C19" s="117" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D19" s="117" t="s">
         <v>273</v>
@@ -7085,7 +7085,7 @@
         <v>72</v>
       </c>
       <c r="C20" s="117" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D20" s="117" t="s">
         <v>273</v>
@@ -7120,10 +7120,10 @@
         <v>258</v>
       </c>
       <c r="C22" s="117" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E22" s="179"/>
       <c r="F22" s="117"/>
@@ -7141,7 +7141,7 @@
         <v>188</v>
       </c>
       <c r="C23" s="117" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D23" s="180" t="s">
         <v>255</v>
@@ -7181,7 +7181,7 @@
         <v>266</v>
       </c>
       <c r="D25" s="91" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E25" s="179"/>
       <c r="F25" s="117"/>
@@ -7213,7 +7213,7 @@
         <v>267</v>
       </c>
       <c r="C27" s="117" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D27" s="117" t="s">
         <v>275</v>
@@ -7248,7 +7248,7 @@
         <v>281</v>
       </c>
       <c r="C29" s="117" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D29" s="117" t="s">
         <v>276</v>
@@ -7283,7 +7283,7 @@
         <v>280</v>
       </c>
       <c r="C31" s="117" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D31" s="117" t="s">
         <v>282</v>
@@ -7328,7 +7328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -7742,7 +7742,7 @@
         <v>163</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E22" s="179" t="s">
         <v>241</v>
@@ -7762,10 +7762,10 @@
         <v>188</v>
       </c>
       <c r="C23" s="117" t="s">
+        <v>375</v>
+      </c>
+      <c r="D23" s="180" t="s">
         <v>376</v>
-      </c>
-      <c r="D23" s="180" t="s">
-        <v>377</v>
       </c>
       <c r="E23" s="179" t="s">
         <v>241</v>
@@ -7796,10 +7796,10 @@
         <v>[Admin_login-15]</v>
       </c>
       <c r="B25" s="117" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C25" s="117" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D25" s="180" t="s">
         <v>189</v>
@@ -7833,13 +7833,13 @@
         <v>[Admin_login-17]</v>
       </c>
       <c r="B27" s="117" t="s">
+        <v>379</v>
+      </c>
+      <c r="C27" s="117" t="s">
         <v>380</v>
       </c>
-      <c r="C27" s="117" t="s">
+      <c r="D27" s="180" t="s">
         <v>381</v>
-      </c>
-      <c r="D27" s="180" t="s">
-        <v>382</v>
       </c>
       <c r="E27" s="179"/>
       <c r="F27" s="117"/>
@@ -7853,7 +7853,7 @@
         <v>264</v>
       </c>
       <c r="B28" s="177" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C28" s="176"/>
       <c r="D28" s="176"/>
@@ -7869,13 +7869,13 @@
         <v>[Admin_login-19]</v>
       </c>
       <c r="B29" s="117" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C29" s="117" t="s">
+        <v>382</v>
+      </c>
+      <c r="D29" s="180" t="s">
         <v>383</v>
-      </c>
-      <c r="D29" s="180" t="s">
-        <v>384</v>
       </c>
       <c r="E29" s="179"/>
       <c r="F29" s="117"/>

</xml_diff>

<commit_message>
- Update CMN plant
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
+++ b/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="315">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -432,12 +432,6 @@
   </si>
   <si>
     <t>Check user logout when user logout with "Logout" link</t>
-  </si>
-  <si>
-    <t>Forgot Password</t>
-  </si>
-  <si>
-    <t>When user login with new password</t>
   </si>
   <si>
     <t>Execute all Registered User unit test cases and passed</t>
@@ -637,18 +631,6 @@
     <t>MS31</t>
   </si>
   <si>
-    <t>Integration Login with Message</t>
-  </si>
-  <si>
-    <t>1. Enter the admin page</t>
-  </si>
-  <si>
-    <t>Admin Dashboard module</t>
-  </si>
-  <si>
-    <t>User Management module</t>
-  </si>
-  <si>
     <t>Back to Check Report</t>
   </si>
   <si>
@@ -677,19 +659,6 @@
   </si>
   <si>
     <t>Check date</t>
-  </si>
-  <si>
-    <t>Check Logout button</t>
-  </si>
-  <si>
-    <t>1. Admin Page is displayed
-2. Content about dashboard is displayed</t>
-  </si>
-  <si>
-    <t>Check clicking on link on Home page screen</t>
-  </si>
-  <si>
-    <t>Common</t>
   </si>
   <si>
     <t>Security</t>
@@ -844,12 +813,6 @@
     <t>Color of all tabs selection is the same</t>
   </si>
   <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>Account</t>
-  </si>
-  <si>
     <t>1. Set language of Browser isVietnamese
 2. Start system from browser
 3. Confirm displaying language of system</t>
@@ -861,9 +824,6 @@
     <t xml:space="preserve">Display Homepage with name and avatar of user </t>
   </si>
   <si>
-    <t>[Admin_login-7]</t>
-  </si>
-  <si>
     <t>DangNHSE02992</t>
   </si>
   <si>
@@ -873,40 +833,10 @@
     <t>VMN</t>
   </si>
   <si>
-    <t>When user forgot password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Log in Page is displayed
-</t>
-  </si>
-  <si>
     <t>Mod_login</t>
   </si>
   <si>
-    <t>Check mod view</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Login successfully
-2. Click on avatar at right side screen
-3. Click on Logout button </t>
-  </si>
-  <si>
-    <t>Integration Login with Posted Article</t>
-  </si>
-  <si>
-    <t>Test "Message list"</t>
-  </si>
-  <si>
-    <t>Test "Message detail"</t>
-  </si>
-  <si>
-    <t>Check "Image" of posted article</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Mod Common module</t>
   </si>
   <si>
     <t>1. Login the system with Mod role.
@@ -958,75 +888,7 @@
 + Posted date</t>
   </si>
   <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Home button</t>
-  </si>
-  <si>
-    <t>Integration Personal page with notification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on "Avatar" in menu bar
-6. Click on "medicinal plants" link </t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on "Avatar" in menu bar
-6. Click on "remedy" link</t>
-  </si>
-  <si>
-    <t>Check "log out"  when user login successfully</t>
-  </si>
-  <si>
-    <t>Integration Medicinal plants with author</t>
-  </si>
-  <si>
     <t>Integration Remedy with HMS</t>
-  </si>
-  <si>
-    <t>Integration Remedy with author</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on "Avatar" in menu bar
-6. Click "Notification" list in personal page</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on "Medicinal Plants" in menu bar
-6. Click on a "medicinal plants" picture of medicinal plants page
-7. Click on "author" link of "medicinal plants detail" page</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on "Remedy" in menu bar
-6. Click on a "Remedy" picture of remedy page
-7. Click on "author" of remedy detail page</t>
   </si>
   <si>
     <t>Vietnamese Medicinal Plants Network</t>
@@ -1069,13 +931,6 @@
 5. Paste link and press Enter</t>
   </si>
   <si>
-    <t>1. Login on one browser
-2. Click Account
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
     <t>User function</t>
   </si>
   <si>
@@ -1088,209 +943,15 @@
     <t>Mod_Function</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Mod Page is displayed with the following list:
-- Header
-- Right Side bar:
-+ Logout button
-- Content details left
-+ Dashboard (default)
-+ Medicinal plant management
-+ Remedy management 
-</t>
-  </si>
-  <si>
     <t>Check "Medicinal plants" tab</t>
   </si>
   <si>
     <t>Check "HMS" tab</t>
-  </si>
-  <si>
-    <t>Integration Personal page with related remedy</t>
-  </si>
-  <si>
-    <t>Integration Personal page with related medicinal plants</t>
-  </si>
-  <si>
-    <t>Check "Notification" tab</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on Avatar menu
-6. Click on Account button
-7. Show message tab</t>
-  </si>
-  <si>
-    <t>Check "remedy" tab</t>
-  </si>
-  <si>
-    <t>Check "Author" tab</t>
-  </si>
-  <si>
-    <t>1. Homepage is displayed 
-2. Reload homepage, homepage is displayed</t>
-  </si>
-  <si>
-    <t>1. Enter the website
-2. Click on Login button in header
-3. Click on "Forgot password" link
-4. Input "dangnh@fpt.edu.vn"
-5. Click "send" button</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. Login page is displayed
-3. Forgot password form is displayed
-4. Email textarea is displayed
-5. Change password page is sent to email "dangnh@fpt.edu.vn"</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button in header
-3. Input: 
-Email: "dangnhse02992@fpt.edu.vn"
-Password: Enter new password (which has been changed in change password page)
-4. Click "Sign in" button of login page</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on Avatar menu
-6. Click on Account button
-7. Click message tab
-8. Click a message of message tab</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on Avatar menu
-6. Click on Account button
-7. Click on Image of posted article tab</t>
-  </si>
-  <si>
-    <t>1. Enter the website: thuocnam.com
-2. Click on Login button
-3. Input:
-+ Email: "dangnhse02992@fpt.edu.vn"
-+ Password: "123456789"
-4. Click on "sign in" button of login page or press enter
-5. Click on "Remedy" in menu bar
-6. Click on a "Remedy" picture of remedy page
-7. Click on "related HMS" of remedy detail page</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Email and password textarea are displayed
-4. Logged in successfully
-5. The "medicinal plants" page is displayed
-6. "Medicinal plants detail" page is displayed
-7. "Author" is displayed</t>
-  </si>
-  <si>
-    <t>1. The Homepage is displayed 
-2. The log in page is displayed
-3. Email and password textarea are displayed
-4. Logged in successfully
-5. The "remedy" page is displayed
-6. "Remedy detail" page is displayed
-7. "Related HMS" is displayed</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Email and password textarea are displayed
-4. Logged in successfully
-5. The "remedy" page is displayed
-6. "Remedy detail" page is displayed
-7. "Author" is displayed</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Email and password textarea are displayed
-4. Logged in successfully
-5. The "personal" page is displayed
-6. "Notification" list is displayed</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Email and password textarea are displayed
-4. Logged in successfully
-5. The "personal" page is displayed
-6. "Remedy detail" page is displayed</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Email and password textarea are displayed
-4. Logged in successfully
-5. The "personal" page is displayed
-6. "Medicinal plants detail" page is displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Homepage and avatar is displayed 
-2. Log out successfully
-3. Homepage is displayed </t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. Login page is displayed
-3. Email and password textarea ara displayed
-4. Log in successfully</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Email, password text area are displayed
-4. Logged in successfully
-5. Avatar logo is displayed
-6. The Account page is displayed
-7. Message is displayed</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Email, password text area are displayed
-4. Logged in successfully
-5. Avatar logo is displayed
-6. The Account page is displayed
-7. Message is displayed
-8. Message detail is displayed</t>
-  </si>
-  <si>
-    <t>1.The Homepage is displayed 
-2. The log in page is displayed
-3. Email, password text area are displayed
-4. Logged in successfully
-5. Avatar logo is displayed
-6. The Account page is displayed
-7. Posted article is displayed</t>
   </si>
   <si>
     <t>1. The Homepage is displayed
 2. Avatar menu is showed
 3. Logout user and redirect to homepage as guest rule</t>
-  </si>
-  <si>
-    <t>1. Enter mod page</t>
-  </si>
-  <si>
-    <t>1. Enter mod page
-2. Click logout button in Right Slide bar</t>
   </si>
   <si>
     <t>1. Enter mod page
@@ -1308,62 +969,6 @@
 2. Input username "email0@gmail.com" password "123456"
 3. Click "Login" button
 4. Click remedy management tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Admin Page is displayed with the following list:
-- Header
-- Right Side bar:
-+ Logout button
-- Content details left
-+ Dashboard (default)
-+ User management
-+ New herb medicine store resgister 
-</t>
-  </si>
-  <si>
-    <t>1. Enter the admin page
-2. Input correct account and password as admin rule
-3. Click logout button in Right Slide bar</t>
-  </si>
-  <si>
-    <t>1. Log in Page is displayed
-2. Login successful as admin rule
-3. Login page is displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Enter the admin page
-2. Click Dashboard tab in Left Slide bar
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click Dashboard tab </t>
-  </si>
-  <si>
-    <t>Check User Management tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Enter the admin page
-2. Click User Management tab in Left Slide bar
-</t>
-  </si>
-  <si>
-    <t>1. Admin Page is displayed
-2. User Information Management page is displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Enter the admin page
-2. Click New Herb Medicine Store tab in Left Slide bar
-</t>
-  </si>
-  <si>
-    <t>1. Admin Page is displayed
-2. New register of herb medicine store information page is displayed</t>
-  </si>
-  <si>
-    <t>New register of herb medicine store</t>
-  </si>
-  <si>
-    <t>Check New register of Herb Medicine Store tap</t>
   </si>
   <si>
     <t>List enviroment requires in this system
@@ -1525,21 +1130,6 @@
   </si>
   <si>
     <t>Check "Related Remedy Article" hyperlink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Login VMN system by Member or Mod role
-2. Click on "Medicinal Plants" on Header
-3. Click on "Detail" hyperlink of any Medicinal Plants Article
-4. Click on "Related Remedy Article" tab
-5. Click on any Remedy Article hyperlink </t>
-  </si>
-  <si>
-    <t>1. Homepage is displayed 
-2. "Medicinal Plants" tab is displayed 
-3. "Medicinal Plants Article Detail" Page is displayed 
-4. The "medicinal plants" page is displayed
-5. "Medicinal plants detail" page is displayed
-6. "Relational remedy" is displayed</t>
   </si>
   <si>
     <t>1. Homepage is displayed 
@@ -1716,36 +1306,77 @@
     <t>Personal Page</t>
   </si>
   <si>
-    <t xml:space="preserve">Integration Log in with </t>
-  </si>
-  <si>
-    <t>Check Dashboard tab</t>
-  </si>
-  <si>
-    <t>1. Login Admin Page by Admin role
-2. Click on Dashboard tab</t>
+    <t>Integration Login with Dashboard</t>
+  </si>
+  <si>
+    <t>Integration Login with Medicinal Plants Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login VMN system by Mod role.
+</t>
+  </si>
+  <si>
+    <t>When Mod click on "Logout" hyperlink</t>
+  </si>
+  <si>
+    <t>1. Login VMN system by Admin role
+2. Click on "Dashboard" hyperlink</t>
   </si>
   <si>
     <t>1. Admin Page is displayed 
-2. Dashboard tab is displayed</t>
-  </si>
-  <si>
-    <t>Integration Login with Dashboard</t>
-  </si>
-  <si>
-    <t>Integration Login with Medicinal Plants Management</t>
-  </si>
-  <si>
-    <t>Integration Login with Remedy Management</t>
-  </si>
-  <si>
-    <t>Check Medicinal Plants Management tab</t>
-  </si>
-  <si>
-    <t>Check Remedy Management</t>
-  </si>
-  <si>
-    <t>Integration Medicinal Plants Management with Medicinal Plants Article Detail</t>
+2. "Dashboard" Page is displayed</t>
+  </si>
+  <si>
+    <t>[Admin module-20]</t>
+  </si>
+  <si>
+    <t>Integration Login with User Management</t>
+  </si>
+  <si>
+    <t>Check "User Management" Page</t>
+  </si>
+  <si>
+    <t>Check "Dashboard" Page</t>
+  </si>
+  <si>
+    <t>1. Login VMN system by Admin role
+2. Click on "User Management" hyperlink</t>
+  </si>
+  <si>
+    <t>1. Admin Page is displayed 
+2. "User Management" Page is displayed</t>
+  </si>
+  <si>
+    <t>[Admin module-27]</t>
+  </si>
+  <si>
+    <t>Integration Login with Waiting HMS Approval</t>
+  </si>
+  <si>
+    <t>Check "Waiting HMS Approval" Page</t>
+  </si>
+  <si>
+    <t>1. Login VMN system by Admin role
+2. Click on "Waiting HMS Approval" hyperlink</t>
+  </si>
+  <si>
+    <t>1. Admin Page is displayed
+2. "Waiting HMS Approval" Page is displayed</t>
+  </si>
+  <si>
+    <t>[Admin module-35]</t>
+  </si>
+  <si>
+    <t>When Admin click on "Logout" hyperlink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login VMN system by Admin role.
+2. Click on "Logout" hyperlink on Header
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login VMN system by Admin role.
+</t>
   </si>
 </sst>
 </file>
@@ -2047,7 +1678,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -2673,13 +2304,26 @@
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="8"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -2689,10 +2333,10 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
         <color auto="1"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -2764,7 +2408,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3285,6 +2929,41 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="41" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="43" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="44" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="37" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="47" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="47" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3334,46 +3013,37 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="43" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="44" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="6" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="37" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="47" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="48" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="48" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="49" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="49" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="48" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="41" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -3506,14 +3176,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3912,13 +3582,13 @@
     <row r="2" spans="1:7" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="195" t="s">
+      <c r="C2" s="208" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+      <c r="G2" s="208"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="6"/>
@@ -3929,44 +3599,44 @@
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="196" t="s">
-        <v>226</v>
-      </c>
-      <c r="D4" s="196"/>
-      <c r="E4" s="196"/>
+      <c r="C4" s="209" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="209"/>
+      <c r="E4" s="209"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="196" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5" s="196"/>
-      <c r="E5" s="196"/>
+      <c r="C5" s="209" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="209"/>
+      <c r="E5" s="209"/>
       <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="197" t="s">
+      <c r="B6" s="210" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="198" t="str">
+      <c r="C6" s="211" t="str">
         <f>C5&amp;"_"&amp;"Integration Test Case"&amp;"_"&amp;"v1.0"</f>
         <v>VMN_Integration Test Case_v1.0</v>
       </c>
-      <c r="D6" s="198"/>
-      <c r="E6" s="198"/>
+      <c r="D6" s="211"/>
+      <c r="E6" s="211"/>
       <c r="F6" s="9" t="s">
         <v>6</v>
       </c>
@@ -3975,10 +3645,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B7" s="197"/>
-      <c r="C7" s="198"/>
-      <c r="D7" s="198"/>
-      <c r="E7" s="198"/>
+      <c r="B7" s="210"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
       <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
@@ -4038,7 +3708,7 @@
         <v>54</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="19" customFormat="1" ht="21.75" customHeight="1">
@@ -4145,39 +3815,39 @@
       <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="201" t="s">
+      <c r="B3" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="201"/>
-      <c r="D3" s="202" t="str">
+      <c r="C3" s="214"/>
+      <c r="D3" s="215" t="str">
         <f>Cover!C4</f>
         <v>Vietnamese Medicinal Plants Network</v>
       </c>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="201" t="s">
+      <c r="B4" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="201"/>
-      <c r="D4" s="202" t="str">
+      <c r="C4" s="214"/>
+      <c r="D4" s="215" t="str">
         <f>Cover!C5</f>
         <v>VMN</v>
       </c>
-      <c r="E4" s="202"/>
-      <c r="F4" s="202"/>
+      <c r="E4" s="215"/>
+      <c r="F4" s="215"/>
     </row>
     <row r="5" spans="2:6" s="35" customFormat="1" ht="72" customHeight="1">
-      <c r="B5" s="199" t="s">
+      <c r="B5" s="212" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="199"/>
-      <c r="D5" s="200" t="s">
-        <v>284</v>
-      </c>
-      <c r="E5" s="200"/>
-      <c r="F5" s="200"/>
+      <c r="C5" s="212"/>
+      <c r="D5" s="213" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" s="213"/>
+      <c r="F5" s="213"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="36"/>
@@ -4215,16 +3885,16 @@
         <v>1</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="D9" s="142" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="113" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="F9" s="112" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="25.5">
@@ -4232,16 +3902,16 @@
         <v>2</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>285</v>
+        <v>213</v>
       </c>
       <c r="D10" s="189" t="s">
-        <v>286</v>
+        <v>214</v>
       </c>
       <c r="E10" s="113" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="112" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="25.5">
@@ -4258,7 +3928,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="112" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="13.5">
@@ -4371,15 +4041,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B1" s="205" t="s">
+      <c r="B1" s="218" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="205"/>
-      <c r="D1" s="205"/>
-      <c r="E1" s="205"/>
-      <c r="F1" s="205"/>
-      <c r="G1" s="205"/>
-      <c r="H1" s="205"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="61"/>
@@ -4395,17 +4065,17 @@
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="202" t="str">
+      <c r="C3" s="215" t="str">
         <f>Cover!C4</f>
         <v>Vietnamese Medicinal Plants Network</v>
       </c>
-      <c r="D3" s="202"/>
-      <c r="E3" s="203" t="s">
+      <c r="D3" s="215"/>
+      <c r="E3" s="216" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="203"/>
+      <c r="F3" s="216"/>
       <c r="G3" s="10" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="H3" s="64"/>
     </row>
@@ -4413,17 +4083,17 @@
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="202" t="str">
+      <c r="C4" s="215" t="str">
         <f>Cover!C5</f>
         <v>VMN</v>
       </c>
-      <c r="D4" s="202"/>
-      <c r="E4" s="203" t="s">
+      <c r="D4" s="215"/>
+      <c r="E4" s="216" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="203"/>
+      <c r="F4" s="216"/>
       <c r="G4" s="10" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="H4" s="64"/>
     </row>
@@ -4431,15 +4101,15 @@
       <c r="B5" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="202" t="str">
+      <c r="C5" s="215" t="str">
         <f>C4&amp;"_"&amp;"Integration Test Report"&amp;"_"&amp;"v1.0"</f>
         <v>VMN_Integration Test Report_v1.0</v>
       </c>
-      <c r="D5" s="202"/>
-      <c r="E5" s="203" t="s">
+      <c r="D5" s="215"/>
+      <c r="E5" s="216" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="203"/>
+      <c r="F5" s="216"/>
       <c r="G5" s="114"/>
       <c r="H5" s="66"/>
     </row>
@@ -4448,12 +4118,12 @@
       <c r="B6" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="204"/>
-      <c r="D6" s="204"/>
-      <c r="E6" s="204"/>
-      <c r="F6" s="204"/>
-      <c r="G6" s="204"/>
-      <c r="H6" s="204"/>
+      <c r="C6" s="217"/>
+      <c r="D6" s="217"/>
+      <c r="E6" s="217"/>
+      <c r="F6" s="217"/>
+      <c r="G6" s="217"/>
+      <c r="H6" s="217"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
       <c r="A7" s="61"/>
@@ -4514,7 +4184,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="142" t="s">
-        <v>237</v>
+        <v>204</v>
       </c>
       <c r="D11" s="75">
         <f>'User Module'!A6</f>
@@ -4543,7 +4213,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="189" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="D12" s="75">
         <f>'Mod Module'!A6</f>
@@ -4555,7 +4225,7 @@
       </c>
       <c r="F12" s="75">
         <f>'Mod Module'!C6</f>
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G12" s="75">
         <f>'Mod Module'!D6</f>
@@ -4563,7 +4233,7 @@
       </c>
       <c r="H12" s="76">
         <f>'Mod Module'!E6</f>
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4584,7 +4254,7 @@
       </c>
       <c r="F13" s="75">
         <f>'Admin Module'!C6</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G13" s="75">
         <f>'Admin Module'!D6</f>
@@ -4592,7 +4262,7 @@
       </c>
       <c r="H13" s="76">
         <f>'Admin Module'!E6</f>
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4611,7 +4281,7 @@
       </c>
       <c r="F14" s="78">
         <f>SUM(F11:F13)</f>
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="G14" s="78">
         <f>SUM(G9:G13)</f>
@@ -4619,7 +4289,7 @@
       </c>
       <c r="H14" s="79">
         <f>SUM(H11:H13)</f>
-        <v>98</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -4706,7 +4376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -4719,11 +4389,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A1" s="206" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="206"/>
-      <c r="C1" s="206"/>
+      <c r="A1" s="219" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="219"/>
+      <c r="C1" s="219"/>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" thickBot="1"/>
     <row r="3" spans="1:3" ht="15">
@@ -4731,279 +4401,279 @@
         <v>16</v>
       </c>
       <c r="B3" s="149" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3" s="150" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15">
       <c r="A4" s="151" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="152" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="152"/>
     </row>
     <row r="5" spans="1:3" ht="15">
       <c r="A5" s="151" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="152" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C5" s="152"/>
     </row>
     <row r="6" spans="1:3" ht="15">
       <c r="A6" s="151" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="152" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="152"/>
     </row>
     <row r="7" spans="1:3" ht="15">
       <c r="A7" s="151" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="152" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" s="152"/>
     </row>
     <row r="8" spans="1:3" ht="15">
       <c r="A8" s="151" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="152" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C8" s="152"/>
     </row>
     <row r="9" spans="1:3" ht="15">
       <c r="A9" s="151" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="152" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C9" s="152"/>
     </row>
     <row r="10" spans="1:3" ht="15">
       <c r="A10" s="151" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="152" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C10" s="152"/>
     </row>
     <row r="11" spans="1:3" ht="15">
       <c r="A11" s="151" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="152" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" s="152"/>
     </row>
     <row r="12" spans="1:3" ht="15">
       <c r="A12" s="151" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" s="152" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C12" s="152"/>
     </row>
     <row r="13" spans="1:3" ht="15">
       <c r="A13" s="151" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" s="152" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C13" s="152"/>
     </row>
     <row r="14" spans="1:3" ht="15">
       <c r="A14" s="151" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B14" s="153" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14" s="152"/>
     </row>
     <row r="15" spans="1:3" ht="15">
       <c r="A15" s="151" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B15" s="152" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C15" s="152"/>
     </row>
     <row r="16" spans="1:3" ht="15">
       <c r="A16" s="151" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16" s="152" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" s="152"/>
     </row>
     <row r="17" spans="1:3" ht="15">
       <c r="A17" s="151" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B17" s="152" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C17" s="152"/>
     </row>
     <row r="18" spans="1:3" ht="15">
       <c r="A18" s="151" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B18" s="152" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C18" s="152"/>
     </row>
     <row r="19" spans="1:3" ht="15">
       <c r="A19" s="151" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B19" s="153" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C19" s="152"/>
     </row>
     <row r="20" spans="1:3" ht="15">
       <c r="A20" s="151" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" s="153" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="152"/>
     </row>
     <row r="21" spans="1:3" ht="15">
       <c r="A21" s="151" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B21" s="153" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C21" s="152"/>
     </row>
     <row r="22" spans="1:3" ht="60">
       <c r="A22" s="151" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B22" s="154" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C22" s="152"/>
     </row>
     <row r="23" spans="1:3" ht="15">
       <c r="A23" s="151" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" s="152" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C23" s="152"/>
     </row>
     <row r="24" spans="1:3" ht="15">
       <c r="A24" s="151" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B24" s="152" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C24" s="152"/>
     </row>
     <row r="25" spans="1:3" ht="15">
       <c r="A25" s="151" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B25" s="152" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C25" s="152"/>
     </row>
     <row r="26" spans="1:3" ht="15">
       <c r="A26" s="155" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B26" s="152" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C26" s="152"/>
     </row>
     <row r="27" spans="1:3" ht="15">
       <c r="A27" s="155" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B27" s="152" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C27" s="152"/>
     </row>
     <row r="28" spans="1:3" ht="15">
       <c r="A28" s="155" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B28" s="152" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C28" s="152"/>
     </row>
     <row r="29" spans="1:3" ht="15">
       <c r="A29" s="155" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B29" s="152" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C29" s="152"/>
     </row>
     <row r="30" spans="1:3" ht="15">
       <c r="A30" s="155" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B30" s="152" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C30" s="152"/>
     </row>
     <row r="31" spans="1:3" ht="15">
       <c r="A31" s="155" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B31" s="152"/>
       <c r="C31" s="152"/>
     </row>
     <row r="32" spans="1:3" ht="15">
       <c r="A32" s="155" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B32" s="152"/>
       <c r="C32" s="152"/>
     </row>
     <row r="33" spans="1:3" ht="15">
       <c r="A33" s="155" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B33" s="152"/>
       <c r="C33" s="152"/>
     </row>
     <row r="34" spans="1:3" ht="15">
       <c r="A34" s="155" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B34" s="152"/>
       <c r="C34" s="152"/>
@@ -5026,8 +4696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="13.5" customHeight="1"/>
@@ -5063,14 +4733,14 @@
       <c r="A2" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="207" t="s">
-        <v>287</v>
-      </c>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="207"/>
+      <c r="B2" s="220" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
       <c r="H2" s="140" t="s">
         <v>22</v>
       </c>
@@ -5083,14 +4753,14 @@
       <c r="A3" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="207" t="s">
+      <c r="B3" s="220" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="207"/>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="220"/>
+      <c r="E3" s="220"/>
+      <c r="F3" s="220"/>
+      <c r="G3" s="220"/>
       <c r="H3" s="140" t="s">
         <v>24</v>
       </c>
@@ -5103,14 +4773,14 @@
       <c r="A4" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="208" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="208"/>
-      <c r="D4" s="208"/>
-      <c r="E4" s="208"/>
-      <c r="F4" s="208"/>
-      <c r="G4" s="208"/>
+      <c r="B4" s="221" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="221"/>
+      <c r="F4" s="221"/>
+      <c r="G4" s="221"/>
       <c r="H4" s="140" t="s">
         <v>27</v>
       </c>
@@ -5130,11 +4800,11 @@
       <c r="D5" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="209" t="s">
+      <c r="E5" s="222" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="209"/>
-      <c r="G5" s="209"/>
+      <c r="F5" s="222"/>
+      <c r="G5" s="222"/>
       <c r="H5" s="141" t="s">
         <v>26</v>
       </c>
@@ -5160,12 +4830,12 @@
         <f>COUNTIF(F11:G673,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="210">
+      <c r="E6" s="223">
         <f>COUNTA(A11:A230)</f>
         <v>48</v>
       </c>
-      <c r="F6" s="210"/>
-      <c r="G6" s="210"/>
+      <c r="F6" s="223"/>
+      <c r="G6" s="223"/>
       <c r="H6" s="98"/>
       <c r="I6" s="94"/>
       <c r="J6" s="94" t="s">
@@ -5225,10 +4895,10 @@
         <v>34</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H10" s="57" t="s">
         <v>35</v>
@@ -5239,9 +4909,9 @@
       <c r="J10" s="94"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A11" s="218"/>
+      <c r="A11" s="201"/>
       <c r="B11" s="58" t="s">
-        <v>310</v>
+        <v>238</v>
       </c>
       <c r="C11" s="58"/>
       <c r="D11" s="58"/>
@@ -5253,18 +4923,18 @@
       <c r="J11" s="94"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A12" s="219" t="str">
+      <c r="A12" s="202" t="str">
         <f t="shared" ref="A12:A17" si="0">IF(OR(B12&lt;&gt;"",D12&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
         <v>[User Module-2]</v>
       </c>
       <c r="B12" s="120" t="s">
-        <v>289</v>
+        <v>217</v>
       </c>
       <c r="C12" s="120" t="s">
-        <v>288</v>
+        <v>216</v>
       </c>
       <c r="D12" s="120" t="s">
-        <v>290</v>
+        <v>218</v>
       </c>
       <c r="E12" s="117"/>
       <c r="F12" s="116"/>
@@ -5274,9 +4944,9 @@
       <c r="J12" s="94"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A13" s="220"/>
+      <c r="A13" s="203"/>
       <c r="B13" s="58" t="s">
-        <v>291</v>
+        <v>219</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="59"/>
@@ -5288,18 +4958,18 @@
       <c r="J13" s="94"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A14" s="219" t="str">
+      <c r="A14" s="202" t="str">
         <f t="shared" si="0"/>
         <v>[User Module-4]</v>
       </c>
       <c r="B14" s="90" t="s">
-        <v>307</v>
+        <v>235</v>
       </c>
       <c r="C14" s="90" t="s">
-        <v>302</v>
+        <v>230</v>
       </c>
       <c r="D14" s="120" t="s">
-        <v>308</v>
+        <v>236</v>
       </c>
       <c r="E14" s="90"/>
       <c r="F14" s="116"/>
@@ -5309,18 +4979,18 @@
       <c r="J14" s="94"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A15" s="219" t="str">
+      <c r="A15" s="202" t="str">
         <f t="shared" si="0"/>
         <v>[User Module-5]</v>
       </c>
       <c r="B15" s="90" t="s">
-        <v>295</v>
+        <v>223</v>
       </c>
       <c r="C15" s="190" t="s">
-        <v>292</v>
+        <v>220</v>
       </c>
       <c r="D15" s="194" t="s">
-        <v>309</v>
+        <v>237</v>
       </c>
       <c r="E15" s="190"/>
       <c r="F15" s="184"/>
@@ -5330,9 +5000,9 @@
       <c r="J15" s="94"/>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A16" s="220"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="58" t="s">
-        <v>293</v>
+        <v>221</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="193"/>
@@ -5344,21 +5014,21 @@
       <c r="J16" s="94"/>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A17" s="219" t="str">
+      <c r="A17" s="202" t="str">
         <f t="shared" si="0"/>
         <v>[User Module-7]</v>
       </c>
       <c r="B17" s="90" t="s">
-        <v>294</v>
+        <v>222</v>
       </c>
       <c r="C17" s="90" t="s">
-        <v>296</v>
+        <v>224</v>
       </c>
       <c r="D17" s="90" t="s">
-        <v>297</v>
+        <v>225</v>
       </c>
       <c r="E17" s="90" t="s">
-        <v>298</v>
+        <v>226</v>
       </c>
       <c r="F17" s="116"/>
       <c r="G17" s="90"/>
@@ -5367,9 +5037,9 @@
       <c r="J17" s="94"/>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A18" s="220"/>
+      <c r="A18" s="203"/>
       <c r="B18" s="58" t="s">
-        <v>299</v>
+        <v>227</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="59"/>
@@ -5386,13 +5056,13 @@
         <v>[User Module-9]</v>
       </c>
       <c r="B19" s="90" t="s">
-        <v>300</v>
+        <v>228</v>
       </c>
       <c r="C19" s="105" t="s">
-        <v>302</v>
+        <v>230</v>
       </c>
       <c r="D19" s="90" t="s">
-        <v>303</v>
+        <v>231</v>
       </c>
       <c r="E19" s="103"/>
       <c r="F19" s="116"/>
@@ -5407,16 +5077,16 @@
         <v>[User Module-10]</v>
       </c>
       <c r="B20" s="90" t="s">
-        <v>304</v>
+        <v>232</v>
       </c>
       <c r="C20" s="105" t="s">
-        <v>301</v>
+        <v>229</v>
       </c>
       <c r="D20" s="103" t="s">
-        <v>305</v>
+        <v>233</v>
       </c>
       <c r="E20" s="103" t="s">
-        <v>306</v>
+        <v>234</v>
       </c>
       <c r="F20" s="116"/>
       <c r="G20" s="157"/>
@@ -5425,11 +5095,11 @@
       <c r="J20" s="94"/>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A21" s="220" t="s">
-        <v>203</v>
+      <c r="A21" s="203" t="s">
+        <v>182</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>352</v>
+        <v>278</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
@@ -5446,16 +5116,16 @@
         <v>[User Module-12]</v>
       </c>
       <c r="B22" s="90" t="s">
-        <v>353</v>
+        <v>279</v>
       </c>
       <c r="C22" s="105" t="s">
-        <v>354</v>
+        <v>280</v>
       </c>
       <c r="D22" s="103" t="s">
-        <v>355</v>
+        <v>281</v>
       </c>
       <c r="E22" s="103" t="s">
-        <v>361</v>
+        <v>287</v>
       </c>
       <c r="F22" s="116"/>
       <c r="G22" s="90"/>
@@ -5464,11 +5134,11 @@
       <c r="J22" s="104"/>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A23" s="220" t="s">
-        <v>203</v>
+      <c r="A23" s="203" t="s">
+        <v>182</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>359</v>
+        <v>285</v>
       </c>
       <c r="C23" s="59"/>
       <c r="D23" s="59"/>
@@ -5485,16 +5155,16 @@
         <v>[User Module-14]</v>
       </c>
       <c r="B24" s="90" t="s">
-        <v>356</v>
+        <v>282</v>
       </c>
       <c r="C24" s="105" t="s">
-        <v>357</v>
+        <v>283</v>
       </c>
       <c r="D24" s="103" t="s">
-        <v>358</v>
+        <v>284</v>
       </c>
       <c r="E24" s="103" t="s">
-        <v>362</v>
+        <v>288</v>
       </c>
       <c r="F24" s="116"/>
       <c r="G24" s="157"/>
@@ -5503,19 +5173,19 @@
       <c r="J24" s="104"/>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A25" s="220" t="s">
-        <v>203</v>
+      <c r="A25" s="203" t="s">
+        <v>182</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>360</v>
+        <v>286</v>
       </c>
       <c r="C25" s="59"/>
       <c r="D25" s="59"/>
-      <c r="E25" s="213"/>
+      <c r="E25" s="196"/>
       <c r="F25" s="59"/>
       <c r="G25" s="59"/>
-      <c r="H25" s="213"/>
-      <c r="I25" s="215"/>
+      <c r="H25" s="196"/>
+      <c r="I25" s="198"/>
       <c r="J25" s="104"/>
     </row>
     <row r="26" spans="1:10" ht="14.25" customHeight="1">
@@ -5524,29 +5194,29 @@
         <v>[User Module-16]</v>
       </c>
       <c r="B26" s="90" t="s">
-        <v>363</v>
+        <v>289</v>
       </c>
       <c r="C26" s="105" t="s">
-        <v>364</v>
-      </c>
-      <c r="D26" s="212" t="s">
-        <v>365</v>
-      </c>
-      <c r="E26" s="214" t="s">
-        <v>366</v>
+        <v>290</v>
+      </c>
+      <c r="D26" s="195" t="s">
+        <v>291</v>
+      </c>
+      <c r="E26" s="197" t="s">
+        <v>292</v>
       </c>
       <c r="F26" s="116"/>
       <c r="G26" s="157"/>
-      <c r="H26" s="216"/>
-      <c r="I26" s="217"/>
+      <c r="H26" s="199"/>
+      <c r="I26" s="200"/>
       <c r="J26" s="104"/>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A27" s="221" t="s">
-        <v>203</v>
+      <c r="A27" s="204" t="s">
+        <v>182</v>
       </c>
       <c r="B27" s="161" t="s">
-        <v>311</v>
+        <v>239</v>
       </c>
       <c r="C27" s="158"/>
       <c r="D27" s="158"/>
@@ -5563,16 +5233,16 @@
         <v>[User Module-18]</v>
       </c>
       <c r="B28" s="116" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" s="116" t="s">
         <v>240</v>
       </c>
-      <c r="C28" s="116" t="s">
-        <v>312</v>
-      </c>
       <c r="D28" s="116" t="s">
-        <v>318</v>
+        <v>246</v>
       </c>
       <c r="E28" s="117" t="s">
-        <v>313</v>
+        <v>241</v>
       </c>
       <c r="F28" s="116"/>
       <c r="G28" s="116"/>
@@ -5581,11 +5251,11 @@
       <c r="J28" s="104"/>
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A29" s="221" t="s">
-        <v>203</v>
+      <c r="A29" s="204" t="s">
+        <v>182</v>
       </c>
       <c r="B29" s="161" t="s">
-        <v>314</v>
+        <v>242</v>
       </c>
       <c r="C29" s="158"/>
       <c r="D29" s="158"/>
@@ -5602,16 +5272,16 @@
         <v>[User Module-20]</v>
       </c>
       <c r="B30" s="116" t="s">
-        <v>315</v>
+        <v>243</v>
       </c>
       <c r="C30" s="116" t="s">
-        <v>316</v>
+        <v>244</v>
       </c>
       <c r="D30" s="116" t="s">
-        <v>317</v>
+        <v>245</v>
       </c>
       <c r="E30" s="117" t="s">
-        <v>319</v>
+        <v>247</v>
       </c>
       <c r="F30" s="116"/>
       <c r="G30" s="116"/>
@@ -5620,11 +5290,11 @@
       <c r="J30" s="104"/>
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A31" s="221" t="s">
-        <v>203</v>
+      <c r="A31" s="204" t="s">
+        <v>182</v>
       </c>
       <c r="B31" s="161" t="s">
-        <v>320</v>
+        <v>248</v>
       </c>
       <c r="C31" s="158"/>
       <c r="D31" s="158"/>
@@ -5641,16 +5311,16 @@
         <v>[User Module-22]</v>
       </c>
       <c r="B32" s="116" t="s">
-        <v>241</v>
+        <v>207</v>
       </c>
       <c r="C32" s="116" t="s">
-        <v>321</v>
+        <v>249</v>
       </c>
       <c r="D32" s="116" t="s">
-        <v>323</v>
+        <v>251</v>
       </c>
       <c r="E32" s="117" t="s">
-        <v>322</v>
+        <v>250</v>
       </c>
       <c r="F32" s="116"/>
       <c r="G32" s="116"/>
@@ -5659,11 +5329,11 @@
       <c r="J32" s="104"/>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A33" s="221" t="s">
-        <v>203</v>
+      <c r="A33" s="204" t="s">
+        <v>182</v>
       </c>
       <c r="B33" s="161" t="s">
-        <v>347</v>
+        <v>273</v>
       </c>
       <c r="C33" s="158"/>
       <c r="D33" s="158"/>
@@ -5680,16 +5350,16 @@
         <v>[User Module-24]</v>
       </c>
       <c r="B34" s="116" t="s">
-        <v>348</v>
+        <v>274</v>
       </c>
       <c r="C34" s="116" t="s">
-        <v>349</v>
+        <v>275</v>
       </c>
       <c r="D34" s="116" t="s">
-        <v>350</v>
+        <v>276</v>
       </c>
       <c r="E34" s="117" t="s">
-        <v>351</v>
+        <v>277</v>
       </c>
       <c r="F34" s="116"/>
       <c r="G34" s="116"/>
@@ -5698,11 +5368,11 @@
       <c r="J34" s="104"/>
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A35" s="221" t="s">
-        <v>203</v>
+      <c r="A35" s="204" t="s">
+        <v>182</v>
       </c>
       <c r="B35" s="161" t="s">
-        <v>344</v>
+        <v>270</v>
       </c>
       <c r="C35" s="158"/>
       <c r="D35" s="158"/>
@@ -5719,16 +5389,16 @@
         <v>[User Module-26]</v>
       </c>
       <c r="B36" s="116" t="s">
-        <v>342</v>
+        <v>268</v>
       </c>
       <c r="C36" s="116" t="s">
-        <v>343</v>
+        <v>269</v>
       </c>
       <c r="D36" s="116" t="s">
-        <v>345</v>
+        <v>271</v>
       </c>
       <c r="E36" s="117" t="s">
-        <v>346</v>
+        <v>272</v>
       </c>
       <c r="F36" s="116"/>
       <c r="G36" s="116"/>
@@ -5737,11 +5407,11 @@
       <c r="J36" s="104"/>
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A37" s="221" t="s">
-        <v>203</v>
+      <c r="A37" s="204" t="s">
+        <v>182</v>
       </c>
       <c r="B37" s="161" t="s">
-        <v>324</v>
+        <v>252</v>
       </c>
       <c r="C37" s="158"/>
       <c r="D37" s="158"/>
@@ -5758,16 +5428,16 @@
         <v>[User Module-28]</v>
       </c>
       <c r="B38" s="116" t="s">
-        <v>325</v>
+        <v>253</v>
       </c>
       <c r="C38" s="116" t="s">
-        <v>335</v>
+        <v>261</v>
       </c>
       <c r="D38" s="116" t="s">
-        <v>328</v>
+        <v>254</v>
       </c>
       <c r="E38" s="117" t="s">
-        <v>329</v>
+        <v>255</v>
       </c>
       <c r="F38" s="116"/>
       <c r="G38" s="116"/>
@@ -5776,11 +5446,11 @@
       <c r="J38" s="104"/>
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A39" s="221" t="s">
-        <v>203</v>
+      <c r="A39" s="204" t="s">
+        <v>182</v>
       </c>
       <c r="B39" s="161" t="s">
-        <v>330</v>
+        <v>256</v>
       </c>
       <c r="C39" s="158"/>
       <c r="D39" s="158"/>
@@ -5797,13 +5467,13 @@
         <v>[User Module-30]</v>
       </c>
       <c r="B40" s="116" t="s">
-        <v>331</v>
+        <v>257</v>
       </c>
       <c r="C40" s="116" t="s">
-        <v>332</v>
+        <v>258</v>
       </c>
       <c r="D40" s="116" t="s">
-        <v>333</v>
+        <v>259</v>
       </c>
       <c r="E40" s="117"/>
       <c r="F40" s="116"/>
@@ -5812,11 +5482,11 @@
       <c r="I40" s="119"/>
     </row>
     <row r="41" spans="1:10" s="175" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A41" s="221" t="s">
-        <v>203</v>
+      <c r="A41" s="204" t="s">
+        <v>182</v>
       </c>
       <c r="B41" s="161" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
       <c r="C41" s="158"/>
       <c r="D41" s="158"/>
@@ -5832,16 +5502,16 @@
         <v>[User Module-32]</v>
       </c>
       <c r="B42" s="116" t="s">
-        <v>334</v>
+        <v>260</v>
       </c>
       <c r="C42" s="116" t="s">
-        <v>336</v>
+        <v>262</v>
       </c>
       <c r="D42" s="116" t="s">
-        <v>337</v>
+        <v>263</v>
       </c>
       <c r="E42" s="117" t="s">
-        <v>338</v>
+        <v>264</v>
       </c>
       <c r="F42" s="116"/>
       <c r="G42" s="116"/>
@@ -5849,11 +5519,11 @@
       <c r="I42" s="119"/>
     </row>
     <row r="43" spans="1:10" s="180" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A43" s="221" t="s">
-        <v>203</v>
+      <c r="A43" s="204" t="s">
+        <v>182</v>
       </c>
       <c r="B43" s="161" t="s">
-        <v>339</v>
+        <v>265</v>
       </c>
       <c r="C43" s="158"/>
       <c r="D43" s="158"/>
@@ -5869,13 +5539,13 @@
         <v>[User Module-34]</v>
       </c>
       <c r="B44" s="116" t="s">
-        <v>331</v>
+        <v>257</v>
       </c>
       <c r="C44" s="116" t="s">
-        <v>341</v>
+        <v>267</v>
       </c>
       <c r="D44" s="116" t="s">
-        <v>340</v>
+        <v>266</v>
       </c>
       <c r="E44" s="117"/>
       <c r="F44" s="116"/>
@@ -5908,7 +5578,7 @@
     <row r="47" spans="1:10" s="180" customFormat="1" ht="14.25" customHeight="1">
       <c r="A47" s="161"/>
       <c r="B47" s="161" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C47" s="161"/>
       <c r="D47" s="161"/>
@@ -5921,7 +5591,7 @@
     <row r="48" spans="1:10" s="161" customFormat="1" ht="14.25" customHeight="1">
       <c r="A48" s="176"/>
       <c r="B48" s="177" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C48" s="178"/>
       <c r="D48" s="178"/>
@@ -5937,20 +5607,20 @@
         <v>ID-32</v>
       </c>
       <c r="B49" s="116" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C49" s="116" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D49" s="116" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E49" s="116"/>
       <c r="F49" s="116"/>
       <c r="G49" s="116"/>
       <c r="H49" s="116"/>
       <c r="I49" s="179" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="181" customFormat="1" ht="14.25" customHeight="1">
@@ -5959,20 +5629,20 @@
         <v>ID-33</v>
       </c>
       <c r="B50" s="116" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="C50" s="116" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="D50" s="116" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E50" s="116"/>
       <c r="F50" s="116"/>
       <c r="G50" s="116"/>
       <c r="H50" s="116"/>
       <c r="I50" s="179" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="181" customFormat="1" ht="14.25" customHeight="1">
@@ -5981,20 +5651,20 @@
         <v>ID-34</v>
       </c>
       <c r="B51" s="116" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="C51" s="116" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="D51" s="116" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E51" s="116"/>
       <c r="F51" s="116"/>
       <c r="G51" s="116"/>
       <c r="H51" s="116"/>
       <c r="I51" s="179" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="180" customFormat="1" ht="14.25" customHeight="1">
@@ -6003,20 +5673,20 @@
         <v>ID-35</v>
       </c>
       <c r="B52" s="116" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="C52" s="116" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="D52" s="116" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E52" s="116"/>
       <c r="F52" s="116"/>
       <c r="G52" s="116"/>
       <c r="H52" s="116"/>
       <c r="I52" s="179" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="175" customFormat="1" ht="14.25" customHeight="1">
@@ -6025,26 +5695,26 @@
         <v>ID-36</v>
       </c>
       <c r="B53" s="116" t="s">
-        <v>367</v>
+        <v>293</v>
       </c>
       <c r="C53" s="116" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="D53" s="116" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E53" s="116"/>
       <c r="F53" s="116"/>
       <c r="G53" s="116"/>
       <c r="H53" s="116"/>
       <c r="I53" s="179" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="175" customFormat="1" ht="14.25" customHeight="1">
       <c r="A54" s="161"/>
       <c r="B54" s="161" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C54" s="161"/>
       <c r="D54" s="161"/>
@@ -6060,20 +5730,20 @@
         <v>ID-37</v>
       </c>
       <c r="B55" s="116" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C55" s="116" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D55" s="116" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E55" s="116"/>
       <c r="F55" s="116"/>
       <c r="G55" s="116"/>
       <c r="H55" s="116"/>
       <c r="I55" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="175" customFormat="1" ht="14.25" customHeight="1">
@@ -6082,20 +5752,20 @@
         <v>ID-38</v>
       </c>
       <c r="B56" s="116" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C56" s="116" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D56" s="116" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E56" s="116"/>
       <c r="F56" s="116"/>
       <c r="G56" s="116"/>
       <c r="H56" s="116"/>
       <c r="I56" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="175" customFormat="1" ht="14.25" customHeight="1">
@@ -6104,20 +5774,20 @@
         <v>ID-39</v>
       </c>
       <c r="B57" s="116" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C57" s="116" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D57" s="116" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="E57" s="116"/>
       <c r="F57" s="116"/>
       <c r="G57" s="116"/>
       <c r="H57" s="116"/>
       <c r="I57" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="175" customFormat="1" ht="14.25" customHeight="1">
@@ -6126,20 +5796,20 @@
         <v>ID-40</v>
       </c>
       <c r="B58" s="116" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C58" s="116" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D58" s="116" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E58" s="116"/>
       <c r="F58" s="116"/>
       <c r="G58" s="116"/>
       <c r="H58" s="116"/>
       <c r="I58" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="175" customFormat="1" ht="14.25" customHeight="1">
@@ -6148,20 +5818,20 @@
         <v>ID-41</v>
       </c>
       <c r="B59" s="116" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C59" s="116" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D59" s="116" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E59" s="116"/>
       <c r="F59" s="116"/>
       <c r="G59" s="116"/>
       <c r="H59" s="116"/>
       <c r="I59" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="175" customFormat="1" ht="14.25" customHeight="1">
@@ -6170,20 +5840,20 @@
         <v>ID-42</v>
       </c>
       <c r="B60" s="116" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C60" s="116" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D60" s="116" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E60" s="116"/>
       <c r="F60" s="116"/>
       <c r="G60" s="116"/>
       <c r="H60" s="116"/>
       <c r="I60" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="13.5" customHeight="1">
@@ -6192,20 +5862,20 @@
         <v>ID-43</v>
       </c>
       <c r="B61" s="116" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C61" s="116" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D61" s="116" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E61" s="116"/>
       <c r="F61" s="116"/>
       <c r="G61" s="116"/>
       <c r="H61" s="116"/>
       <c r="I61" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="13.5" customHeight="1">
@@ -6214,20 +5884,20 @@
         <v>ID-44</v>
       </c>
       <c r="B62" s="116" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C62" s="116" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D62" s="116" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E62" s="116"/>
       <c r="F62" s="116"/>
       <c r="G62" s="116"/>
       <c r="H62" s="116"/>
       <c r="I62" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="13.5" customHeight="1">
@@ -6236,20 +5906,20 @@
         <v>ID-45</v>
       </c>
       <c r="B63" s="116" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C63" s="116" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D63" s="116" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E63" s="116"/>
       <c r="F63" s="116"/>
       <c r="G63" s="116"/>
       <c r="H63" s="116"/>
       <c r="I63" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="13.5" customHeight="1">
@@ -6258,20 +5928,20 @@
         <v>ID-46</v>
       </c>
       <c r="B64" s="116" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C64" s="116" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D64" s="116" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="E64" s="116"/>
       <c r="F64" s="116"/>
       <c r="G64" s="116"/>
       <c r="H64" s="116"/>
       <c r="I64" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="13.5" customHeight="1">
@@ -6280,20 +5950,20 @@
         <v>ID-47</v>
       </c>
       <c r="B65" s="116" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C65" s="116" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D65" s="116" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E65" s="116"/>
       <c r="F65" s="116"/>
       <c r="G65" s="116"/>
       <c r="H65" s="116"/>
       <c r="I65" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="13.5" customHeight="1">
@@ -6302,20 +5972,20 @@
         <v>ID-48</v>
       </c>
       <c r="B66" s="116" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C66" s="116" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D66" s="116" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E66" s="116"/>
       <c r="F66" s="116"/>
       <c r="G66" s="116"/>
       <c r="H66" s="116"/>
       <c r="I66" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="13.5" customHeight="1">
@@ -6324,20 +5994,20 @@
         <v>ID-49</v>
       </c>
       <c r="B67" s="116" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C67" s="116" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D67" s="116" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E67" s="116"/>
       <c r="F67" s="116"/>
       <c r="G67" s="116"/>
       <c r="H67" s="116"/>
       <c r="I67" s="116" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -6384,10 +6054,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:D20"/>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="13.5" customHeight="1"/>
@@ -6410,7 +6080,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="130" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="131" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B1" s="132"/>
       <c r="C1" s="132"/>
@@ -6423,46 +6093,46 @@
       <c r="A2" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="207" t="s">
-        <v>196</v>
-      </c>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="207"/>
+      <c r="B2" s="220" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
       <c r="J2" s="94" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="130" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="135" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="207" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="207"/>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
+        <v>124</v>
+      </c>
+      <c r="B3" s="220" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="220"/>
+      <c r="D3" s="220"/>
+      <c r="E3" s="220"/>
+      <c r="F3" s="220"/>
+      <c r="G3" s="220"/>
       <c r="J3" s="94" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="130" customFormat="1" ht="14.25">
       <c r="A4" s="134" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="208" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="208"/>
-      <c r="D4" s="208"/>
-      <c r="E4" s="208"/>
-      <c r="F4" s="208"/>
-      <c r="G4" s="208"/>
+        <v>126</v>
+      </c>
+      <c r="B4" s="221" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="221"/>
+      <c r="F4" s="221"/>
+      <c r="G4" s="221"/>
       <c r="J4" s="95"/>
     </row>
     <row r="5" spans="1:10" s="130" customFormat="1" ht="14.25">
@@ -6473,43 +6143,43 @@
         <v>24</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D5" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="211" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="211"/>
-      <c r="G5" s="211"/>
+      <c r="E5" s="224" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="224"/>
+      <c r="G5" s="224"/>
       <c r="J5" s="94" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="130" customFormat="1" ht="15" thickBot="1">
       <c r="A6" s="125">
-        <f>COUNTIF(F11:G258,"Pass")</f>
+        <f>COUNTIF(F11:G251,"Pass")</f>
         <v>0</v>
       </c>
       <c r="B6" s="100">
-        <f>COUNTIF(F11:G705,"Fail")</f>
+        <f>COUNTIF(F11:G698,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C6" s="100">
         <f>E6-D6-B6-A6</f>
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D6" s="101">
-        <f>COUNTIF(F11:G705,"N/A")</f>
+        <f>COUNTIF(F11:G698,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="210">
-        <f>COUNTA(A11:A263)*2</f>
-        <v>38</v>
-      </c>
-      <c r="F6" s="210"/>
-      <c r="G6" s="210"/>
+      <c r="E6" s="223">
+        <f>COUNTA(A11:A256)*2</f>
+        <v>20</v>
+      </c>
+      <c r="F6" s="223"/>
+      <c r="G6" s="223"/>
       <c r="J6" s="94" t="s">
         <v>27</v>
       </c>
@@ -6540,25 +6210,25 @@
         <v>30</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I10" s="56" t="s">
         <v>36</v>
@@ -6567,7 +6237,7 @@
     <row r="11" spans="1:10" s="130" customFormat="1" ht="14.25" customHeight="1">
       <c r="A11" s="128"/>
       <c r="B11" s="58" t="s">
-        <v>368</v>
+        <v>219</v>
       </c>
       <c r="C11" s="58"/>
       <c r="D11" s="58"/>
@@ -6579,12 +6249,18 @@
     </row>
     <row r="12" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
       <c r="A12" s="157" t="str">
-        <f t="shared" ref="A12:A20" si="0">IF(OR(B12&lt;&gt;"",D12&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v/>
-      </c>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
+        <f t="shared" ref="A12:A13" si="0">IF(OR(B12&lt;&gt;"",D12&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Mod_login-2]</v>
+      </c>
+      <c r="B12" s="90" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="90" t="s">
+        <v>296</v>
+      </c>
+      <c r="D12" s="120" t="s">
+        <v>236</v>
+      </c>
       <c r="E12" s="162"/>
       <c r="F12" s="116"/>
       <c r="G12" s="116"/>
@@ -6594,120 +6270,138 @@
     <row r="13" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
       <c r="A13" s="157" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
+        <v>[Mod_login-3]</v>
+      </c>
+      <c r="B13" s="90" t="s">
+        <v>297</v>
+      </c>
+      <c r="C13" s="190" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" s="194" t="s">
+        <v>237</v>
+      </c>
       <c r="E13" s="187"/>
       <c r="F13" s="116"/>
       <c r="G13" s="116"/>
       <c r="H13" s="165"/>
       <c r="I13" s="165"/>
     </row>
-    <row r="14" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A14" s="157" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B14" s="116"/>
-      <c r="C14" s="116"/>
-      <c r="D14" s="116"/>
-      <c r="E14" s="164"/>
-      <c r="F14" s="116"/>
-      <c r="G14" s="116"/>
-      <c r="H14" s="165"/>
-      <c r="I14" s="165"/>
-    </row>
-    <row r="15" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A15" s="157" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+    <row r="14" spans="1:10" ht="14.25" customHeight="1">
+      <c r="A14" s="167"/>
+      <c r="B14" s="168" t="s">
+        <v>295</v>
+      </c>
+      <c r="C14" s="167"/>
+      <c r="D14" s="167"/>
+      <c r="E14" s="167"/>
+      <c r="F14" s="167"/>
+      <c r="G14" s="167"/>
+      <c r="H14" s="167"/>
+      <c r="I14" s="169"/>
+      <c r="J14" s="104"/>
+    </row>
+    <row r="15" spans="1:10" ht="14.25" customHeight="1">
+      <c r="A15" s="157"/>
       <c r="B15" s="116"/>
       <c r="C15" s="116"/>
       <c r="D15" s="116"/>
-      <c r="E15" s="164"/>
+      <c r="E15" s="170"/>
       <c r="F15" s="116"/>
       <c r="G15" s="116"/>
       <c r="H15" s="165"/>
-      <c r="I15" s="165"/>
-    </row>
-    <row r="16" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A16" s="157" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="I15" s="166"/>
+      <c r="J15" s="104"/>
+    </row>
+    <row r="16" spans="1:10" ht="14.25" customHeight="1">
+      <c r="A16" s="157"/>
       <c r="B16" s="116"/>
       <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="164"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="170"/>
       <c r="F16" s="116"/>
       <c r="G16" s="116"/>
       <c r="H16" s="165"/>
-      <c r="I16" s="165"/>
-    </row>
-    <row r="17" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A17" s="157" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B17" s="116"/>
-      <c r="C17" s="116"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="164"/>
-      <c r="F17" s="116"/>
-      <c r="G17" s="116"/>
-      <c r="H17" s="165"/>
-      <c r="I17" s="165"/>
-    </row>
-    <row r="18" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
+      <c r="I16" s="166"/>
+      <c r="J16" s="104"/>
+    </row>
+    <row r="17" spans="1:10" ht="14.25" customHeight="1">
+      <c r="A17" s="167" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="167"/>
+      <c r="D17" s="167"/>
+      <c r="E17" s="167"/>
+      <c r="F17" s="167"/>
+      <c r="G17" s="167"/>
+      <c r="H17" s="167"/>
+      <c r="I17" s="169"/>
+      <c r="J17" s="104"/>
+    </row>
+    <row r="18" spans="1:10" ht="13.5" customHeight="1">
       <c r="A18" s="157" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B18" s="116"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="164"/>
+        <f t="shared" ref="A18:A24" si="1">IF(OR(B18&lt;&gt;"",D18&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Mod_login-8]</v>
+      </c>
+      <c r="B18" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="90" t="s">
+        <v>183</v>
+      </c>
+      <c r="D18" s="90" t="s">
+        <v>208</v>
+      </c>
+      <c r="E18" s="170"/>
       <c r="F18" s="116"/>
       <c r="G18" s="116"/>
       <c r="H18" s="165"/>
-      <c r="I18" s="165"/>
-    </row>
-    <row r="19" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A19" s="157" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="164"/>
-      <c r="F19" s="116"/>
-      <c r="G19" s="116"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165"/>
-    </row>
-    <row r="20" spans="1:10" ht="14.25" customHeight="1">
+      <c r="I18" s="166"/>
+    </row>
+    <row r="19" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A19" s="167" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" s="167"/>
+      <c r="D19" s="167"/>
+      <c r="E19" s="167"/>
+      <c r="F19" s="167"/>
+      <c r="G19" s="167"/>
+      <c r="H19" s="167"/>
+      <c r="I19" s="169"/>
+    </row>
+    <row r="20" spans="1:10" ht="13.5" customHeight="1">
       <c r="A20" s="157" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
+        <f t="shared" si="1"/>
+        <v>[Mod_login-10]</v>
+      </c>
+      <c r="B20" s="116" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="116" t="s">
+        <v>209</v>
+      </c>
+      <c r="D20" s="116" t="s">
+        <v>185</v>
+      </c>
       <c r="E20" s="164"/>
       <c r="F20" s="116"/>
       <c r="G20" s="116"/>
       <c r="H20" s="165"/>
       <c r="I20" s="166"/>
-      <c r="J20" s="104"/>
-    </row>
-    <row r="21" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A21" s="167"/>
-      <c r="B21" s="168" t="s">
-        <v>204</v>
+    </row>
+    <row r="21" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A21" s="167" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" s="58" t="s">
+        <v>188</v>
       </c>
       <c r="C21" s="167"/>
       <c r="D21" s="167"/>
@@ -6716,190 +6410,61 @@
       <c r="G21" s="167"/>
       <c r="H21" s="167"/>
       <c r="I21" s="169"/>
-      <c r="J21" s="104"/>
-    </row>
-    <row r="22" spans="1:10" ht="14.25" customHeight="1">
+    </row>
+    <row r="22" spans="1:10" ht="13.5" customHeight="1">
       <c r="A22" s="157" t="str">
-        <f t="shared" ref="A22:A31" si="1">IF(OR(B22&lt;&gt;"",D22&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <f t="shared" si="1"/>
         <v>[Mod_login-12]</v>
       </c>
       <c r="B22" s="116" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C22" s="116" t="s">
-        <v>267</v>
+        <v>210</v>
       </c>
       <c r="D22" s="116" t="s">
-        <v>239</v>
-      </c>
-      <c r="E22" s="170"/>
+        <v>186</v>
+      </c>
+      <c r="E22" s="164"/>
       <c r="F22" s="116"/>
       <c r="G22" s="116"/>
       <c r="H22" s="165"/>
       <c r="I22" s="166"/>
-      <c r="J22" s="104"/>
-    </row>
-    <row r="23" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A23" s="157" t="str">
+    </row>
+    <row r="23" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A23" s="167" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="167"/>
+      <c r="I23" s="169"/>
+    </row>
+    <row r="24" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A24" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>[Mod_login-13]</v>
-      </c>
-      <c r="B23" s="116" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="116" t="s">
-        <v>268</v>
-      </c>
-      <c r="D23" s="171" t="s">
-        <v>195</v>
-      </c>
-      <c r="E23" s="170"/>
-      <c r="F23" s="116"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="165"/>
-      <c r="I23" s="166"/>
-      <c r="J23" s="104"/>
-    </row>
-    <row r="24" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A24" s="167" t="s">
-        <v>203</v>
-      </c>
-      <c r="B24" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="167"/>
-      <c r="D24" s="167"/>
-      <c r="E24" s="167"/>
-      <c r="F24" s="167"/>
-      <c r="G24" s="167"/>
-      <c r="H24" s="167"/>
-      <c r="I24" s="169"/>
-      <c r="J24" s="104"/>
-    </row>
-    <row r="25" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A25" s="157" t="str">
-        <f t="shared" si="1"/>
-        <v>[Mod_login-15]</v>
-      </c>
-      <c r="B25" s="90" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="90" t="s">
-        <v>205</v>
-      </c>
-      <c r="D25" s="90" t="s">
-        <v>266</v>
-      </c>
-      <c r="E25" s="170"/>
-      <c r="F25" s="116"/>
-      <c r="G25" s="116"/>
-      <c r="H25" s="165"/>
-      <c r="I25" s="166"/>
-    </row>
-    <row r="26" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A26" s="167" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="58" t="s">
-        <v>209</v>
-      </c>
-      <c r="C26" s="167"/>
-      <c r="D26" s="167"/>
-      <c r="E26" s="167"/>
-      <c r="F26" s="167"/>
-      <c r="G26" s="167"/>
-      <c r="H26" s="167"/>
-      <c r="I26" s="169"/>
-    </row>
-    <row r="27" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A27" s="157" t="str">
-        <f t="shared" si="1"/>
-        <v>[Mod_login-17]</v>
-      </c>
-      <c r="B27" s="116" t="s">
-        <v>206</v>
-      </c>
-      <c r="C27" s="116" t="s">
-        <v>269</v>
-      </c>
-      <c r="D27" s="116" t="s">
-        <v>207</v>
-      </c>
-      <c r="E27" s="164"/>
-      <c r="F27" s="116"/>
-      <c r="G27" s="116"/>
-      <c r="H27" s="165"/>
-      <c r="I27" s="166"/>
-    </row>
-    <row r="28" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A28" s="167" t="s">
-        <v>203</v>
-      </c>
-      <c r="B28" s="58" t="s">
-        <v>210</v>
-      </c>
-      <c r="C28" s="167"/>
-      <c r="D28" s="167"/>
-      <c r="E28" s="167"/>
-      <c r="F28" s="167"/>
-      <c r="G28" s="167"/>
-      <c r="H28" s="167"/>
-      <c r="I28" s="169"/>
-    </row>
-    <row r="29" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A29" s="157" t="str">
-        <f t="shared" si="1"/>
-        <v>[Mod_login-19]</v>
-      </c>
-      <c r="B29" s="116" t="s">
-        <v>213</v>
-      </c>
-      <c r="C29" s="116" t="s">
-        <v>270</v>
-      </c>
-      <c r="D29" s="116" t="s">
-        <v>208</v>
-      </c>
-      <c r="E29" s="164"/>
-      <c r="F29" s="116"/>
-      <c r="G29" s="116"/>
-      <c r="H29" s="165"/>
-      <c r="I29" s="166"/>
-    </row>
-    <row r="30" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A30" s="167" t="s">
-        <v>203</v>
-      </c>
-      <c r="B30" s="58" t="s">
+        <v>[Mod_login-14]</v>
+      </c>
+      <c r="B24" s="116" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" s="116" t="s">
         <v>211</v>
       </c>
-      <c r="C30" s="167"/>
-      <c r="D30" s="167"/>
-      <c r="E30" s="167"/>
-      <c r="F30" s="167"/>
-      <c r="G30" s="167"/>
-      <c r="H30" s="167"/>
-      <c r="I30" s="169"/>
-    </row>
-    <row r="31" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A31" s="157" t="str">
-        <f t="shared" si="1"/>
-        <v>[Mod_login-21]</v>
-      </c>
-      <c r="B31" s="116" t="s">
-        <v>212</v>
-      </c>
-      <c r="C31" s="116" t="s">
-        <v>271</v>
-      </c>
-      <c r="D31" s="116" t="s">
-        <v>214</v>
-      </c>
-      <c r="E31" s="164"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="165"/>
-      <c r="I31" s="166"/>
+      <c r="D24" s="116" t="s">
+        <v>192</v>
+      </c>
+      <c r="E24" s="164"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="165"/>
+      <c r="I24" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6910,7 +6475,7 @@
     <mergeCell ref="E6:G6"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G3 F12:G20 F22:G24">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1:G3 F12:G13 F15:G17">
       <formula1>$J$2:$J$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G8">
@@ -6935,8 +6500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="13.5" customHeight="1"/>
@@ -6944,8 +6509,8 @@
     <col min="1" max="1" width="18.125" style="129" customWidth="1"/>
     <col min="2" max="2" width="42.125" style="104" customWidth="1"/>
     <col min="3" max="3" width="33" style="104" customWidth="1"/>
-    <col min="4" max="4" width="30.625" style="104" customWidth="1"/>
-    <col min="5" max="5" width="15.125" style="104" customWidth="1"/>
+    <col min="4" max="4" width="28.875" style="104" customWidth="1"/>
+    <col min="5" max="5" width="17.375" style="104" customWidth="1"/>
     <col min="6" max="6" width="9.125" style="104" customWidth="1"/>
     <col min="7" max="7" width="7.375" style="104" customWidth="1"/>
     <col min="8" max="8" width="15.125" style="108" customWidth="1"/>
@@ -6959,7 +6524,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="130" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="131" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B1" s="132"/>
       <c r="C1" s="132"/>
@@ -6972,46 +6537,46 @@
       <c r="A2" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="207" t="s">
+      <c r="B2" s="220" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="207"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
       <c r="J2" s="94" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="130" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="135" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="207" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="207"/>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
+        <v>124</v>
+      </c>
+      <c r="B3" s="220" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="220"/>
+      <c r="D3" s="220"/>
+      <c r="E3" s="220"/>
+      <c r="F3" s="220"/>
+      <c r="G3" s="220"/>
       <c r="J3" s="94" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="130" customFormat="1" ht="14.25">
       <c r="A4" s="134" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="208" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="208"/>
-      <c r="D4" s="208"/>
-      <c r="E4" s="208"/>
-      <c r="F4" s="208"/>
-      <c r="G4" s="208"/>
+        <v>126</v>
+      </c>
+      <c r="B4" s="221" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="221"/>
+      <c r="F4" s="221"/>
+      <c r="G4" s="221"/>
       <c r="J4" s="95"/>
     </row>
     <row r="5" spans="1:10" s="130" customFormat="1" ht="14.25">
@@ -7022,16 +6587,16 @@
         <v>24</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D5" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="211" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="211"/>
-      <c r="G5" s="211"/>
+      <c r="E5" s="224" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="224"/>
+      <c r="G5" s="224"/>
       <c r="J5" s="94" t="s">
         <v>29</v>
       </c>
@@ -7047,18 +6612,18 @@
       </c>
       <c r="C6" s="100">
         <f>E6-D6-B6-A6</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D6" s="101">
         <f>COUNTIF(F11:G708,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="210">
-        <f>COUNTA(A11:A265)*2</f>
-        <v>12</v>
-      </c>
-      <c r="F6" s="210"/>
-      <c r="G6" s="210"/>
+      <c r="E6" s="223">
+        <f>COUNTA(A11:A265)</f>
+        <v>5</v>
+      </c>
+      <c r="F6" s="223"/>
+      <c r="G6" s="223"/>
       <c r="J6" s="94" t="s">
         <v>27</v>
       </c>
@@ -7089,25 +6654,25 @@
         <v>30</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D10" s="57" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I10" s="57" t="s">
         <v>36</v>
@@ -7116,7 +6681,7 @@
     <row r="11" spans="1:10" s="130" customFormat="1" ht="14.25" customHeight="1">
       <c r="A11" s="167"/>
       <c r="B11" s="168" t="s">
-        <v>372</v>
+        <v>294</v>
       </c>
       <c r="C11" s="167"/>
       <c r="D11" s="167"/>
@@ -7127,26 +6692,31 @@
       <c r="I11" s="169"/>
     </row>
     <row r="12" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A12" s="222"/>
-      <c r="B12" s="223" t="s">
-        <v>369</v>
-      </c>
-      <c r="C12" s="223" t="s">
-        <v>370</v>
-      </c>
-      <c r="D12" s="223" t="s">
-        <v>371</v>
-      </c>
-      <c r="E12" s="224"/>
-      <c r="F12" s="223"/>
-      <c r="G12" s="223"/>
-      <c r="H12" s="225"/>
-      <c r="I12" s="226"/>
+      <c r="A12" s="157" t="str">
+        <f t="shared" ref="A12:A17" si="0">IF(OR(B12&lt;&gt;"",D12&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Admin_login-2]</v>
+      </c>
+      <c r="B12" s="205" t="s">
+        <v>303</v>
+      </c>
+      <c r="C12" s="205" t="s">
+        <v>298</v>
+      </c>
+      <c r="D12" s="205" t="s">
+        <v>299</v>
+      </c>
+      <c r="E12" s="170" t="s">
+        <v>300</v>
+      </c>
+      <c r="F12" s="205"/>
+      <c r="G12" s="205"/>
+      <c r="H12" s="206"/>
+      <c r="I12" s="207"/>
     </row>
     <row r="13" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A13" s="167"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="168" t="s">
-        <v>373</v>
+        <v>301</v>
       </c>
       <c r="C13" s="167"/>
       <c r="D13" s="167"/>
@@ -7157,22 +6727,31 @@
       <c r="I13" s="169"/>
     </row>
     <row r="14" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A14" s="157"/>
+      <c r="A14" s="157" t="str">
+        <f t="shared" si="0"/>
+        <v>[Admin_login-4]</v>
+      </c>
       <c r="B14" s="116" t="s">
-        <v>375</v>
-      </c>
-      <c r="C14" s="116"/>
-      <c r="D14" s="116"/>
-      <c r="E14" s="164"/>
+        <v>302</v>
+      </c>
+      <c r="C14" s="116" t="s">
+        <v>304</v>
+      </c>
+      <c r="D14" s="116" t="s">
+        <v>305</v>
+      </c>
+      <c r="E14" s="164" t="s">
+        <v>306</v>
+      </c>
       <c r="F14" s="116"/>
       <c r="G14" s="116"/>
       <c r="H14" s="165"/>
       <c r="I14" s="165"/>
     </row>
     <row r="15" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A15" s="167"/>
+      <c r="A15" s="58"/>
       <c r="B15" s="168" t="s">
-        <v>374</v>
+        <v>307</v>
       </c>
       <c r="C15" s="167"/>
       <c r="D15" s="167"/>
@@ -7183,25 +6762,34 @@
       <c r="I15" s="169"/>
     </row>
     <row r="16" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A16" s="157"/>
+      <c r="A16" s="157" t="str">
+        <f t="shared" si="0"/>
+        <v>[Admin_login-6]</v>
+      </c>
       <c r="B16" s="116" t="s">
-        <v>376</v>
-      </c>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="164"/>
+        <v>308</v>
+      </c>
+      <c r="C16" s="116" t="s">
+        <v>309</v>
+      </c>
+      <c r="D16" s="116" t="s">
+        <v>310</v>
+      </c>
+      <c r="E16" s="164" t="s">
+        <v>311</v>
+      </c>
       <c r="F16" s="116"/>
       <c r="G16" s="116"/>
       <c r="H16" s="165"/>
       <c r="I16" s="165"/>
     </row>
     <row r="17" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A17" s="167"/>
-      <c r="B17" s="168" t="s">
-        <v>377</v>
-      </c>
-      <c r="C17" s="167"/>
-      <c r="D17" s="167"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
       <c r="E17" s="167"/>
       <c r="F17" s="167"/>
       <c r="G17" s="167"/>
@@ -7209,10 +6797,19 @@
       <c r="I17" s="169"/>
     </row>
     <row r="18" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A18" s="157"/>
-      <c r="B18" s="116"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
+      <c r="A18" s="157" t="str">
+        <f t="shared" ref="A18:A19" si="1">IF(OR(B18&lt;&gt;"",D18&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Admin_login-8]</v>
+      </c>
+      <c r="B18" s="90" t="s">
+        <v>235</v>
+      </c>
+      <c r="C18" s="90" t="s">
+        <v>314</v>
+      </c>
+      <c r="D18" s="120" t="s">
+        <v>236</v>
+      </c>
       <c r="E18" s="164"/>
       <c r="F18" s="116"/>
       <c r="G18" s="116"/>
@@ -7220,10 +6817,19 @@
       <c r="I18" s="165"/>
     </row>
     <row r="19" spans="1:10" s="110" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A19" s="157"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
+      <c r="A19" s="157" t="str">
+        <f t="shared" si="1"/>
+        <v>[Admin_login-9]</v>
+      </c>
+      <c r="B19" s="90" t="s">
+        <v>312</v>
+      </c>
+      <c r="C19" s="190" t="s">
+        <v>313</v>
+      </c>
+      <c r="D19" s="194" t="s">
+        <v>237</v>
+      </c>
       <c r="E19" s="164"/>
       <c r="F19" s="116"/>
       <c r="G19" s="116"/>
@@ -7231,177 +6837,122 @@
       <c r="I19" s="165"/>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A20" s="157"/>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="164"/>
-      <c r="F20" s="116"/>
-      <c r="G20" s="116"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="166"/>
+      <c r="A20" s="225"/>
+      <c r="B20" s="226"/>
+      <c r="C20" s="226"/>
+      <c r="D20" s="226"/>
+      <c r="E20" s="227"/>
+      <c r="F20" s="226"/>
+      <c r="G20" s="226"/>
+      <c r="H20" s="228"/>
+      <c r="I20" s="229"/>
       <c r="J20" s="104"/>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A21" s="167"/>
-      <c r="B21" s="168"/>
-      <c r="C21" s="167"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
-      <c r="F21" s="167"/>
-      <c r="G21" s="167"/>
-      <c r="H21" s="167"/>
-      <c r="I21" s="169"/>
+      <c r="A21" s="230"/>
+      <c r="B21" s="230"/>
+      <c r="C21" s="230"/>
+      <c r="D21" s="230"/>
+      <c r="E21" s="230"/>
+      <c r="F21" s="230"/>
+      <c r="G21" s="230"/>
+      <c r="H21" s="230"/>
+      <c r="I21" s="230"/>
       <c r="J21" s="104"/>
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A22" s="157" t="str">
-        <f t="shared" ref="A22:A23" si="0">IF(OR(B22&lt;&gt;"",D22&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[Admin_login-12]</v>
-      </c>
-      <c r="B22" s="116"/>
-      <c r="C22" s="116" t="s">
-        <v>126</v>
-      </c>
-      <c r="D22" s="116" t="s">
-        <v>272</v>
-      </c>
-      <c r="E22" s="170" t="s">
-        <v>190</v>
-      </c>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="165"/>
-      <c r="I22" s="166"/>
+      <c r="A22" s="194"/>
+      <c r="B22" s="194"/>
+      <c r="C22" s="194"/>
+      <c r="D22" s="194"/>
+      <c r="E22" s="231"/>
+      <c r="F22" s="194"/>
+      <c r="G22" s="194"/>
+      <c r="H22" s="232"/>
+      <c r="I22" s="233"/>
       <c r="J22" s="104"/>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A23" s="157" t="str">
-        <f t="shared" si="0"/>
-        <v>[Admin_login-13]</v>
-      </c>
-      <c r="B23" s="116"/>
-      <c r="C23" s="116" t="s">
-        <v>273</v>
-      </c>
-      <c r="D23" s="171" t="s">
-        <v>274</v>
-      </c>
-      <c r="E23" s="170" t="s">
-        <v>190</v>
-      </c>
-      <c r="F23" s="116"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="165"/>
-      <c r="I23" s="166"/>
+      <c r="A23" s="194"/>
+      <c r="B23" s="194"/>
+      <c r="C23" s="194"/>
+      <c r="D23" s="234"/>
+      <c r="E23" s="231"/>
+      <c r="F23" s="194"/>
+      <c r="G23" s="194"/>
+      <c r="H23" s="232"/>
+      <c r="I23" s="233"/>
       <c r="J23" s="104"/>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A24" s="167"/>
-      <c r="B24" s="168" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24" s="167"/>
-      <c r="D24" s="167"/>
-      <c r="E24" s="167"/>
-      <c r="F24" s="167"/>
-      <c r="G24" s="167"/>
-      <c r="H24" s="167"/>
-      <c r="I24" s="169"/>
+      <c r="A24" s="230"/>
+      <c r="B24" s="230"/>
+      <c r="C24" s="230"/>
+      <c r="D24" s="230"/>
+      <c r="E24" s="230"/>
+      <c r="F24" s="230"/>
+      <c r="G24" s="230"/>
+      <c r="H24" s="230"/>
+      <c r="I24" s="230"/>
       <c r="J24" s="104"/>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A25" s="157" t="str">
-        <f t="shared" ref="A25" si="1">IF(OR(B25&lt;&gt;"",D25&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[Admin_login-15]</v>
-      </c>
-      <c r="B25" s="116" t="s">
-        <v>276</v>
-      </c>
-      <c r="C25" s="116" t="s">
-        <v>275</v>
-      </c>
-      <c r="D25" s="171" t="s">
-        <v>140</v>
-      </c>
-      <c r="E25" s="170" t="s">
-        <v>190</v>
-      </c>
-      <c r="F25" s="116"/>
-      <c r="G25" s="116"/>
-      <c r="H25" s="165"/>
-      <c r="I25" s="166"/>
+      <c r="A25" s="194"/>
+      <c r="B25" s="194"/>
+      <c r="C25" s="194"/>
+      <c r="D25" s="234"/>
+      <c r="E25" s="231"/>
+      <c r="F25" s="194"/>
+      <c r="G25" s="194"/>
+      <c r="H25" s="232"/>
+      <c r="I25" s="233"/>
       <c r="J25" s="104"/>
     </row>
     <row r="26" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A26" s="167"/>
-      <c r="B26" s="168" t="s">
-        <v>128</v>
-      </c>
-      <c r="C26" s="167"/>
-      <c r="D26" s="167"/>
-      <c r="E26" s="167"/>
-      <c r="F26" s="167"/>
-      <c r="G26" s="167"/>
-      <c r="H26" s="167"/>
-      <c r="I26" s="169"/>
+      <c r="A26" s="230"/>
+      <c r="B26" s="230"/>
+      <c r="C26" s="230"/>
+      <c r="D26" s="230"/>
+      <c r="E26" s="230"/>
+      <c r="F26" s="230"/>
+      <c r="G26" s="230"/>
+      <c r="H26" s="230"/>
+      <c r="I26" s="230"/>
       <c r="J26" s="104"/>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A27" s="157" t="str">
-        <f t="shared" ref="A27:A29" si="2">IF(OR(B27&lt;&gt;"",D27&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[Admin_login-17]</v>
-      </c>
-      <c r="B27" s="116" t="s">
-        <v>277</v>
-      </c>
-      <c r="C27" s="116" t="s">
-        <v>278</v>
-      </c>
-      <c r="D27" s="171" t="s">
-        <v>279</v>
-      </c>
-      <c r="E27" s="170"/>
-      <c r="F27" s="116"/>
-      <c r="G27" s="116"/>
-      <c r="H27" s="165"/>
-      <c r="I27" s="166"/>
+      <c r="A27" s="194"/>
+      <c r="B27" s="194"/>
+      <c r="C27" s="194"/>
+      <c r="D27" s="234"/>
+      <c r="E27" s="231"/>
+      <c r="F27" s="194"/>
+      <c r="G27" s="194"/>
+      <c r="H27" s="232"/>
+      <c r="I27" s="233"/>
       <c r="J27" s="104"/>
     </row>
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A28" s="167" t="s">
-        <v>203</v>
-      </c>
-      <c r="B28" s="168" t="s">
-        <v>282</v>
-      </c>
-      <c r="C28" s="167"/>
-      <c r="D28" s="167"/>
-      <c r="E28" s="167"/>
-      <c r="F28" s="167"/>
-      <c r="G28" s="167"/>
-      <c r="H28" s="167"/>
-      <c r="I28" s="169"/>
+      <c r="A28" s="230"/>
+      <c r="B28" s="230"/>
+      <c r="C28" s="230"/>
+      <c r="D28" s="230"/>
+      <c r="E28" s="230"/>
+      <c r="F28" s="230"/>
+      <c r="G28" s="230"/>
+      <c r="H28" s="230"/>
+      <c r="I28" s="230"/>
     </row>
     <row r="29" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A29" s="157" t="str">
-        <f t="shared" si="2"/>
-        <v>[Admin_login-19]</v>
-      </c>
-      <c r="B29" s="116" t="s">
-        <v>283</v>
-      </c>
-      <c r="C29" s="116" t="s">
-        <v>280</v>
-      </c>
-      <c r="D29" s="171" t="s">
-        <v>281</v>
-      </c>
-      <c r="E29" s="170"/>
-      <c r="F29" s="116"/>
-      <c r="G29" s="116"/>
-      <c r="H29" s="165"/>
-      <c r="I29" s="166"/>
+      <c r="A29" s="194"/>
+      <c r="B29" s="194"/>
+      <c r="C29" s="194"/>
+      <c r="D29" s="235"/>
+      <c r="E29" s="236"/>
+      <c r="F29" s="194"/>
+      <c r="G29" s="194"/>
+      <c r="H29" s="232"/>
+      <c r="I29" s="233"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7423,8 +6974,8 @@
     <hyperlink ref="A1" location="'Test Report'!A1" display="Back to Test Report"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Upfile SRS qua achive vs reference
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
+++ b/WIP/Deliverable/Report3/VMN_Integration Test Case_v1.0_EN.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16729"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14880" tabRatio="743"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14880" tabRatio="743" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <definedName name="Statistic" comment="fsfsdfs" localSheetId="4">#REF!</definedName>
     <definedName name="Statistic" comment="fsfsdfs">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterate="1" iterateCount="10000" iterateDelta="1.0000000000000001E-5" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterate="1" iterateCount="10000" iterateDelta="1.0000000000000001E-5" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="349">
   <si>
     <t>Project Name</t>
   </si>
@@ -1601,7 +1601,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy;@"/>
   </numFmts>
@@ -3200,58 +3200,6 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="44" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="47" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="48" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="49" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="49" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3259,15 +3207,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="52" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="52" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="49" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="53" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3281,23 +3220,84 @@
     <xf numFmtId="0" fontId="14" fillId="10" borderId="53" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="47" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="48" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="49" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="52" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="49" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -3430,14 +3430,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3817,7 +3817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B10" sqref="B10:G11"/>
     </sheetView>
   </sheetViews>
@@ -3836,13 +3836,13 @@
     <row r="2" spans="1:7" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="202" t="s">
+      <c r="C2" s="215" t="s">
         <v>339</v>
       </c>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="215"/>
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="6"/>
@@ -3853,11 +3853,11 @@
       <c r="B4" s="190" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="203" t="s">
+      <c r="C4" s="216" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="203"/>
-      <c r="E4" s="203"/>
+      <c r="D4" s="216"/>
+      <c r="E4" s="216"/>
       <c r="F4" s="190" t="s">
         <v>1</v>
       </c>
@@ -3869,11 +3869,11 @@
       <c r="B5" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="203" t="s">
+      <c r="C5" s="216" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="203"/>
-      <c r="E5" s="203"/>
+      <c r="D5" s="216"/>
+      <c r="E5" s="216"/>
       <c r="F5" s="190" t="s">
         <v>3</v>
       </c>
@@ -3882,15 +3882,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="231" t="s">
+      <c r="B6" s="217" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="204" t="str">
+      <c r="C6" s="218" t="str">
         <f>C5&amp;"_"&amp;"Integration Test Case"&amp;"_"&amp;"v1.0"</f>
         <v>VMN_Integration Test Case_v1.0</v>
       </c>
-      <c r="D6" s="204"/>
-      <c r="E6" s="204"/>
+      <c r="D6" s="218"/>
+      <c r="E6" s="218"/>
       <c r="F6" s="190" t="s">
         <v>5</v>
       </c>
@@ -3899,10 +3899,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B7" s="231"/>
-      <c r="C7" s="204"/>
-      <c r="D7" s="204"/>
-      <c r="E7" s="204"/>
+      <c r="B7" s="217"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="218"/>
+      <c r="E7" s="218"/>
       <c r="F7" s="190" t="s">
         <v>340</v>
       </c>
@@ -3923,27 +3923,27 @@
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" s="232" t="s">
+      <c r="B10" s="210" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1">
-      <c r="B11" s="233" t="s">
+      <c r="B11" s="211" t="s">
         <v>342</v>
       </c>
-      <c r="C11" s="234" t="s">
+      <c r="C11" s="212" t="s">
         <v>340</v>
       </c>
-      <c r="D11" s="234" t="s">
+      <c r="D11" s="212" t="s">
         <v>343</v>
       </c>
-      <c r="E11" s="234" t="s">
+      <c r="E11" s="212" t="s">
         <v>344</v>
       </c>
-      <c r="F11" s="234" t="s">
+      <c r="F11" s="212" t="s">
         <v>345</v>
       </c>
-      <c r="G11" s="235" t="s">
+      <c r="G11" s="213" t="s">
         <v>346</v>
       </c>
     </row>
@@ -4069,39 +4069,39 @@
       <c r="E2" s="29"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="207" t="s">
+      <c r="B3" s="221" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="207"/>
-      <c r="D3" s="208" t="str">
+      <c r="C3" s="221"/>
+      <c r="D3" s="222" t="str">
         <f>Cover!C4</f>
         <v>Vietnamese Medicinal Plants Network</v>
       </c>
-      <c r="E3" s="208"/>
-      <c r="F3" s="208"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="222"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="207" t="s">
+      <c r="B4" s="221" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="207"/>
-      <c r="D4" s="208" t="str">
+      <c r="C4" s="221"/>
+      <c r="D4" s="222" t="str">
         <f>Cover!C5</f>
         <v>VMN</v>
       </c>
-      <c r="E4" s="208"/>
-      <c r="F4" s="208"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="222"/>
     </row>
     <row r="5" spans="2:6" s="30" customFormat="1" ht="72" customHeight="1">
-      <c r="B5" s="205" t="s">
+      <c r="B5" s="219" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="205"/>
-      <c r="D5" s="206" t="s">
+      <c r="C5" s="219"/>
+      <c r="D5" s="220" t="s">
         <v>348</v>
       </c>
-      <c r="E5" s="206"/>
-      <c r="F5" s="206"/>
+      <c r="E5" s="220"/>
+      <c r="F5" s="220"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="31"/>
@@ -4295,15 +4295,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B1" s="211" t="s">
+      <c r="B1" s="225" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="211"/>
-      <c r="D1" s="211"/>
-      <c r="E1" s="211"/>
-      <c r="F1" s="211"/>
-      <c r="G1" s="211"/>
-      <c r="H1" s="211"/>
+      <c r="C1" s="225"/>
+      <c r="D1" s="225"/>
+      <c r="E1" s="225"/>
+      <c r="F1" s="225"/>
+      <c r="G1" s="225"/>
+      <c r="H1" s="225"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="56"/>
@@ -4319,15 +4319,15 @@
       <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="208" t="str">
+      <c r="C3" s="222" t="str">
         <f>Cover!C4</f>
         <v>Vietnamese Medicinal Plants Network</v>
       </c>
-      <c r="D3" s="208"/>
-      <c r="E3" s="209" t="s">
+      <c r="D3" s="222"/>
+      <c r="E3" s="223" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="209"/>
+      <c r="F3" s="223"/>
       <c r="G3" s="9" t="s">
         <v>107</v>
       </c>
@@ -4337,15 +4337,15 @@
       <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="208" t="str">
+      <c r="C4" s="222" t="str">
         <f>Cover!C5</f>
         <v>VMN</v>
       </c>
-      <c r="D4" s="208"/>
-      <c r="E4" s="209" t="s">
+      <c r="D4" s="222"/>
+      <c r="E4" s="223" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="209"/>
+      <c r="F4" s="223"/>
       <c r="G4" s="9" t="s">
         <v>111</v>
       </c>
@@ -4355,15 +4355,15 @@
       <c r="B5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="208" t="str">
+      <c r="C5" s="222" t="str">
         <f>C4&amp;"_"&amp;"Integration Test Report"&amp;"_"&amp;"v1.0"</f>
         <v>VMN_Integration Test Report_v1.0</v>
       </c>
-      <c r="D5" s="208"/>
-      <c r="E5" s="209" t="s">
+      <c r="D5" s="222"/>
+      <c r="E5" s="223" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="209"/>
+      <c r="F5" s="223"/>
       <c r="G5" s="109"/>
       <c r="H5" s="61"/>
     </row>
@@ -4372,12 +4372,12 @@
       <c r="B6" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="210"/>
-      <c r="D6" s="210"/>
-      <c r="E6" s="210"/>
-      <c r="F6" s="210"/>
-      <c r="G6" s="210"/>
-      <c r="H6" s="210"/>
+      <c r="C6" s="224"/>
+      <c r="D6" s="224"/>
+      <c r="E6" s="224"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="224"/>
+      <c r="H6" s="224"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
       <c r="A7" s="56"/>
@@ -4479,7 +4479,7 @@
       </c>
       <c r="F12" s="70">
         <f>'Mod Module'!C6</f>
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G12" s="70">
         <f>'Mod Module'!D6</f>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="H12" s="71">
         <f>'Mod Module'!E6</f>
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4535,7 +4535,7 @@
       </c>
       <c r="F14" s="73">
         <f>SUM(F11:F13)</f>
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="G14" s="73">
         <f>SUM(G9:G13)</f>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="H14" s="74">
         <f>SUM(H11:H13)</f>
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -4667,14 +4667,14 @@
       <c r="A2" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="229" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
       <c r="H2" s="134" t="s">
         <v>14</v>
       </c>
@@ -4687,14 +4687,14 @@
       <c r="A3" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="215" t="s">
+      <c r="B3" s="229" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="215"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
+      <c r="C3" s="229"/>
+      <c r="D3" s="229"/>
+      <c r="E3" s="229"/>
+      <c r="F3" s="229"/>
+      <c r="G3" s="229"/>
       <c r="H3" s="134" t="s">
         <v>16</v>
       </c>
@@ -4707,14 +4707,14 @@
       <c r="A4" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="216" t="s">
+      <c r="B4" s="230" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="216"/>
-      <c r="D4" s="216"/>
-      <c r="E4" s="216"/>
-      <c r="F4" s="216"/>
-      <c r="G4" s="216"/>
+      <c r="C4" s="230"/>
+      <c r="D4" s="230"/>
+      <c r="E4" s="230"/>
+      <c r="F4" s="230"/>
+      <c r="G4" s="230"/>
       <c r="H4" s="134" t="s">
         <v>19</v>
       </c>
@@ -4734,11 +4734,11 @@
       <c r="D5" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="217" t="s">
+      <c r="E5" s="231" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="217"/>
-      <c r="G5" s="217"/>
+      <c r="F5" s="231"/>
+      <c r="G5" s="231"/>
       <c r="H5" s="135" t="s">
         <v>18</v>
       </c>
@@ -4764,12 +4764,12 @@
         <f>COUNTIF(F11:G679,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="218">
+      <c r="E6" s="232">
         <f>COUNTA(A11:A236)*2</f>
         <v>104</v>
       </c>
-      <c r="F6" s="218"/>
-      <c r="G6" s="218"/>
+      <c r="F6" s="232"/>
+      <c r="G6" s="232"/>
       <c r="H6" s="93"/>
       <c r="I6" s="89"/>
       <c r="J6" s="89" t="s">
@@ -5610,13 +5610,13 @@
       <c r="B53" s="194" t="s">
         <v>62</v>
       </c>
-      <c r="C53" s="212"/>
-      <c r="D53" s="213"/>
-      <c r="E53" s="213"/>
-      <c r="F53" s="213"/>
-      <c r="G53" s="213"/>
-      <c r="H53" s="213"/>
-      <c r="I53" s="214"/>
+      <c r="C53" s="226"/>
+      <c r="D53" s="227"/>
+      <c r="E53" s="227"/>
+      <c r="F53" s="227"/>
+      <c r="G53" s="227"/>
+      <c r="H53" s="227"/>
+      <c r="I53" s="228"/>
     </row>
     <row r="54" spans="1:9" s="146" customFormat="1" ht="14.25" customHeight="1">
       <c r="A54" s="158"/>
@@ -6087,8 +6087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:G6"/>
+    <sheetView topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="13.5" customHeight="1"/>
@@ -6124,14 +6124,14 @@
       <c r="A2" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="229" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
       <c r="J2" s="89" t="s">
         <v>14</v>
       </c>
@@ -6140,14 +6140,14 @@
       <c r="A3" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="215" t="s">
+      <c r="B3" s="229" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="215"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
+      <c r="C3" s="229"/>
+      <c r="D3" s="229"/>
+      <c r="E3" s="229"/>
+      <c r="F3" s="229"/>
+      <c r="G3" s="229"/>
       <c r="J3" s="89" t="s">
         <v>16</v>
       </c>
@@ -6156,14 +6156,14 @@
       <c r="A4" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="216" t="s">
+      <c r="B4" s="230" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="216"/>
-      <c r="D4" s="216"/>
-      <c r="E4" s="216"/>
-      <c r="F4" s="216"/>
-      <c r="G4" s="216"/>
+      <c r="C4" s="230"/>
+      <c r="D4" s="230"/>
+      <c r="E4" s="230"/>
+      <c r="F4" s="230"/>
+      <c r="G4" s="230"/>
       <c r="J4" s="90"/>
     </row>
     <row r="5" spans="1:10" s="124" customFormat="1" ht="14.25">
@@ -6179,11 +6179,11 @@
       <c r="D5" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="219" t="s">
+      <c r="E5" s="233" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="219"/>
-      <c r="G5" s="219"/>
+      <c r="F5" s="233"/>
+      <c r="G5" s="233"/>
       <c r="J5" s="89" t="s">
         <v>21</v>
       </c>
@@ -6199,18 +6199,18 @@
       </c>
       <c r="C6" s="95">
         <f>E6-D6-B6-A6</f>
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D6" s="96">
         <f>COUNTIF(F11:G694,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="218">
+      <c r="E6" s="232">
         <f>COUNTA(A11:A252)*2</f>
-        <v>52</v>
-      </c>
-      <c r="F6" s="218"/>
-      <c r="G6" s="218"/>
+        <v>44</v>
+      </c>
+      <c r="F6" s="232"/>
+      <c r="G6" s="232"/>
       <c r="J6" s="89" t="s">
         <v>19</v>
       </c>
@@ -6266,9 +6266,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A11" s="150" t="s">
-        <v>111</v>
-      </c>
+      <c r="A11" s="150"/>
       <c r="B11" s="53" t="s">
         <v>133</v>
       </c>
@@ -6304,9 +6302,7 @@
       <c r="I12" s="149"/>
     </row>
     <row r="13" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A13" s="150" t="s">
-        <v>111</v>
-      </c>
+      <c r="A13" s="150"/>
       <c r="B13" s="53" t="s">
         <v>208</v>
       </c>
@@ -6341,9 +6337,7 @@
       <c r="I14" s="149"/>
     </row>
     <row r="15" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A15" s="150" t="s">
-        <v>111</v>
-      </c>
+      <c r="A15" s="150"/>
       <c r="B15" s="53" t="s">
         <v>253</v>
       </c>
@@ -6378,9 +6372,7 @@
       <c r="I16" s="149"/>
     </row>
     <row r="17" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A17" s="150" t="s">
-        <v>111</v>
-      </c>
+      <c r="A17" s="150"/>
       <c r="B17" s="53" t="s">
         <v>259</v>
       </c>
@@ -6415,7 +6407,7 @@
       <c r="I18" s="111"/>
     </row>
     <row r="19" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A19" s="222"/>
+      <c r="A19" s="204"/>
       <c r="B19" s="150" t="s">
         <v>264</v>
       </c>
@@ -6425,11 +6417,11 @@
       <c r="F19" s="150"/>
       <c r="G19" s="150"/>
       <c r="H19" s="150"/>
-      <c r="I19" s="220"/>
+      <c r="I19" s="202"/>
     </row>
     <row r="20" spans="1:9" ht="13.5" customHeight="1">
       <c r="A20" s="111" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B20&lt;&gt;"",D20&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
         <v>[Mod_login-10]</v>
       </c>
       <c r="B20" s="111" t="s">
@@ -6485,13 +6477,13 @@
       <c r="D22" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="E22" s="226" t="s">
+      <c r="E22" s="205" t="s">
         <v>277</v>
       </c>
-      <c r="F22" s="226"/>
-      <c r="G22" s="226"/>
-      <c r="H22" s="226"/>
-      <c r="I22" s="226"/>
+      <c r="F22" s="205"/>
+      <c r="G22" s="205"/>
+      <c r="H22" s="205"/>
+      <c r="I22" s="205"/>
     </row>
     <row r="23" spans="1:9" ht="13.5" customHeight="1">
       <c r="A23" s="111" t="str">
@@ -6507,7 +6499,7 @@
       <c r="D23" s="111" t="s">
         <v>273</v>
       </c>
-      <c r="E23" s="226" t="s">
+      <c r="E23" s="205" t="s">
         <v>278</v>
       </c>
       <c r="F23" s="111"/>
@@ -6529,7 +6521,7 @@
       <c r="D24" s="111" t="s">
         <v>276</v>
       </c>
-      <c r="E24" s="226" t="s">
+      <c r="E24" s="205" t="s">
         <v>279</v>
       </c>
       <c r="F24" s="111"/>
@@ -6551,13 +6543,13 @@
       <c r="D25" s="111" t="s">
         <v>276</v>
       </c>
-      <c r="E25" s="226" t="s">
+      <c r="E25" s="205" t="s">
         <v>280</v>
       </c>
-      <c r="F25" s="226"/>
-      <c r="G25" s="226"/>
-      <c r="H25" s="226"/>
-      <c r="I25" s="226"/>
+      <c r="F25" s="205"/>
+      <c r="G25" s="205"/>
+      <c r="H25" s="205"/>
+      <c r="I25" s="205"/>
     </row>
     <row r="26" spans="1:9" ht="13.5" customHeight="1">
       <c r="A26" s="111" t="str">
@@ -6573,7 +6565,7 @@
       <c r="D26" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="E26" s="226" t="s">
+      <c r="E26" s="205" t="s">
         <v>281</v>
       </c>
       <c r="F26" s="111"/>
@@ -6595,7 +6587,7 @@
       <c r="D27" s="111" t="s">
         <v>288</v>
       </c>
-      <c r="E27" s="226" t="s">
+      <c r="E27" s="205" t="s">
         <v>282</v>
       </c>
       <c r="F27" s="111"/>
@@ -6617,7 +6609,7 @@
       <c r="D28" s="111" t="s">
         <v>288</v>
       </c>
-      <c r="E28" s="226" t="s">
+      <c r="E28" s="205" t="s">
         <v>283</v>
       </c>
       <c r="F28" s="111"/>
@@ -6626,7 +6618,7 @@
       <c r="I28" s="111"/>
     </row>
     <row r="29" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A29" s="222"/>
+      <c r="A29" s="204"/>
       <c r="B29" s="150" t="s">
         <v>289</v>
       </c>
@@ -6636,7 +6628,7 @@
       <c r="F29" s="150"/>
       <c r="G29" s="150"/>
       <c r="H29" s="150"/>
-      <c r="I29" s="220"/>
+      <c r="I29" s="202"/>
     </row>
     <row r="30" spans="1:9" ht="13.5" customHeight="1">
       <c r="A30" s="111" t="str">
@@ -6652,13 +6644,13 @@
       <c r="D30" s="111" t="s">
         <v>300</v>
       </c>
-      <c r="E30" s="226" t="s">
+      <c r="E30" s="205" t="s">
         <v>313</v>
       </c>
-      <c r="F30" s="226"/>
-      <c r="G30" s="226"/>
-      <c r="H30" s="226"/>
-      <c r="I30" s="226"/>
+      <c r="F30" s="205"/>
+      <c r="G30" s="205"/>
+      <c r="H30" s="205"/>
+      <c r="I30" s="205"/>
     </row>
     <row r="31" spans="1:9" ht="13.5" customHeight="1">
       <c r="A31" s="111" t="str">
@@ -6674,13 +6666,13 @@
       <c r="D31" s="111" t="s">
         <v>302</v>
       </c>
-      <c r="E31" s="226" t="s">
+      <c r="E31" s="205" t="s">
         <v>314</v>
       </c>
-      <c r="F31" s="226"/>
-      <c r="G31" s="226"/>
-      <c r="H31" s="226"/>
-      <c r="I31" s="226"/>
+      <c r="F31" s="205"/>
+      <c r="G31" s="205"/>
+      <c r="H31" s="205"/>
+      <c r="I31" s="205"/>
     </row>
     <row r="32" spans="1:9" ht="13.5" customHeight="1">
       <c r="A32" s="111" t="str">
@@ -6696,13 +6688,13 @@
       <c r="D32" s="111" t="s">
         <v>302</v>
       </c>
-      <c r="E32" s="226" t="s">
+      <c r="E32" s="205" t="s">
         <v>315</v>
       </c>
-      <c r="F32" s="226"/>
-      <c r="G32" s="226"/>
-      <c r="H32" s="226"/>
-      <c r="I32" s="226"/>
+      <c r="F32" s="205"/>
+      <c r="G32" s="205"/>
+      <c r="H32" s="205"/>
+      <c r="I32" s="205"/>
     </row>
     <row r="33" spans="1:9" ht="13.5" customHeight="1">
       <c r="A33" s="111" t="str">
@@ -6718,13 +6710,13 @@
       <c r="D33" s="111" t="s">
         <v>305</v>
       </c>
-      <c r="E33" s="226" t="s">
+      <c r="E33" s="205" t="s">
         <v>316</v>
       </c>
-      <c r="F33" s="227"/>
-      <c r="G33" s="227"/>
-      <c r="H33" s="228"/>
-      <c r="I33" s="227"/>
+      <c r="F33" s="206"/>
+      <c r="G33" s="206"/>
+      <c r="H33" s="207"/>
+      <c r="I33" s="206"/>
     </row>
     <row r="34" spans="1:9" ht="13.5" customHeight="1">
       <c r="A34" s="111" t="str">
@@ -6740,13 +6732,13 @@
       <c r="D34" s="111" t="s">
         <v>307</v>
       </c>
-      <c r="E34" s="226" t="s">
+      <c r="E34" s="205" t="s">
         <v>317</v>
       </c>
-      <c r="F34" s="227"/>
-      <c r="G34" s="227"/>
-      <c r="H34" s="228"/>
-      <c r="I34" s="227"/>
+      <c r="F34" s="206"/>
+      <c r="G34" s="206"/>
+      <c r="H34" s="207"/>
+      <c r="I34" s="206"/>
     </row>
     <row r="35" spans="1:9" ht="13.5" customHeight="1">
       <c r="A35" s="111" t="str">
@@ -6762,13 +6754,13 @@
       <c r="D35" s="111" t="s">
         <v>307</v>
       </c>
-      <c r="E35" s="226" t="s">
+      <c r="E35" s="205" t="s">
         <v>318</v>
       </c>
-      <c r="F35" s="227"/>
-      <c r="G35" s="227"/>
-      <c r="H35" s="228"/>
-      <c r="I35" s="227"/>
+      <c r="F35" s="206"/>
+      <c r="G35" s="206"/>
+      <c r="H35" s="207"/>
+      <c r="I35" s="206"/>
     </row>
     <row r="36" spans="1:9" ht="13.5" customHeight="1">
       <c r="A36" s="111" t="str">
@@ -6784,13 +6776,13 @@
       <c r="D36" s="111" t="s">
         <v>302</v>
       </c>
-      <c r="E36" s="226" t="s">
+      <c r="E36" s="205" t="s">
         <v>319</v>
       </c>
-      <c r="F36" s="227"/>
-      <c r="G36" s="227"/>
-      <c r="H36" s="228"/>
-      <c r="I36" s="227"/>
+      <c r="F36" s="206"/>
+      <c r="G36" s="206"/>
+      <c r="H36" s="207"/>
+      <c r="I36" s="206"/>
     </row>
     <row r="37" spans="1:9" ht="13.5" customHeight="1">
       <c r="A37" s="111" t="str">
@@ -6806,13 +6798,13 @@
       <c r="D37" s="111" t="s">
         <v>311</v>
       </c>
-      <c r="E37" s="226" t="s">
+      <c r="E37" s="205" t="s">
         <v>320</v>
       </c>
-      <c r="F37" s="227"/>
-      <c r="G37" s="227"/>
-      <c r="H37" s="228"/>
-      <c r="I37" s="227"/>
+      <c r="F37" s="206"/>
+      <c r="G37" s="206"/>
+      <c r="H37" s="207"/>
+      <c r="I37" s="206"/>
     </row>
     <row r="38" spans="1:9" ht="13.5" customHeight="1">
       <c r="A38" s="111" t="str">
@@ -6828,13 +6820,13 @@
       <c r="D38" s="111" t="s">
         <v>311</v>
       </c>
-      <c r="E38" s="226" t="s">
+      <c r="E38" s="205" t="s">
         <v>321</v>
       </c>
-      <c r="F38" s="227"/>
-      <c r="G38" s="227"/>
-      <c r="H38" s="228"/>
-      <c r="I38" s="227"/>
+      <c r="F38" s="206"/>
+      <c r="G38" s="206"/>
+      <c r="H38" s="207"/>
+      <c r="I38" s="206"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6870,8 +6862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="13.5" customHeight="1"/>
@@ -6907,14 +6899,14 @@
       <c r="A2" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="229" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
       <c r="J2" s="89" t="s">
         <v>14</v>
       </c>
@@ -6923,14 +6915,14 @@
       <c r="A3" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="215" t="s">
+      <c r="B3" s="229" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="215"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
+      <c r="C3" s="229"/>
+      <c r="D3" s="229"/>
+      <c r="E3" s="229"/>
+      <c r="F3" s="229"/>
+      <c r="G3" s="229"/>
       <c r="J3" s="89" t="s">
         <v>16</v>
       </c>
@@ -6939,14 +6931,14 @@
       <c r="A4" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="216" t="s">
+      <c r="B4" s="230" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="216"/>
-      <c r="D4" s="216"/>
-      <c r="E4" s="216"/>
-      <c r="F4" s="216"/>
-      <c r="G4" s="216"/>
+      <c r="C4" s="230"/>
+      <c r="D4" s="230"/>
+      <c r="E4" s="230"/>
+      <c r="F4" s="230"/>
+      <c r="G4" s="230"/>
       <c r="J4" s="90"/>
     </row>
     <row r="5" spans="1:10" s="124" customFormat="1" ht="14.25">
@@ -6962,11 +6954,11 @@
       <c r="D5" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="219" t="s">
+      <c r="E5" s="233" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="219"/>
-      <c r="G5" s="219"/>
+      <c r="F5" s="233"/>
+      <c r="G5" s="233"/>
       <c r="J5" s="89" t="s">
         <v>21</v>
       </c>
@@ -6988,12 +6980,12 @@
         <f>COUNTIF(F11:G707,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="218">
+      <c r="E6" s="232">
         <f>COUNTA(A11:A264)*2</f>
         <v>22</v>
       </c>
-      <c r="F6" s="218"/>
-      <c r="G6" s="218"/>
+      <c r="F6" s="232"/>
+      <c r="G6" s="232"/>
       <c r="J6" s="89" t="s">
         <v>19</v>
       </c>
@@ -7208,19 +7200,19 @@
       <c r="B20" s="111" t="s">
         <v>230</v>
       </c>
-      <c r="C20" s="226" t="s">
+      <c r="C20" s="205" t="s">
         <v>231</v>
       </c>
-      <c r="D20" s="226" t="s">
+      <c r="D20" s="205" t="s">
         <v>233</v>
       </c>
-      <c r="E20" s="226" t="s">
+      <c r="E20" s="205" t="s">
         <v>330</v>
       </c>
-      <c r="F20" s="226"/>
-      <c r="G20" s="226"/>
-      <c r="H20" s="226"/>
-      <c r="I20" s="230"/>
+      <c r="F20" s="205"/>
+      <c r="G20" s="205"/>
+      <c r="H20" s="205"/>
+      <c r="I20" s="209"/>
       <c r="J20" s="99"/>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
@@ -7231,19 +7223,19 @@
       <c r="B21" s="175" t="s">
         <v>239</v>
       </c>
-      <c r="C21" s="226" t="s">
+      <c r="C21" s="205" t="s">
         <v>240</v>
       </c>
-      <c r="D21" s="226" t="s">
+      <c r="D21" s="205" t="s">
         <v>241</v>
       </c>
-      <c r="E21" s="226" t="s">
+      <c r="E21" s="205" t="s">
         <v>329</v>
       </c>
-      <c r="F21" s="226"/>
-      <c r="G21" s="226"/>
-      <c r="H21" s="226"/>
-      <c r="I21" s="230"/>
+      <c r="F21" s="205"/>
+      <c r="G21" s="205"/>
+      <c r="H21" s="205"/>
+      <c r="I21" s="209"/>
       <c r="J21" s="99"/>
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1">
@@ -7254,19 +7246,19 @@
       <c r="B22" s="175" t="s">
         <v>325</v>
       </c>
-      <c r="C22" s="226" t="s">
+      <c r="C22" s="205" t="s">
         <v>326</v>
       </c>
-      <c r="D22" s="226" t="s">
+      <c r="D22" s="205" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="226" t="s">
+      <c r="E22" s="205" t="s">
         <v>331</v>
       </c>
-      <c r="F22" s="226"/>
-      <c r="G22" s="226"/>
-      <c r="H22" s="226"/>
-      <c r="I22" s="230"/>
+      <c r="F22" s="205"/>
+      <c r="G22" s="205"/>
+      <c r="H22" s="205"/>
+      <c r="I22" s="209"/>
       <c r="J22" s="99"/>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1">
@@ -7277,33 +7269,33 @@
       <c r="B23" s="175" t="s">
         <v>327</v>
       </c>
-      <c r="C23" s="226" t="s">
+      <c r="C23" s="205" t="s">
         <v>328</v>
       </c>
-      <c r="D23" s="226" t="s">
+      <c r="D23" s="205" t="s">
         <v>241</v>
       </c>
-      <c r="E23" s="221" t="s">
+      <c r="E23" s="203" t="s">
         <v>332</v>
       </c>
-      <c r="F23" s="221"/>
-      <c r="G23" s="221"/>
-      <c r="H23" s="221"/>
-      <c r="I23" s="229"/>
+      <c r="F23" s="203"/>
+      <c r="G23" s="203"/>
+      <c r="H23" s="203"/>
+      <c r="I23" s="208"/>
       <c r="J23" s="99"/>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
       <c r="A24" s="53"/>
-      <c r="B24" s="223" t="s">
+      <c r="B24" s="234" t="s">
         <v>238</v>
       </c>
-      <c r="C24" s="224"/>
-      <c r="D24" s="224"/>
-      <c r="E24" s="224"/>
-      <c r="F24" s="224"/>
-      <c r="G24" s="224"/>
-      <c r="H24" s="224"/>
-      <c r="I24" s="225"/>
+      <c r="C24" s="235"/>
+      <c r="D24" s="235"/>
+      <c r="E24" s="235"/>
+      <c r="F24" s="235"/>
+      <c r="G24" s="235"/>
+      <c r="H24" s="235"/>
+      <c r="I24" s="236"/>
       <c r="J24" s="99"/>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1">
@@ -7323,10 +7315,10 @@
       <c r="E25" s="111" t="s">
         <v>333</v>
       </c>
-      <c r="F25" s="226"/>
-      <c r="G25" s="226"/>
-      <c r="H25" s="226"/>
-      <c r="I25" s="236"/>
+      <c r="F25" s="205"/>
+      <c r="G25" s="205"/>
+      <c r="H25" s="205"/>
+      <c r="I25" s="214"/>
       <c r="J25" s="99"/>
     </row>
     <row r="26" spans="1:10" ht="14.25" customHeight="1">
@@ -7346,10 +7338,10 @@
       <c r="E26" s="111" t="s">
         <v>334</v>
       </c>
-      <c r="F26" s="226"/>
-      <c r="G26" s="226"/>
-      <c r="H26" s="226"/>
-      <c r="I26" s="236"/>
+      <c r="F26" s="205"/>
+      <c r="G26" s="205"/>
+      <c r="H26" s="205"/>
+      <c r="I26" s="214"/>
       <c r="J26" s="99"/>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1">
@@ -7369,10 +7361,10 @@
       <c r="E27" s="111" t="s">
         <v>335</v>
       </c>
-      <c r="F27" s="226"/>
-      <c r="G27" s="226"/>
-      <c r="H27" s="226"/>
-      <c r="I27" s="236"/>
+      <c r="F27" s="205"/>
+      <c r="G27" s="205"/>
+      <c r="H27" s="205"/>
+      <c r="I27" s="214"/>
       <c r="J27" s="99"/>
     </row>
     <row r="28" spans="1:10" ht="13.5" customHeight="1">
@@ -7381,10 +7373,10 @@
       <c r="C28" s="111"/>
       <c r="D28" s="111"/>
       <c r="E28" s="111"/>
-      <c r="F28" s="226"/>
-      <c r="G28" s="226"/>
-      <c r="H28" s="226"/>
-      <c r="I28" s="236"/>
+      <c r="F28" s="205"/>
+      <c r="G28" s="205"/>
+      <c r="H28" s="205"/>
+      <c r="I28" s="214"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>